<commit_message>
Working backend so far
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J89"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>320.68298</v>
+        <v>320.6878</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>163.04446</v>
+        <v>163.0597</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -593,7 +593,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>157.74072</v>
+        <v>157.74315</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>146.06949</v>
+        <v>146.0713</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -681,7 +681,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>76.48515</v>
+        <v>76.48631</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -725,7 +725,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>65.02343999999999</v>
+        <v>65.02419999999999</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -769,7 +769,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>46.0062</v>
+        <v>46.007133</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -813,7 +813,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>25.758955</v>
+        <v>25.759068</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>24.691505</v>
+        <v>24.691805</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>21.261005</v>
+        <v>21.261477</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>19.365265</v>
+        <v>19.36528</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -989,7 +989,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>16.283064</v>
+        <v>16.283268</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1033,7 +1033,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>12.02059</v>
+        <v>12.020853</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>11.560017</v>
+        <v>11.56027</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1121,7 +1121,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>11.422302</v>
+        <v>11.422516</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1165,7 +1165,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>11.268749</v>
+        <v>11.269152</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>9.852751</v>
+        <v>9.852928</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1253,7 +1253,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>9.773137999999999</v>
+        <v>9.773457000000001</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>8.219555</v>
+        <v>8.218931</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1341,7 +1341,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>7.700857</v>
+        <v>7.700903</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1385,7 +1385,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>7.661665</v>
+        <v>7.6617393</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1429,7 +1429,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>7.1618767</v>
+        <v>7.1621685</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1473,7 +1473,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>6.8640747</v>
+        <v>6.864105</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>6.4529076</v>
+        <v>6.452999</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1561,7 +1561,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>5.8218613</v>
+        <v>5.8221245</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1605,7 +1605,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>5.5119667</v>
+        <v>5.511585</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1649,7 +1649,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>4.839899</v>
+        <v>4.806385</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1693,7 +1693,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>4.701618</v>
+        <v>4.701643</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>4.325636</v>
+        <v>4.325392</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1781,7 +1781,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>4.2810135</v>
+        <v>4.281063</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1825,7 +1825,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>4.160721</v>
+        <v>4.1608124</v>
       </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
@@ -1865,7 +1865,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>4.1212997</v>
+        <v>4.1213493</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1909,7 +1909,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>4.0957336</v>
+        <v>4.095972</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1953,7 +1953,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>3.4143295</v>
+        <v>3.4143333</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1997,7 +1997,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>3.31678</v>
+        <v>3.3168545</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -2041,7 +2041,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>3.1636581</v>
+        <v>3.1638184</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -2085,7 +2085,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>3.096241</v>
+        <v>3.0962734</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -2129,7 +2129,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>2.9316444</v>
+        <v>2.9316483</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -2217,7 +2217,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>2.6659985</v>
+        <v>2.666113</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -2261,7 +2261,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>2.6303253</v>
+        <v>2.630474</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -2305,7 +2305,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>2.620596</v>
+        <v>2.6206264</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -2349,7 +2349,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>2.60289</v>
+        <v>2.6030064</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -2393,7 +2393,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>2.5592842</v>
+        <v>2.5434074</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -2437,7 +2437,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>2.4698067</v>
+        <v>2.4696312</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -2462,218 +2462,218 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>DL-887a2385045f651122c064ee4d0928fc</t>
+          <t>DL-37c373fee1dff1bb24a16495a09080f5</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Endless coughs to buy the latest Nintendo console... and miss it</t>
+          <t>Nintendo Switch 2 vs Nintendo Switch : what are the main differences?</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://www.vozpopuli.com/altavoz/cultura/colas-interminables-para-comprar-la-ultima-consola-de-nintendo-y-se-quedan-sin-ella.html</t>
+          <t>https://www.numerama.com/tech/1988347-nintendo-switch-2-vs-nintendo-switch-quelles-sont-les-principales-differences.html</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Nintendo announced the launch of their new Nintendo Switch 2 console on May 5th. The lack of'stock' has caused the consequent anger of those who have been left without their longed-for toy. Even some, who had paid in advance months in advance, have ended up without theirs.</t>
+          <t>Switch 2 is a direct evolution of the Switch (Standard and OLED) it is also able to play its games, thanks to backwards compatibility. The launch catalogue already offers its own exclusives with the latest Mario Kart World, available only on this new model. There are also many improvements that, when completed, make this console a much more significant advance than the OLED Switch had been compared to the classic Switch.</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>2.323763</v>
+        <v>2.4266968</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-06-07T02:45:07+00:00</t>
+          <t>2025-06-10T14:12:11+00:00</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>['The Nintendo Switch is today the third best-selling video game console in history and, at the rate it is going, everything indicates that it will soon reach second place.', 'The Nintendo Switch 2 was officially released on June 5, 2025, although there were people who were able to get it on June 4 to try it out earlier. However, there is a big problem with its release: there is not enough stock for everyone.']</t>
+          <t>['The Nintendo Switch 2 relies on a catalogue of exclusive games. Mario kart World is the first of its kind and there is no chance that it will be seen on previous generations. So a big argument: that of ensuring compatibility with the next games.', 'Which Nintendo Switch to choose? After reviewing the many differences between the models, the question remains: what is the best choice for Nintendo Switch in 2025?', 'In short, the Switch 2 is now the best option at Nintendo, not only because it’s the latest console to date (the OLED Switch was not specifically recommended at the time of its release). But this new Switch 2 marks a new chapter.']</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>-0.7184</v>
+        <v>0.8268</v>
       </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>0.132</v>
       </c>
       <c r="J47" t="n">
-        <v>0.115</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>DL-ce5f9cdf63998a111dd0a2e7410853d6</t>
+          <t>DL-887a2385045f651122c064ee4d0928fc</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Meta in talks with Disney, A24 and others to secure content for VR headsets</t>
+          <t>Endless coughs to buy the latest Nintendo console... and miss it</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://gigazine.net/gsc_news/en/20250605-meta-vr-contents-from-disney-a24/</t>
+          <t>https://www.vozpopuli.com/altavoz/cultura/colas-interminables-para-comprar-la-ultima-consola-de-nintendo-y-se-quedan-sin-ella.html</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>FFmpeg has integrated WebRTC support, enabling ultra-low latency streaming of less than 1 second with OBS, the latest codecs can be selected, and even streaming without a server is now possible X files lawsuit against eight users who tried to unfairly increase their revenue by abusing 'creator revenue sharing' Meta announces details of AI smart glasses 'Aria Gen 2', explaining cutting-edge camera and sensor technology Results of 'MLPerf Training v5.0', which</t>
+          <t>Nintendo announced the launch of their new Nintendo Switch 2 console on May 5th. The lack of'stock' has caused the consequent anger of those who have been left without their longed-for toy. Even some, who had paid in advance months in advance, have ended up without theirs.</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>2.3176193</v>
+        <v>2.3237877</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-06-05T06:24:00+00:00</t>
+          <t>2025-06-07T02:45:07+00:00</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>["reaffirms plans to invest $100 billion in Arizona over next five years\nPart of 'MetaHuman', a game development tool that allows you to create and move ultra-realistic 3DCG characters for free, is integrated into Unreal Engine 5.6\nThe reason why the Nintendo", "Switch 2 was not loaned to the media for pre-release review was because 'important features and updates for the console' will be provided on the release date of June 5th.", "Speculation is rife that the Chinese-made high-performance AI model 'DeepSeek-R1-0528' may have been distilled using Google's AI 'Gemini'\nAttention is drawn to the warning in the Nintendo Switch 2 manual that reads, 'Do not remove the shatterproof film"]</t>
+          <t>['The Nintendo Switch is today the third best-selling video game console in history and, at the rate it is going, everything indicates that it will soon reach second place.', 'The Nintendo Switch 2 was officially released on June 5, 2025, although there were people who were able to get it on June 4 to try it out earlier. However, there is a big problem with its release: there is not enough stock for everyone.']</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>0.4588</v>
+        <v>-0.7184</v>
       </c>
       <c r="I48" t="n">
-        <v>0.133</v>
+        <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>0.108</v>
+        <v>0.115</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>DL-b080cb5509d88a1ec15ee8a2c6106938</t>
+          <t>DL-ce5f9cdf63998a111dd0a2e7410853d6</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Get the most out of your Nintendo Switch 2 with these 3 TVs I've picked to pair with it, including one of the best OLED TVs I've seen</t>
+          <t>Meta in talks with Disney, A24 and others to secure content for VR headsets</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://www.techradar.com/televisions/get-the-most-out-of-your-nintendo-switch-2-with-these-3-tvs-ive-picked-to-pair-with-it-including-one-of-the-best-oled-tvs-ive-seen</t>
+          <t>https://gigazine.net/gsc_news/en/20250605-meta-vr-contents-from-disney-a24/</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>TechRadar look for VRR, 120Hz refresh rate and Auto Low Latency Mode. Low input lag for responsive performance and top-notch picture quality are also important. LG B4 48-inch 4K OLED TV : £879 now £849 at Best Buy The LG C4 provides premium OLED picture quality and a full array of gaming features.</t>
+          <t>FFmpeg has integrated WebRTC support, enabling ultra-low latency streaming of less than 1 second with OBS, the latest codecs can be selected, and even streaming without a server is now possible X files lawsuit against eight users who tried to unfairly increase their revenue by abusing 'creator revenue sharing' Meta announces details of AI smart glasses 'Aria Gen 2', explaining cutting-edge camera and sensor technology Results of 'MLPerf Training v5.0', which</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>2.035572</v>
+        <v>2.3176746</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-06-06T08:00:00</t>
+          <t>2025-06-05T06:24:00+00:00</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>['The Nintendo Switch 2 has finally arrived, and it brings several upgrades over its predecessor, including 4K resolution, 120Hz (at 1080p resolution) and HDR support.', 'And there’s no better time to buy one to pair with your Nintendo Switch 2 with ambitious ports such as Cyberpunk: 2077 available from launch.', 'The Switch 2 can once again take advantage of that low input lag time for ultra-responsive performance (crucial for Mario Kart World) and the B4’s 4K, HDR and 120Hz support to level-up their experience from the original Nintendo Switch.']</t>
+          <t>["reaffirms plans to invest $100 billion in Arizona over next five years\nPart of 'MetaHuman', a game development tool that allows you to create and move ultra-realistic 3DCG characters for free, is integrated into Unreal Engine 5.6\nThe reason why the Nintendo", "Switch 2 was not loaned to the media for pre-release review was because 'important features and updates for the console' will be provided on the release date of June 5th.", "Speculation is rife that the Chinese-made high-performance AI model 'DeepSeek-R1-0528' may have been distilled using Google's AI 'Gemini'\nAttention is drawn to the warning in the Nintendo Switch 2 manual that reads, 'Do not remove the shatterproof film"]</t>
         </is>
       </c>
       <c r="H49" t="n">
-        <v>0.5719</v>
+        <v>0.4588</v>
       </c>
       <c r="I49" t="n">
-        <v>0.181</v>
+        <v>0.133</v>
       </c>
       <c r="J49" t="n">
-        <v>0.116</v>
+        <v>0.108</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>DL-bc0bf2ef431589eeb38d530dce7bdf45</t>
+          <t>DL-b080cb5509d88a1ec15ee8a2c6106938</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Bouncemasters demo now available on Steam</t>
+          <t>Get the most out of your Nintendo Switch 2 with these 3 TVs I've picked to pair with it, including one of the best OLED TVs I've seen</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://thatsgaming.nl/bouncemasters-demo-nu-beschikbaar-op-steam/</t>
+          <t>https://www.techradar.com/televisions/get-the-most-out-of-your-nintendo-switch-2-with-these-3-tvs-ive-picked-to-pair-with-it-including-one-of-the-best-oled-tvs-ive-seen</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Bouncemasters is a fun physics-based arcade game inspired by Yetisports. The full version comes out on Steam in the third quarter of 2025. TAMAGOTCHI PLAZA is coming to the Nintendo Switch 2 and Nintendo Switch 2. Both versions will be compatible with the Tamagotchi Uni device.</t>
+          <t>TechRadar look for VRR, 120Hz refresh rate and Auto Low Latency Mode. Low input lag for responsive performance and top-notch picture quality are also important. LG B4 48-inch 4K OLED TV : £879 now £849 at Best Buy The LG C4 provides premium OLED picture quality and a full array of gaming features.</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>1.8310566</v>
+        <v>2.0356522</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-06-06T18:57:55+00:00</t>
+          <t>2025-06-06T08:00:00</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>['Nintendo Switch 2 players who already own the original Switch version of TAMGOTCHI PLAZA can access the exclusive content by creating the Tamagotchi Plaza Nintendo Switch 2 upgrade package.', 'TAMAGOTCHI PLAZA brings back the unique and engaging experience of the series: setting up idiosyncratic shops and serving cute characters.']</t>
+          <t>['The Nintendo Switch 2 has finally arrived, and it brings several upgrades over its predecessor, including 4K resolution, 120Hz (at 1080p resolution) and HDR support.', 'And there’s no better time to buy one to pair with your Nintendo Switch 2 with ambitious ports such as Cyberpunk: 2077 available from launch.', 'The Switch 2 can once again take advantage of that low input lag time for ultra-responsive performance (crucial for Mario Kart World) and the B4’s 4K, HDR and 120Hz support to level-up their experience from the original Nintendo Switch.']</t>
         </is>
       </c>
       <c r="H50" t="n">
-        <v>0.7579</v>
+        <v>0.5719</v>
       </c>
       <c r="I50" t="n">
-        <v>0.137</v>
+        <v>0.181</v>
       </c>
       <c r="J50" t="n">
-        <v>0</v>
+        <v>0.116</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>DL-17c1cd3dca5a8d385d5f912ade6383f3</t>
+          <t>DL-bc0bf2ef431589eeb38d530dce7bdf45</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 launches today. Here’s what to know</t>
+          <t>Bouncemasters demo now available on Steam</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://www.wsaw.com/2025/06/05/nintendo-switch-2-launches-today-heres-what-know/</t>
+          <t>https://thatsgaming.nl/bouncemasters-demo-nu-beschikbaar-op-steam/</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Nintendo’s new console, the Switch 2, arrives on store shelves globally after being announced in April. Nearly all US Best Buy stores opened just after midnight to accommodate eager fans. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table.</t>
+          <t>Bouncemasters is a fun physics-based arcade game inspired by Yetisports. The full version comes out on Steam in the third quarter of 2025. TAMAGOTCHI PLAZA is coming to the Nintendo Switch 2 and Nintendo Switch 2. Both versions will be compatible with the Tamagotchi Uni device.</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>1.7731018</v>
+        <v>1.8311577</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-06-05T13:46:00+00:00</t>
+          <t>2025-06-06T18:57:55+00:00</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>['In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.', 'Nintendo Switch 2 gaming devices are stored on the day Nintendo starts selling the new consoles globally, at an electronics store in Tokyo, Japan, on June 5.\nNintendo has also given the console hardware a much-needed upgrade.']</t>
+          <t>['Nintendo Switch 2 players who already own the original Switch version of TAMGOTCHI PLAZA can access the exclusive content by creating the Tamagotchi Plaza Nintendo Switch 2 upgrade package.', 'TAMAGOTCHI PLAZA brings back the unique and engaging experience of the series: setting up idiosyncratic shops and serving cute characters.']</t>
         </is>
       </c>
       <c r="H51" t="n">
-        <v>0.8442</v>
+        <v>0.7579</v>
       </c>
       <c r="I51" t="n">
-        <v>0.171</v>
+        <v>0.137</v>
       </c>
       <c r="J51" t="n">
         <v>0</v>
@@ -2682,126 +2682,126 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>DL-6b1dfb573ca972c47a35c3452e0b887c</t>
+          <t>DL-17c1cd3dca5a8d385d5f912ade6383f3</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>With the release of the Nintendo Switch 2, what's the future for the Switch?</t>
+          <t>The Nintendo Switch 2 launches today. Here’s what to know</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://www.gamekult.com/actualite/avec-la-sortie-de-la-nintendo-switch-2-quel-avenir-pour-la-switch-3050864092.html</t>
+          <t>https://www.wsaw.com/2025/06/05/nintendo-switch-2-launches-today-heres-what-know/</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Nintendo has always shown a rigorous follow-up on its previous consoles. Examples include the 3DS, which was eligible for new features until 2019 (two years after Switch’s release), and an online store until 2023. The real question would be whether Nintendo would be willing to offer its productions on both machines at the same time.</t>
+          <t>Nintendo’s new console, the Switch 2, arrives on store shelves globally after being announced in April. Nearly all US Best Buy stores opened just after midnight to accommodate eager fans. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table.</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>1.5549698</v>
-      </c>
-      <c r="F52" t="inlineStr"/>
+        <v>1.7731247</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2025-06-05T13:46:00+00:00</t>
+        </is>
+      </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>['Samus will be on both Switches A situation that is explained by Nintendo’s legacy, but also by the fact that the adoption rate of the console is probably still questionable at the moment.', 'If Nintendo has not spoken out on this issue, Kyoto is well aware that the switch 2 adoption curve is more uncertain than the first one, in the sense that consumers will be much more reluctant to switch, mainly for price reasons of course.']</t>
+          <t>['In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.', 'Nintendo Switch 2 gaming devices are stored on the day Nintendo starts selling the new consoles globally, at an electronics store in Tokyo, Japan, on June 5.\nNintendo has also given the console hardware a much-needed upgrade.']</t>
         </is>
       </c>
       <c r="H52" t="n">
-        <v>-0.2732</v>
+        <v>0.8442</v>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>0.171</v>
       </c>
       <c r="J52" t="n">
-        <v>0.039</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>DL-05605b9ac8551ba2df3061a3bb23d284</t>
+          <t>DL-6b1dfb573ca972c47a35c3452e0b887c</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>My Switch 2 Review in Progress: It's Good, but Don't Give In to the FOMO Yet</t>
+          <t>With the release of the Nintendo Switch 2, what's the future for the Switch?</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://www.cnet.com/tech/gaming/my-switch-2-review-in-progress-its-good-but-dont-give-in-to-the-fomo-yet/</t>
+          <t>https://www.gamekult.com/actualite/avec-la-sortie-de-la-nintendo-switch-2-quel-avenir-pour-la-switch-3050864092.html</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 is all anyone in gaming is talking about right now, and it could very well be the biggest gadget of 2025. By now, thousands of Switch 2 owners have one in hand as well, and the company will certainly sell thousands more this year. This clearly feels like a really good upgrade to aging Switches, but it's also not anything any current Switch owner needs to rush into.</t>
+          <t>Nintendo has always shown a rigorous follow-up on its previous consoles. Examples include the 3DS, which was eligible for new features until 2019 (two years after Switch’s release), and an online store until 2023. The real question would be whether Nintendo would be willing to offer its productions on both machines at the same time.</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>1.5476303</v>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>2025-06-06T22:34:00+00:00</t>
-        </is>
-      </c>
+        <v>1.5550461</v>
+      </c>
+      <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
-          <t>["By now, thousands of Switch 2 owners have one in hand as well, and the company will certainly sell thousands more this year, especially during the holidays. So, how good is Nintendo's new console? And is it worth upgrading from the original Switch?", "I haven't had enough time to fully review the Switch 2 yet, and the Switch 2 hasn't had enough time to spread its wings and grow its game library. These are early days for Nintendo's new console, but there's some stuff I can already tell you.", "It's a simple thing, but it really makes swapping them into accessories and back into the Switch feel effortless, the way Nintendo always advertised the experience as feeling."]</t>
+          <t>['Samus will be on both Switches A situation that is explained by Nintendo’s legacy, but also by the fact that the adoption rate of the console is probably still questionable at the moment.', 'If Nintendo has not spoken out on this issue, Kyoto is well aware that the switch 2 adoption curve is more uncertain than the first one, in the sense that consumers will be much more reluctant to switch, mainly for price reasons of course.']</t>
         </is>
       </c>
       <c r="H53" t="n">
-        <v>0.8443000000000001</v>
+        <v>-0.2732</v>
       </c>
       <c r="I53" t="n">
-        <v>0.177</v>
+        <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>0</v>
+        <v>0.039</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>DL-f18eecd6ae1aa3953cec4cf5dcc3e634</t>
+          <t>DL-05605b9ac8551ba2df3061a3bb23d284</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>'I own a Switch 2 - this console case beats Nintendo's thanks to one main feature'</t>
+          <t>My Switch 2 Review in Progress: It's Good, but Don't Give In to the FOMO Yet</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://www.birminghammail.co.uk/whats-on/shopping/i-switch-2-console-case-31823315</t>
+          <t>https://www.cnet.com/tech/gaming/my-switch-2-review-in-progress-its-good-but-dont-give-in-to-the-fomo-yet/</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 is out and I was lucky enough to get my hands on the Switch 2 on release day. There are plenty of choices out there, including the official Nintendo Switch 2, which can be bought almost everywhere. Amazon lawnmower reduced from over £100 is 'lightweight' and 'easy to handle'</t>
+          <t>The Nintendo Switch 2 is all anyone in gaming is talking about right now, and it could very well be the biggest gadget of 2025. By now, thousands of Switch 2 owners have one in hand as well, and the company will certainly sell thousands more this year. This clearly feels like a really good upgrade to aging Switches, but it's also not anything any current Switch owner needs to rush into.</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>1.5303574</v>
+        <v>1.5476952</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-06-10T10:29:21+00:00</t>
+          <t>2025-06-06T22:34:00+00:00</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>["The Nintendo Switch 2 is out and in the search for a new case - I might have found my top choice thanks to one main feature\nI was lucky enough to get my hands on the Nintendo Switch 2 on release day, and it's definitely one of my favourite purchases so", "Without going into a massive review of the console, it is the definitive Switch experience, and it's exciting to see what the future holds for it."]</t>
+          <t>["By now, thousands of Switch 2 owners have one in hand as well, and the company will certainly sell thousands more this year, especially during the holidays. So, how good is Nintendo's new console? And is it worth upgrading from the original Switch?", "I haven't had enough time to fully review the Switch 2 yet, and the Switch 2 hasn't had enough time to spread its wings and grow its game library. These are early days for Nintendo's new console, but there's some stuff I can already tell you.", "It's a simple thing, but it really makes swapping them into accessories and back into the Switch feel effortless, the way Nintendo always advertised the experience as feeling."]</t>
         </is>
       </c>
       <c r="H54" t="n">
-        <v>0.7287</v>
+        <v>0.8443000000000001</v>
       </c>
       <c r="I54" t="n">
-        <v>0.137</v>
+        <v>0.177</v>
       </c>
       <c r="J54" t="n">
         <v>0</v>
@@ -2810,42 +2810,42 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>DL-518e1f4a2492da2505d9f7e5db4b46e6</t>
+          <t>DL-f18eecd6ae1aa3953cec4cf5dcc3e634</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Microsoft Launches First Portable Game Console</t>
+          <t>'I own a Switch 2 - this console case beats Nintendo's thanks to one main feature'</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://jurnalul.ro/it/tehnica/microsoft-lansare-prima-consola-jocuri-portabila-1000410.html</t>
+          <t>https://www.birminghammail.co.uk/whats-on/shopping/i-switch-2-console-case-31823315</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>"Xbox Ally brings together the power offered by Xbox and the freedom offered by Windows," Bond says. The console price and exact launch dates will be announced in the coming months. Microsoft says both models evoke the brand's traditional controllers.</t>
+          <t>The Nintendo Switch 2 is out and I was lucky enough to get my hands on the Switch 2 on release day. There are plenty of choices out there, including the official Nintendo Switch 2, which can be bought almost everywhere. Amazon lawnmower reduced from over £100 is 'lightweight' and 'easy to handle'</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>1.5025616</v>
+        <v>1.5207672</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-06-09T00:00:00</t>
+          <t>2025-06-10T10:29:21+00:00</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>['"Xbox Ally and Xbox Ally X are perfect for players who are looking for an accessible gaming experience while travelling, whether by plane or between the two comfortable indoor seats," Microsoft said in a statement, according to the AFP.', "The announcement came just days after Japan's Nintendo launched the Switch 2 portable console."]</t>
+          <t>["The Nintendo Switch 2 is out and in the search for a new case - I might have found my top choice thanks to one main feature\nI was lucky enough to get my hands on the Nintendo Switch 2 on release day, and it's definitely one of my favourite purchases so", "Without going into a massive review of the console, it is the definitive Switch experience, and it's exciting to see what the future holds for it."]</t>
         </is>
       </c>
       <c r="H55" t="n">
-        <v>0.6369</v>
+        <v>0.7287</v>
       </c>
       <c r="I55" t="n">
-        <v>0.097</v>
+        <v>0.137</v>
       </c>
       <c r="J55" t="n">
         <v>0</v>
@@ -2854,42 +2854,42 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>DL-62f6feb86add6bac2ca72da8a1135b3b</t>
+          <t>DL-518e1f4a2492da2505d9f7e5db4b46e6</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Belkin unveils new gaming portfolio featuring power-packed charging accessories, gaming essentials</t>
+          <t>Microsoft Launches First Portable Game Console</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://www.tahawultech.com/business/belkin-unveils-new-gaming-portfolio-featuring-power-packed-charging-accessories-gaming-essentials/</t>
+          <t>https://jurnalul.ro/it/tehnica/microsoft-lansare-prima-consola-jocuri-portabila-1000410.html</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Belkin is “Leveling up your play” – bringing a new level of reliability to the gaming ecosystem that differentiates through premium materials, timeless design, and in-house engineering. The new range includes elevated accessories designed to enhance the gaming experience, featuring on-the-go charging solutions, audio gear, robust screen protection, and new travel cases built for effortless portability and protection.</t>
+          <t>"Xbox Ally brings together the power offered by Xbox and the freedom offered by Windows," Bond says. The console price and exact launch dates will be announced in the coming months. Microsoft says both models evoke the brand's traditional controllers.</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>1.5013828</v>
+        <v>1.5027504</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-06-06T17:45:51+00:00</t>
+          <t>2025-06-09T00:00:00</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>['Belkin’s first iteration of gaming accessories will feature products designed to be compatible with Nintendo Switch 2\nLOS ANGELES, CA – Belkin, a leading consumer electronics brand for over 40 years, today announced its entry into the gaming accessories', 'space with the launch of a new lineup designed to be compatible with the highly anticipated Nintendo Switch 2.', 'Built on decades of experience in power, connectivity and device protection, and released under Belkin’s innovation-focused Future Ventures category, this marks the company’s first collection of products tailored specifically for the gaming community.']</t>
+          <t>['"Xbox Ally and Xbox Ally X are perfect for players who are looking for an accessible gaming experience while travelling, whether by plane or between the two comfortable indoor seats," Microsoft said in a statement, according to the AFP.', "The announcement came just days after Japan's Nintendo launched the Switch 2 portable console."]</t>
         </is>
       </c>
       <c r="H56" t="n">
-        <v>0.6705</v>
+        <v>0.6369</v>
       </c>
       <c r="I56" t="n">
-        <v>0.104</v>
+        <v>0.097</v>
       </c>
       <c r="J56" t="n">
         <v>0</v>
@@ -2898,346 +2898,346 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>DL-5dcc26e57d179cf942f68c4c1a43add8</t>
+          <t>DL-62f6feb86add6bac2ca72da8a1135b3b</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: Everything to know about the price and features</t>
+          <t>Belkin unveils new gaming portfolio featuring power-packed charging accessories, gaming essentials</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://abc11.com/post/nintendo-switch-2-heres-everything-need-know-price-features/16656981/</t>
+          <t>https://www.tahawultech.com/business/belkin-unveils-new-gaming-portfolio-featuring-power-packed-charging-accessories-gaming-essentials/</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>The long-awaited release of the Nintendo Switch 2 is set to arrive early Thursday morning. Here's what to know about the hype behind the Switch 2, the key features of the gaming system and how to buy it. Online pre-orders are largely sold out but gamers can purchase a limited in-store supply starting at 12:01 a.m. ET on Thursday. The Nintendo Switch has sold more than 152 million consoles.</t>
+          <t>Belkin is “Leveling up your play” – bringing a new level of reliability to the gaming ecosystem that differentiates through premium materials, timeless design, and in-house engineering. The new range includes elevated accessories designed to enhance the gaming experience, featuring on-the-go charging solutions, audio gear, robust screen protection, and new travel cases built for effortless portability and protection.</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>1.4305363</v>
+        <v>1.501461</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-06-05T16:14:46</t>
+          <t>2025-06-06T17:45:51+00:00</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>['The price of the Nintendo Switch 2 in the U.S. is $449.99, while a bundle that includes "Mario Kart World" runs $499.99.\nThat price remains unchanged by Trumps tariffs, the Japan-based gaming giant said in April.', '"Nintendo Switch 2 accessories will experience price adjustments from those announced on April 2 due to changes in market conditions," the company said.', '"Other adjustments to the price of any Nintendo product are also possible in the future depending on market conditions."']</t>
+          <t>['Belkin’s first iteration of gaming accessories will feature products designed to be compatible with Nintendo Switch 2\nLOS ANGELES, CA – Belkin, a leading consumer electronics brand for over 40 years, today announced its entry into the gaming accessories', 'space with the launch of a new lineup designed to be compatible with the highly anticipated Nintendo Switch 2.', 'Built on decades of experience in power, connectivity and device protection, and released under Belkin’s innovation-focused Future Ventures category, this marks the company’s first collection of products tailored specifically for the gaming community.']</t>
         </is>
       </c>
       <c r="H57" t="n">
-        <v>-0.34</v>
+        <v>0.6705</v>
       </c>
       <c r="I57" t="n">
-        <v>0</v>
+        <v>0.104</v>
       </c>
       <c r="J57" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>DL-a77fb4dd359d5198b3f658382e12f176</t>
+          <t>DL-5dcc26e57d179cf942f68c4c1a43add8</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>These Nintendo Switch 2 Edition upgrades can keep you from breaking the bank</t>
+          <t>Nintendo Switch 2: Everything to know about the price and features</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>https://www.pockettactics.com/nintendo-switch/switch-2-edition-upgrades</t>
+          <t>https://abc11.com/post/nintendo-switch-2-heres-everything-need-know-price-features/16656981/</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>I picked up the Nintendo Switch 2 yesterday, losing many hours already to the likes of Mario Kart World and Cyberpunk 2077. On top of the price of the console itself, it'll cost you $1.2k to buy all of the Switch 2 launch games. If you do have those two excellent RPGs, you can actually upgrade them to their Switch 2 versions for free. I'm thrilled to see Pokémon Scarlet and Violet get one.</t>
+          <t>The long-awaited release of the Nintendo Switch 2 is set to arrive early Thursday morning. Here's what to know about the hype behind the Switch 2, the key features of the gaming system and how to buy it. Online pre-orders are largely sold out but gamers can purchase a limited in-store supply starting at 12:01 a.m. ET on Thursday. The Nintendo Switch has sold more than 152 million consoles.</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>1.3596001</v>
+        <v>1.4305553</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-06-06T17:42:06</t>
+          <t>2025-06-05T16:14:46</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>['Looking to the future, it appears as though Nintendo is partial to Switch 2 upgrades, just like Xbox and PlayStation with their respective games and consoles, as one of the best Mario Party games, Super Mario Party Jamboree – Nintendo Switch 2 Edition', 'With an upgrade price of $19.99, you can enjoy Kirby and the Forgotten Land Switch 2 Edition. Better still, this comes with the Star-Crossed World DLC, giving you something completely new to experience as you revisit this fun Kirby adventure.', "While I already have a Nintendo Switch 2, I do like knowing that people who don't intend to pick it up just yet – perhaps even for a couple of years – have a reasonable option to upgrade some new Switch games they do buy between now and then, with other"]</t>
+          <t>['The price of the Nintendo Switch 2 in the U.S. is $449.99, while a bundle that includes "Mario Kart World" runs $499.99.\nThat price remains unchanged by Trumps tariffs, the Japan-based gaming giant said in April.', '"Nintendo Switch 2 accessories will experience price adjustments from those announced on April 2 due to changes in market conditions," the company said.', '"Other adjustments to the price of any Nintendo product are also possible in the future depending on market conditions."']</t>
         </is>
       </c>
       <c r="H58" t="n">
-        <v>0.8979</v>
+        <v>-0.34</v>
       </c>
       <c r="I58" t="n">
-        <v>0.181</v>
+        <v>0</v>
       </c>
       <c r="J58" t="n">
-        <v>0.032</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>DL-2ce32c01c084cc6ab184d989c771b28e</t>
+          <t>DL-a77fb4dd359d5198b3f658382e12f176</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 already has a flaw: its autonomy</t>
+          <t>These Nintendo Switch 2 Edition upgrades can keep you from breaking the bank</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://www.numerama.com/tech/1985971-la-nintendo-switch-2-a-deja-un-defaut-son-autonomie.html</t>
+          <t>https://www.pockettactics.com/nintendo-switch/switch-2-edition-upgrades</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>The console is at the level of the very first version of the Switch, dated 2017. Our first tests, with a console set to 50% brightness and 50% audio volume, are not likely to reassure those who feared the worst about Switch 2’s autonomy. Cyberpunk 2077 was first launched for half an hour: the console has been upgraded from 50% battery to 22% battery.</t>
+          <t>I picked up the Nintendo Switch 2 yesterday, losing many hours already to the likes of Mario Kart World and Cyberpunk 2077. On top of the price of the console itself, it'll cost you $1.2k to buy all of the Switch 2 launch games. If you do have those two excellent RPGs, you can actually upgrade them to their Switch 2 versions for free. I'm thrilled to see Pokémon Scarlet and Violet get one.</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>1.3131561</v>
+        <v>1.3596745</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-06-06T08:28:24</t>
+          <t>2025-06-06T17:42:06</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>['I accept everything Managing my choices No miracle for Nintendo Switch 2 autonomy Your data deserves better protection. Scams, viruses and ransomware are no longer fatal.', 'If we extrapolate our little experiment (which requires repeating several times to refine), we would barely exceed the two hours of play on Cyberpunk 2077, while we could hope to reach the 3h30 on The Legend of Zelda: Breath of the Wild.', 'The Legend of Zelda: Breath of the Wild consumes a lot on Nintendo Switch 2 // Source: Nino Barbey for Numerama The choice to return to an LCD panel is really not the idea of the century, especially since its refresh rate of 120 Hz must consume more (']</t>
+          <t>['Looking to the future, it appears as though Nintendo is partial to Switch 2 upgrades, just like Xbox and PlayStation with their respective games and consoles, as one of the best Mario Party games, Super Mario Party Jamboree – Nintendo Switch 2 Edition', 'With an upgrade price of $19.99, you can enjoy Kirby and the Forgotten Land Switch 2 Edition. Better still, this comes with the Star-Crossed World DLC, giving you something completely new to experience as you revisit this fun Kirby adventure.', "While I already have a Nintendo Switch 2, I do like knowing that people who don't intend to pick it up just yet – perhaps even for a couple of years – have a reasonable option to upgrade some new Switch games they do buy between now and then, with other"]</t>
         </is>
       </c>
       <c r="H59" t="n">
-        <v>-0.738</v>
+        <v>0.8979</v>
       </c>
       <c r="I59" t="n">
-        <v>0.064</v>
+        <v>0.181</v>
       </c>
       <c r="J59" t="n">
-        <v>0.145</v>
+        <v>0.032</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>DL-f93e2da6e1d3e279a286496afdb81d0a</t>
+          <t>DL-2ce32c01c084cc6ab184d989c771b28e</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>I Can't Believe How Much Easier Voice Chat Is on the Switch 2</t>
+          <t>The Nintendo Switch 2 already has a flaw: its autonomy</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://au.pcmag.com/gaming-systems/111364/i-cant-believe-how-much-easier-voice-chat-is-on-the-switch-2</t>
+          <t>https://www.numerama.com/tech/1985971-la-nintendo-switch-2-a-deja-un-defaut-son-autonomie.html</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>The Switch 2 promises one of the company’s most ambitious online features yet with GameChat. I tested it before launch to see how Nintendo uses cameras and microphones to turn online gaming into a more fun, welcoming experience. Nintendo Switch 2 should support most USB-C webcams, even those with lower resolutions.</t>
+          <t>The console is at the level of the very first version of the Switch, dated 2017. Our first tests, with a console set to 50% brightness and 50% audio volume, are not likely to reassure those who feared the worst about Switch 2’s autonomy. Cyberpunk 2077 was first launched for half an hour: the console has been upgraded from 50% battery to 22% battery.</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>1.2322922</v>
+        <v>1.3132324</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-06-03T14:12:48+00:00</t>
+          <t>2025-06-06T08:28:24</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>["The Switch 2 promises one of the company’s most ambitious online features yet with GameChat, which is the system's new online communication system.", 'I tested it before launch to see how Nintendo uses cameras and microphones to turn online gaming into a more fun, welcoming experience.', "GameChat is so baked into the Switch 2 experience that there's a dedicated button for it on the Joy-Con controllers. Pressing the new C button launches the GameChat menu that lets you create a lobby or see which friends are online and ready to play."]</t>
+          <t>['I accept everything Managing my choices No miracle for Nintendo Switch 2 autonomy Your data deserves better protection. Scams, viruses and ransomware are no longer fatal.', 'If we extrapolate our little experiment (which requires repeating several times to refine), we would barely exceed the two hours of play on Cyberpunk 2077, while we could hope to reach the 3h30 on The Legend of Zelda: Breath of the Wild.', 'The Legend of Zelda: Breath of the Wild consumes a lot on Nintendo Switch 2 // Source: Nino Barbey for Numerama The choice to return to an LCD panel is really not the idea of the century, especially since its refresh rate of 120 Hz must consume more (']</t>
         </is>
       </c>
       <c r="H60" t="n">
-        <v>0.9226</v>
+        <v>-0.738</v>
       </c>
       <c r="I60" t="n">
-        <v>0.264</v>
+        <v>0.064</v>
       </c>
       <c r="J60" t="n">
-        <v>0.038</v>
+        <v>0.145</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>DL-b108c340c0dc3990b6d0f186f3c32267</t>
+          <t>DL-f93e2da6e1d3e279a286496afdb81d0a</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Nintendo Switch2 India Launch On THIS Date --Check Features And Expected Price</t>
+          <t>I Can't Believe How Much Easier Voice Chat Is on the Switch 2</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://zeenews.india.com/technology/nintendo-switch2-india-launch-on-this-date-check-features-and-expected-price-2911893.html</t>
+          <t>https://au.pcmag.com/gaming-systems/111364/i-cant-believe-how-much-easier-voice-chat-is-on-the-switch-2</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Nintendo Switch2 has gone out of stock globally within a day of its roll out. Priced at $499, Switch 2 comes with some major features upgrade over previous gen Switch. Switch2 is Powered by Nvidia Terga T239 chip with an octa-core ARM CORTEX- A78C CPU AND 12SM Ampere GPU. It comes with 12GB LPDDR5X RAM AND Faster loading speed.</t>
+          <t>The Switch 2 promises one of the company’s most ambitious online features yet with GameChat. I tested it before launch to see how Nintendo uses cameras and microphones to turn online gaming into a more fun, welcoming experience. Nintendo Switch 2 should support most USB-C webcams, even those with lower resolutions.</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>1.2009258</v>
+        <v>1.2323608</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-06-06T00:00:00</t>
+          <t>2025-06-03T14:12:48+00:00</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>['Priced at $499, Switch 2 comes with some major features upgrade over previous gen Switch.\nMajor Specification of Switch2\nDisplay: Nintendo Switch2 comes with larger 7.9-inch 1080p LCD touchscreen with HDR10 support and a refresh rate of 120Hz.']</t>
+          <t>["The Switch 2 promises one of the company’s most ambitious online features yet with GameChat, which is the system's new online communication system.", 'I tested it before launch to see how Nintendo uses cameras and microphones to turn online gaming into a more fun, welcoming experience.', "GameChat is so baked into the Switch 2 experience that there's a dedicated button for it on the Joy-Con controllers. Pressing the new C button launches the GameChat menu that lets you create a lobby or see which friends are online and ready to play."]</t>
         </is>
       </c>
       <c r="H61" t="n">
-        <v>0</v>
+        <v>0.9226</v>
       </c>
       <c r="I61" t="n">
-        <v>0</v>
+        <v>0.264</v>
       </c>
       <c r="J61" t="n">
-        <v>0</v>
+        <v>0.038</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>DL-201b8ebcf779d686eb6aa318af25eaa9</t>
+          <t>DL-b108c340c0dc3990b6d0f186f3c32267</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Launched sales of Nintendo Switch 2 - in which countries the console is available</t>
+          <t>Nintendo Switch2 India Launch On THIS Date --Check Features And Expected Price</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://games.24tv.ua/ru/startovali-prodazhi-nintendo-switch-2-v-kakih-stranah-dostupna-konsol-games_n2839620/amp</t>
+          <t>https://zeenews.india.com/technology/nintendo-switch2-india-launch-on-this-date-check-features-and-expected-price-2911893.html</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Nintendo decided to seriously oppose speculators who traditionally buy consoles for resale at an inflated price. Fans began to take seats in queues a few hours before the opening of the stores. Some even took a break from work to buy a novelty.</t>
+          <t>Nintendo Switch2 has gone out of stock globally within a day of its roll out. Priced at $499, Switch 2 comes with some major features upgrade over previous gen Switch. Switch2 is Powered by Nvidia Terga T239 chip with an octa-core ARM CORTEX- A78C CPU AND 12SM Ampere GPU. It comes with 12GB LPDDR5X RAM AND Faster loading speed.</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>1.0896873</v>
-      </c>
-      <c r="F62" t="inlineStr"/>
+        <v>1.2009792</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>2025-06-06T00:00:00</t>
+        </is>
+      </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>['It should be noted that neither in Ukraine nor in Russia Nintendo products are officially sold. On the eve of Nvidia CEO Jensen Huang said that Switch 2 will receive special AI processors that improve the gaming experience in real time.']</t>
+          <t>['Priced at $499, Switch 2 comes with some major features upgrade over previous gen Switch.\nMajor Specification of Switch2\nDisplay: Nintendo Switch2 comes with larger 7.9-inch 1080p LCD touchscreen with HDR10 support and a refresh rate of 120Hz.']</t>
         </is>
       </c>
       <c r="H62" t="n">
-        <v>-0.1779</v>
+        <v>0</v>
       </c>
       <c r="I62" t="n">
         <v>0</v>
       </c>
       <c r="J62" t="n">
-        <v>0.042</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>DL-9403699c5a8c3acb6752501c45ccc38e</t>
+          <t>DL-201b8ebcf779d686eb6aa318af25eaa9</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 – Release brings 20 games directly</t>
+          <t>Launched sales of Nintendo Switch 2 - in which countries the console is available</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>https://www.toptechnews.de/2025/06/05/nintendo-switch-2-release-bringt-direkt-20-spiele-mit-sich/</t>
+          <t>https://games.24tv.ua/ru/startovali-prodazhi-nintendo-switch-2-v-kakih-stranah-dostupna-konsol-games_n2839620/amp</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2, Mario Kart World and more than 20 other titles are now available. Nintendo Switch 2 is the first new Nintendo console to be released since the introduction of Nintendo Switch eight years ago. The new Joy-Con 2 controllers are magnetically attached to the console and can be operated like a mouse by sliding them on a surface.</t>
+          <t>Nintendo decided to seriously oppose speculators who traditionally buy consoles for resale at an inflated price. Fans began to take seats in queues a few hours before the opening of the stores. Some even took a break from work to buy a novelty.</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>1.0810165</v>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>2025-06-05T15:28:24+00:00</t>
-        </is>
-      </c>
+        <v>1.0896988</v>
+      </c>
+      <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
-          <t>['If a compatible USB-C camera, such as the Nintendo Switch 2 camera (available separately), is connected, up to four people can also communicate with each other via video chat.', 'To optimize the gaming experience of Nintendo Switch titles on Nintendo Switch 2, there will be free updates for selected games that improve graphics or add new features, for example.2 The content of the free updates varies by game.', 'Sid Meier’s Civilization® VII – Nintendo Switch 2 Edition: Players can now influence the course of history on Nintendo Switch 2.']</t>
+          <t>['It should be noted that neither in Ukraine nor in Russia Nintendo products are officially sold. On the eve of Nvidia CEO Jensen Huang said that Switch 2 will receive special AI processors that improve the gaming experience in real time.']</t>
         </is>
       </c>
       <c r="H63" t="n">
-        <v>0.743</v>
+        <v>-0.1779</v>
       </c>
       <c r="I63" t="n">
-        <v>0.106</v>
+        <v>0</v>
       </c>
       <c r="J63" t="n">
-        <v>0</v>
+        <v>0.042</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>DL-90b89c57db6bd0dda29585ae2b322970</t>
+          <t>DL-9403699c5a8c3acb6752501c45ccc38e</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Switch 2 is important for Nintendo, but also for a Nvidia that does not want to lose ground against AMD.</t>
+          <t>Nintendo Switch 2 – Release brings 20 games directly</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://www.xataka.com/videojuegos/switch-2-importante-para-nintendo-tambien-para-nvidia-que-no-quiere-perder-terreno-amd</t>
+          <t>https://www.toptechnews.de/2025/06/05/nintendo-switch-2-release-bringt-direkt-20-spiele-mit-sich/</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 returns to the load When a leading company, what it wants is to have even more part of the cake. Nvidia dominates the world of PC video games with an iron hand. AMD is doing well with its latest generations, but the singing voice is still carried by the company led by Jensen Huang.</t>
+          <t>Nintendo Switch 2, Mario Kart World and more than 20 other titles are now available. Nintendo Switch 2 is the first new Nintendo console to be released since the introduction of Nintendo Switch eight years ago. The new Joy-Con 2 controllers are magnetically attached to the console and can be operated like a mouse by sliding them on a surface.</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>1.0759926</v>
+        <v>1.0810337</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-06-06T21:47:33+00:00</t>
+          <t>2025-06-05T15:28:24+00:00</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>['Nintendo Switch 2 is here.', 'When a new generation of consoles arrives, beyond the new games and experiences it enables, there is a fundamental issue that may not be of much interest to all users, but is of vital importance to the technology industry: who signs the processor.']</t>
+          <t>['If a compatible USB-C camera, such as the Nintendo Switch 2 camera (available separately), is connected, up to four people can also communicate with each other via video chat.', 'To optimize the gaming experience of Nintendo Switch titles on Nintendo Switch 2, there will be free updates for selected games that improve graphics or add new features, for example.2 The content of the free updates varies by game.', 'Sid Meier’s Civilization® VII – Nintendo Switch 2 Edition: Players can now influence the course of history on Nintendo Switch 2.']</t>
         </is>
       </c>
       <c r="H64" t="n">
-        <v>0.4118</v>
+        <v>0.743</v>
       </c>
       <c r="I64" t="n">
-        <v>0.08400000000000001</v>
+        <v>0.106</v>
       </c>
       <c r="J64" t="n">
         <v>0</v>
@@ -3246,42 +3246,42 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>DL-8eed788f4c6b98f895779a24abd5aba6</t>
+          <t>DL-90b89c57db6bd0dda29585ae2b322970</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 guide: pre-order links, accessories and launch games</t>
+          <t>Switch 2 is important for Nintendo, but also for a Nvidia that does not want to lose ground against AMD.</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>https://www.theshortcut.com/p/nintendo-switch-2-guide-pre-order-live</t>
+          <t>https://www.xataka.com/videojuegos/switch-2-importante-para-nintendo-tambien-para-nvidia-que-no-quiere-perder-terreno-amd</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>There are 10 tech stories in today’s Substack issue of The Shortcut Skip ahead to story 2 to 10 for more Nintendo Switch 2 is arriving at stores across the United States tonight. This is your chance to skip the line. Walmart always has more console inventory and better servers than GameStop.</t>
+          <t>Nintendo Switch 2 returns to the load When a leading company, what it wants is to have even more part of the cake. Nvidia dominates the world of PC video games with an iron hand. AMD is doing well with its latest generations, but the singing voice is still carried by the company led by Jensen Huang.</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>1.0604935</v>
+        <v>1.0760536</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-06-05T03:05:04</t>
+          <t>2025-06-06T21:47:33+00:00</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>['My personal Switch 2 pre-order from Target was delayed at the last minute. So I’m in line – with the diehard Nintendo gamers, some of whom arrived at 8am ET – hoping to secure a Switch 2 from Best Buy at midnight. Review coming soon.\nThe best part?']</t>
+          <t>['Nintendo Switch 2 is here.', 'When a new generation of consoles arrives, beyond the new games and experiences it enables, there is a fundamental issue that may not be of much interest to all users, but is of vital importance to the technology industry: who signs the processor.']</t>
         </is>
       </c>
       <c r="H65" t="n">
-        <v>0.7717000000000001</v>
+        <v>0.4118</v>
       </c>
       <c r="I65" t="n">
-        <v>0.146</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="J65" t="n">
         <v>0</v>
@@ -3290,221 +3290,221 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>DL-cbe41ea394a2ced64f8f9324991f8418</t>
+          <t>DL-8eed788f4c6b98f895779a24abd5aba6</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Osceola County Sheriff Lopez to make first court appearance after facing federal charges</t>
+          <t>Nintendo Switch 2 guide: pre-order links, accessories and launch games</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>https://spotonflorida.com/central-florida/5775312/osceola-county-sheriff-lopez-to-make.html</t>
+          <t>https://www.theshortcut.com/p/nintendo-switch-2-guide-pre-order-live</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Sheriff Marcos Lopez has been booked at Lake County Jail without bond. Over 250,000 pay homage to Pope Francis as world leaders prepare to attend funeral.</t>
+          <t>There are 10 tech stories in today’s Substack issue of The Shortcut Skip ahead to story 2 to 10 for more Nintendo Switch 2 is arriving at stores across the United States tonight. This is your chance to skip the line. Walmart always has more console inventory and better servers than GameStop.</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>1.051199</v>
+        <v>1.0605202</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-06-06T14:15:38+00:00</t>
+          <t>2025-06-05T03:05:04</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>['Environment Day\n09:49 Disneyland ride shuts down after car derails off track: Witness\n08:35 Ex-GOP congressman David Jolly launches Democratic run for Florida governor (Video)\n08:35 Tavares residents concerned over proposed mixed-use development (Video)\n08:35 Experience', "Kissimmee aims to boost visitors through 'gastro tourism,' value-focused vacations (Video)\n08:35 The Morning News | Live Central Florida headlines, weather and traffic (Video)\n08:34 Gamers camp out for Nintendo Switch 2 (Video)\n08:34 Are traffic control"]</t>
+          <t>['My personal Switch 2 pre-order from Target was delayed at the last minute. So I’m in line – with the diehard Nintendo gamers, some of whom arrived at 8am ET – hoping to secure a Switch 2 from Best Buy at midnight. Review coming soon.\nThe best part?']</t>
         </is>
       </c>
       <c r="H66" t="n">
-        <v>-0.2969</v>
+        <v>0.7717000000000001</v>
       </c>
       <c r="I66" t="n">
-        <v>0.048</v>
+        <v>0.146</v>
       </c>
       <c r="J66" t="n">
-        <v>0.093</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>DL-f75243e86744d36c28e7960ee772b4c0</t>
+          <t>DL-cbe41ea394a2ced64f8f9324991f8418</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Microsoft unveils Xbox gaming handheld launching in 2025 (updated with hands-on)</t>
+          <t>Osceola County Sheriff Lopez to make first court appearance after facing federal charges</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>https://venturebeat.com/business/microsoft-unveils-xbox-gaming-handheld-launching-in-2025/</t>
+          <t>https://spotonflorida.com/central-florida/5775312/osceola-county-sheriff-lopez-to-make.html</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Microsoft is diving into the handheld gaming market with its own Xbox-branded handheld in partnership with PC maker Asus. It has the Windows OS, a full Xbox screen experience, and Armoury Crate SE as a central hub for device management. The handheld will compete with rivals such as the Nintendo Switch 2 and the Valve Steam Deck.</t>
+          <t>Sheriff Marcos Lopez has been booked at Lake County Jail without bond. Over 250,000 pay homage to Pope Francis as world leaders prepare to attend funeral.</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>1.0159454</v>
+        <v>1.0512486</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-06-08T20:53:17+00:00</t>
+          <t>2025-06-06T14:15:38+00:00</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>['“The Xbox experience grows with you,” said Sarah Bond, president of Xbox, in the Xbox Showcase.\nThe company plans to launch the handheld in 2025. As such, it will compete with rivals such as the Nintendo Switch 2 and the Valve Steam Deck.', 'This one promises the power of an Xbox experience in your hands. It has a seven-inch IPS VRR screen.\nThe move could inspire both fear and derision, as the prospect for such a move has done in the past.']</t>
+          <t>['Environment Day\n09:49 Disneyland ride shuts down after car derails off track: Witness\n08:35 Ex-GOP congressman David Jolly launches Democratic run for Florida governor (Video)\n08:35 Tavares residents concerned over proposed mixed-use development (Video)\n08:35 Experience', "Kissimmee aims to boost visitors through 'gastro tourism,' value-focused vacations (Video)\n08:35 The Morning News | Live Central Florida headlines, weather and traffic (Video)\n08:34 Gamers camp out for Nintendo Switch 2 (Video)\n08:34 Are traffic control"]</t>
         </is>
       </c>
       <c r="H67" t="n">
-        <v>0.0772</v>
+        <v>-0.2969</v>
       </c>
       <c r="I67" t="n">
-        <v>0.024</v>
+        <v>0.048</v>
       </c>
       <c r="J67" t="n">
-        <v>0</v>
+        <v>0.093</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>DL-1c59b6df7e032db28024c576f73acce5</t>
+          <t>DL-f75243e86744d36c28e7960ee772b4c0</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>It started - Switch 2 with the first technical problems. Difficulties when downloading Mario Kart World</t>
+          <t>Microsoft unveils Xbox gaming handheld launching in 2025 (updated with hands-on)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>https://www.gram.pl/news/zaczelo-sie-switch-2-z-pierwszymi-problemami-technicznymi-utrudnienia-przy-pobieraniu-mario-kart-world</t>
+          <t>https://venturebeat.com/business/microsoft-unveils-xbox-gaming-handheld-launching-in-2025/</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Players who wanted to start their adventure with Nintendo Switch 2 reported serious problems with downloading the game. Error 2813-0171 The phrase "Mario Kart World doesn't want to be downloaded" quickly began to dominate search engines and forums. The source of the problem may be differences in console boot packages.</t>
+          <t>Microsoft is diving into the handheld gaming market with its own Xbox-branded handheld in partnership with PC maker Asus. It has the Windows OS, a full Xbox screen experience, and Armoury Crate SE as a central hub for device management. The handheld will compete with rivals such as the Nintendo Switch 2 and the Valve Steam Deck.</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>1.008112</v>
+        <v>1.0158577</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-06-06T10:10:00</t>
+          <t>2025-06-08T20:53:17+00:00</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>['Users who purchased Nintendo Switch 2 with Mario Kart World graphics printed directly on the box have problems activating the game.', 'In turn, people who purchased the version with the attached sticker and download code, seem not to experience difficulties. GramTV reports: This is confirmed by reports from the USA.']</t>
+          <t>['“The Xbox experience grows with you,” said Sarah Bond, president of Xbox, in the Xbox Showcase.\nThe company plans to launch the handheld in 2025. As such, it will compete with rivals such as the Nintendo Switch 2 and the Valve Steam Deck.', 'This one promises the power of an Xbox experience in your hands. It has a seven-inch IPS VRR screen.\nThe move could inspire both fear and derision, as the prospect for such a move has done in the past.']</t>
         </is>
       </c>
       <c r="H68" t="n">
-        <v>-0.743</v>
+        <v>0.0772</v>
       </c>
       <c r="I68" t="n">
-        <v>0.065</v>
+        <v>0.024</v>
       </c>
       <c r="J68" t="n">
-        <v>0.196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>DL-a693f23c7ac4e39135b5cc47d8513970</t>
+          <t>DL-1c59b6df7e032db28024c576f73acce5</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Shortly before release: Games and accessories for the Nintendo Switch 2</t>
+          <t>It started - Switch 2 with the first technical problems. Difficulties when downloading Mario Kart World</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>https://www.hardwareluxx.de/index.php/news/consumer-electronics/konsolen/66294-kurz-vor-dem-release-spiele-und-zubehoer-fuer-die-nintendo-switch-2.html</t>
+          <t>https://www.gram.pl/news/zaczelo-sie-switch-2-z-pierwszymi-problemami-technicznymi-utrudnienia-przy-pobieraniu-mario-kart-world</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 will finally have a successor next Thursday. A new design with a larger screen and of course a more powerful hardware should make the Switch 2 a real 4K console. Some online retailers such as Amazon, MediaMarkt or Coolblue list the starting title “Mario Kart World” from 79 euros and thus 10 euros below the actual price recommendation. This also applies to "The Legend of Zelda: Tears of the Kingdom"</t>
+          <t>Players who wanted to start their adventure with Nintendo Switch 2 reported serious problems with downloading the game. Error 2813-0171 The phrase "Mario Kart World doesn't want to be downloaded" quickly began to dominate search engines and forums. The source of the problem may be differences in console boot packages.</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>1.0045853</v>
+        <v>1.0081596</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-06-03T08:37:58</t>
+          <t>2025-06-06T10:10:00</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>['Above all, you should purchase an additional memory card when buying the Nintendo Switch 2, because the integrated 256 GB could quickly become scarce. The official Nintendo SanDisk costs with 256 GB already 55 euros.', 'However, all microSD Express cards with a capacity of theoretically up to 2 TB can be used.', 'These should make data transfer rates of at least 800 MB/s possible, which in addition corresponds to the 10-fold of the predecessor and significantly restricts the selection.']</t>
+          <t>['Users who purchased Nintendo Switch 2 with Mario Kart World graphics printed directly on the box have problems activating the game.', 'In turn, people who purchased the version with the attached sticker and download code, seem not to experience difficulties. GramTV reports: This is confirmed by reports from the USA.']</t>
         </is>
       </c>
       <c r="H69" t="n">
-        <v>0.5849</v>
+        <v>-0.743</v>
       </c>
       <c r="I69" t="n">
-        <v>0.099</v>
+        <v>0.065</v>
       </c>
       <c r="J69" t="n">
-        <v>0.028</v>
+        <v>0.196</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>DL-736adae141649efa336e9f7ce03ea527</t>
+          <t>DL-a693f23c7ac4e39135b5cc47d8513970</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 launches today. Here’s what to know</t>
+          <t>Shortly before release: Games and accessories for the Nintendo Switch 2</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>https://localnews8.com/money/cnn-business-consumer/2025/06/05/the-nintendo-switch-2-launches-today-heres-what-to-know/</t>
+          <t>https://www.hardwareluxx.de/index.php/news/consumer-electronics/konsolen/66294-kurz-vor-dem-release-spiele-und-zubehoer-fuer-die-nintendo-switch-2.html</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Nintendo's new console, the Switch 2, arrives on store shelves globally after being announced in April. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table; or on. a TV when plugged in to its accompanying dock, like its predecessor. Nintendo’s decision to stick with a winning template for the Switch 2 is a testament to the original’s popularity.</t>
+          <t>Nintendo Switch 2 will finally have a successor next Thursday. A new design with a larger screen and of course a more powerful hardware should make the Switch 2 a real 4K console. Some online retailers such as Amazon, MediaMarkt or Coolblue list the starting title “Mario Kart World” from 79 euros and thus 10 euros below the actual price recommendation. This also applies to "The Legend of Zelda: Tears of the Kingdom"</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>0.91181374</v>
+        <v>1.0046387</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-06-05T13:14:10</t>
+          <t>2025-06-03T08:37:58</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>['In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.\nNintendo has also given the console hardware a much-needed upgrade.', 'The Switch 2 has a larger 7.9-inch display compared to the original Switch’s 6.2-inch screen, and the Joy-Cons now snap to the console magnetically, which should make them easier to attach or remove from the console.']</t>
+          <t>['Above all, you should purchase an additional memory card when buying the Nintendo Switch 2, because the integrated 256 GB could quickly become scarce. The official Nintendo SanDisk costs with 256 GB already 55 euros.', 'However, all microSD Express cards with a capacity of theoretically up to 2 TB can be used.', 'These should make data transfer rates of at least 800 MB/s possible, which in addition corresponds to the 10-fold of the predecessor and significantly restricts the selection.']</t>
         </is>
       </c>
       <c r="H70" t="n">
-        <v>0.9136</v>
+        <v>0.5849</v>
       </c>
       <c r="I70" t="n">
-        <v>0.194</v>
+        <v>0.099</v>
       </c>
       <c r="J70" t="n">
-        <v>0</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="71">
@@ -3529,7 +3529,7 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>0.91181374</v>
+        <v>0.9118271</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
@@ -3554,7 +3554,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>DL-876ccd4580e6106d2c30aa8425da537a</t>
+          <t>DL-736adae141649efa336e9f7ce03ea527</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -3564,32 +3564,32 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>https://ustimesmirror.com/the-nintendo-switch-2-launches-today-heres-what-to-know/</t>
+          <t>https://localnews8.com/money/cnn-business-consumer/2025/06/05/the-nintendo-switch-2-launches-today-heres-what-to-know/</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Nintendo's new console, the Switch 2, arrives on store shelves globally. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table. Nintendo’s decision to stick with a winning template for the Switch 2 is a testament to the original’s popularity but also a gamble that its success will endure.</t>
+          <t>Nintendo's new console, the Switch 2, arrives on store shelves globally after being announced in April. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table; or on. a TV when plugged in to its accompanying dock, like its predecessor. Nintendo’s decision to stick with a winning template for the Switch 2 is a testament to the original’s popularity.</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>0.91181374</v>
+        <v>0.9118271</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-06-05T15:15:59+00:00</t>
+          <t>2025-06-05T13:14:10</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>['The Switch 2 iterates its predecessor with several new features, including a Game Chat function that lets gamers communicate with other players by tapping a button on the console.', 'In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.\nNintendo has also given the console hardware a much-needed upgrade.']</t>
+          <t>['In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.\nNintendo has also given the console hardware a much-needed upgrade.', 'The Switch 2 has a larger 7.9-inch display compared to the original Switch’s 6.2-inch screen, and the Joy-Cons now snap to the console magnetically, which should make them easier to attach or remove from the console.']</t>
         </is>
       </c>
       <c r="H72" t="n">
-        <v>0.8922</v>
+        <v>0.9136</v>
       </c>
       <c r="I72" t="n">
-        <v>0.212</v>
+        <v>0.194</v>
       </c>
       <c r="J72" t="n">
         <v>0</v>
@@ -3598,123 +3598,123 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>DL-58363b4cfde0e0889c7251f2961ae5ee</t>
+          <t>DL-876ccd4580e6106d2c30aa8425da537a</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 : a promising new breath despite some disillusionment</t>
+          <t>The Nintendo Switch 2 launches today. Here’s what to know</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>https://s2pmag.ch/avis-la-nintendo-switch-2-un-nouveau-souffle-prometteur-malgre-quelques-desillusions/</t>
+          <t>https://ustimesmirror.com/the-nintendo-switch-2-launches-today-heres-what-to-know/</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 has finally slipped into our hands. What lessons can we learn from these first moments of ownership? A complete and careful case The Switch 2 comes in a package with an almost confusing simplicity, compact dimensions that are unmistakably reminiscent of its grandmother. The console is delivered ready for use, accompanied by the necessary accessories to take full advantage of it.</t>
+          <t>Nintendo's new console, the Switch 2, arrives on store shelves globally. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table. Nintendo’s decision to stick with a winning template for the Switch 2 is a testament to the original’s popularity but also a gamble that its success will endure.</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>0.8860931399999999</v>
+        <v>0.9118271</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-06-09T06:16:01</t>
+          <t>2025-06-05T15:15:59+00:00</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>['A balanced review, promises to be confirmed In the end, this Nintendo Switch 2 turns out to be capable of the best as well as the least good, offering contrasting experiences according to titles and usages.']</t>
+          <t>['The Switch 2 iterates its predecessor with several new features, including a Game Chat function that lets gamers communicate with other players by tapping a button on the console.', 'In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.\nNintendo has also given the console hardware a much-needed upgrade.']</t>
         </is>
       </c>
       <c r="H73" t="n">
-        <v>0.5413</v>
+        <v>0.8922</v>
       </c>
       <c r="I73" t="n">
-        <v>0.094</v>
+        <v>0.212</v>
       </c>
       <c r="J73" t="n">
-        <v>0.025</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>DL-d31952a6c00a7f14a8bb1d96ce43f30c</t>
+          <t>DL-58363b4cfde0e0889c7251f2961ae5ee</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Video games: Microsoft unveils the first portable versions of the Xbox</t>
+          <t>The Nintendo Switch 2 : a promising new breath despite some disillusionment</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>https://www.lessentiel.lu/fr/story/jeux-video-microsoft-devoile-les-premieres-versions-portables-de-la-xbox-103361849</t>
+          <t>https://s2pmag.ch/avis-la-nintendo-switch-2-un-nouveau-souffle-prometteur-malgre-quelques-desillusions/</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Xbox portable consoles, ROG Ally and Ally X, designed with Asus, will be marketed for the end of the year celebrations. This Twitter content cannot be displayed due to your current choice of cookies. The price of the consoles and exact date of their launch will be announced in the coming months.</t>
+          <t>The Nintendo Switch 2 has finally slipped into our hands. What lessons can we learn from these first moments of ownership? A complete and careful case The Switch 2 comes in a package with an almost confusing simplicity, compact dimensions that are unmistakably reminiscent of its grandmother. The console is delivered ready for use, accompanied by the necessary accessories to take full advantage of it.</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>0.8757744</v>
+        <v>0.8862343</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-06-10T09:56:00+00:00</t>
+          <t>2025-06-09T06:16:01</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>["Faced with Nintendo Switch 2 The design of both models evokes the brand's traditional handles, with the same buttons, joysticks and handles, but with a longer format to integrate a central screen.", '"Xbox Ally and Xbox Ally X are perfect for players looking for an accessible gaming experience on the go, whether between two planes or between two comfortable lounge chairs," Microsoft said in a press release.']</t>
+          <t>['A balanced review, promises to be confirmed In the end, this Nintendo Switch 2 turns out to be capable of the best as well as the least good, offering contrasting experiences according to titles and usages.']</t>
         </is>
       </c>
       <c r="H74" t="n">
-        <v>0</v>
+        <v>0.5413</v>
       </c>
       <c r="I74" t="n">
-        <v>0</v>
+        <v>0.094</v>
       </c>
       <c r="J74" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>DL-48f470a3b04e45099a9bd8f8b9d0942b</t>
+          <t>DL-d31952a6c00a7f14a8bb1d96ce43f30c</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>What comes in the box of the Nintendo Switch 2? Look at the unboxing of the console, the Pro Controller and the camera.</t>
+          <t>Video games: Microsoft unveils the first portable versions of the Xbox</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>https://www.tecmundo.com.br/voxel/501558-o-que-vem-na-caixa-do-nintendo-switch-2-confira-unboxing-do-console-pro-controller-e-camera.htm</t>
+          <t>https://www.lessentiel.lu/fr/story/jeux-video-microsoft-devoile-les-premieres-versions-portables-de-la-xbox-103361849</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Derek Keller introduces the new model of the Big N, which brings a series of innovations over the first Switch. The new model accompanies the game Mario Kart World, one of the launch titles of the new console. In addition to highlighting the visual and functional changes, the video also reveals technical details and curiosities about the accessories.</t>
+          <t>Xbox portable consoles, ROG Ally and Ally X, designed with Asus, will be marketed for the end of the year celebrations. This Twitter content cannot be displayed due to your current choice of cookies. The price of the consoles and exact date of their launch will be announced in the coming months.</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0.7912369</v>
+        <v>0.8698616</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-06-05T21:33:00+00:00</t>
+          <t>2025-06-10T09:56:00+00:00</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>['In addition to highlighting the visual and functional changes to the device, the video also reveals technical details and curiosities about the accessories, paving the way for the upcoming full reviews that will soon be available on the Voxel channel', "More compact box and redesigned design One of the first noticeable changes on the Nintendo Switch 2 is the new packaging format. Even though it's a physically larger console, the box has been optimized and it's more compact and organized."]</t>
+          <t>["Faced with Nintendo Switch 2 The design of both models evokes the brand's traditional handles, with the same buttons, joysticks and handles, but with a longer format to integrate a central screen.", '"Xbox Ally and Xbox Ally X are perfect for players looking for an accessible gaming experience on the go, whether between two planes or between two comfortable lounge chairs," Microsoft said in a press release.']</t>
         </is>
       </c>
       <c r="H75" t="n">
@@ -3730,130 +3730,130 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>DL-56a2f5145d0be40c3efde1b4a27402f4</t>
+          <t>DL-48f470a3b04e45099a9bd8f8b9d0942b</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: The LCD screen receives fierce criticism from fans and experts - and we too would have liked a different display</t>
+          <t>What comes in the box of the Nintendo Switch 2? Look at the unboxing of the console, the Pro Controller and the camera.</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>https://www.gamepro.de/artikel/nintendo-switch-2-lcd-bildschirm-erntet-heftige-kritik,3434354.html</t>
+          <t>https://www.tecmundo.com.br/voxel/501558-o-que-vem-na-caixa-do-nintendo-switch-2-confira-unboxing-do-console-pro-controller-e-camera.htm</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Switch 2 is out and despite many new display features there is some strong criticism, both from fans and tech enthusiasts. We have therefore looked into it ourselves and also measured it, and we are also disenchanted. The LCD display from the Taiwanese manufacturer InnoLux brings some great functions – for example HDR for higher color dynamics, 120 Hertz and VRR – but also disappoints massively in some central points.</t>
+          <t>Derek Keller introduces the new model of the Big N, which brings a series of innovations over the first Switch. The new model accompanies the game Mario Kart World, one of the launch titles of the new console. In addition to highlighting the visual and functional changes, the video also reveals technical details and curiosities about the accessories.</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>0.78873825</v>
+        <v>0.79125595</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-06-08T17:30:00</t>
+          <t>2025-06-05T21:33:00+00:00</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>['Until a pixel is switched to another color, it takes a while, and the resulting image artifacts are perceived as ghosting or blurring.', 'And in this respect, the Switch 2 display with its 120 Hertz is particularly vulnerable, as many buyers write in the comments below the post. How do we rate the display of the Nintendo Switch 2?']</t>
+          <t>['In addition to highlighting the visual and functional changes to the device, the video also reveals technical details and curiosities about the accessories, paving the way for the upcoming full reviews that will soon be available on the Voxel channel', "More compact box and redesigned design One of the first noticeable changes on the Nintendo Switch 2 is the new packaging format. Even though it's a physically larger console, the box has been optimized and it's more compact and organized."]</t>
         </is>
       </c>
       <c r="H76" t="n">
-        <v>0.1531</v>
+        <v>0</v>
       </c>
       <c r="I76" t="n">
-        <v>0.108</v>
+        <v>0</v>
       </c>
       <c r="J76" t="n">
-        <v>0.073</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>DL-380770c64735dbc1c56d63a05fb4b763</t>
+          <t>DL-56a2f5145d0be40c3efde1b4a27402f4</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>What are the best TVs to choose for the Nintendo Switch 2?</t>
+          <t>Nintendo Switch 2: The LCD screen receives fierce criticism from fans and experts - and we too would have liked a different display</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>https://www.frandroid.com/guide-dachat/2638901_quels-sont-les-meilleurs-tv-a-choisir-pour-la-switch-2</t>
+          <t>https://www.gamepro.de/artikel/nintendo-switch-2-lcd-bildschirm-erntet-heftige-kritik,3434354.html</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 is available and to take full advantage of the power of the new Nintendo console, it is essential to choose a TV at the right height. The definition The Ultra HD 4K definition is now indispensable for the Switch 2, which offers graphics in very high resolution when used in dock mode. This resolution provides an image of remarkable sharpness, with finer details and greater immersion.</t>
+          <t>Switch 2 is out and despite many new display features there is some strong criticism, both from fans and tech enthusiasts. We have therefore looked into it ourselves and also measured it, and we are also disenchanted. The LCD display from the Taiwanese manufacturer InnoLux brings some great functions – for example HDR for higher color dynamics, 120 Hertz and VRR – but also disappoints massively in some central points.</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>0.77731705</v>
+        <v>0.7887001</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-06-07T17:00:06</t>
+          <t>2025-06-08T17:30:00</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>['Philips The One PUS8909 // Source: Philips In short, whether you prefer reactivity, image quality, brightness or immersion, there are now televisions perfectly suited to the Nintendo Switch 2.', 'OLED, Mini LED, QLED or LED, each technology has its advantages, but all the references cited here guarantee a fluid, immersive gaming experience that is faithful to the vision of Nintendo game creators.', 'All you need to know about the Switch 2 Want to know everything about the Nintendo Switch 2 after the Direct announcements? Find our video recap on YouTube for a quick and clear summary.']</t>
+          <t>['Until a pixel is switched to another color, it takes a while, and the resulting image artifacts are perceived as ghosting or blurring.', 'And in this respect, the Switch 2 display with its 120 Hertz is particularly vulnerable, as many buyers write in the comments below the post. How do we rate the display of the Nintendo Switch 2?']</t>
         </is>
       </c>
       <c r="H77" t="n">
-        <v>0.7964</v>
+        <v>0.1531</v>
       </c>
       <c r="I77" t="n">
-        <v>0.114</v>
+        <v>0.108</v>
       </c>
       <c r="J77" t="n">
-        <v>0</v>
+        <v>0.073</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>DL-4de785c3d00dac3779286d8e34763c81</t>
+          <t>DL-380770c64735dbc1c56d63a05fb4b763</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>How to Transfer Your Switch Data to Nintendo Switch 2</t>
+          <t>What are the best TVs to choose for the Nintendo Switch 2?</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>https://www.iphoneincanada.ca/2025/06/05/how-to-transfer-your-data-nintendo-switch-2/</t>
+          <t>https://www.frandroid.com/guide-dachat/2638901_quels-sont-les-meilleurs-tv-a-choisir-pour-la-switch-2</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Nintendo provides a streamlined way to conduct a system transfer from Nintendo Switch to the Switch 2. Players can transfer profile data, save data, screenshots or video, and system settings. Nintendo notes that there is an expiry date for all system transfer data.</t>
+          <t>The Nintendo Switch 2 is available and to take full advantage of the power of the new Nintendo console, it is essential to choose a TV at the right height. The definition The Ultra HD 4K definition is now indispensable for the Switch 2, which offers graphics in very high resolution when used in dock mode. This resolution provides an image of remarkable sharpness, with finer details and greater immersion.</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0.7033539</v>
+        <v>0.7773247</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2025-06-05T11:06:10+00:00</t>
+          <t>2025-06-07T17:00:06</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>['By selecting ‘ I Don’t Have a Nintendo Switch 2 Yet’, you can upload your data to Nintendo’s servers in anticipation of when your Nintendo Switch 2 arrives.', 'Follow the on-screen prompts until you’re sent a ‘Verification code’ to your My Nintendo account email address. Input the code and select ‘Send Data to the Server’. This will then upload your save data to Nintendo’s cloud servers.', 'Once the upload is complete, you can review the system transfer information and select ‘Start Restoring Factory Settings’ to complete the process. Note: This will delete all data from the original console.']</t>
+          <t>['Philips The One PUS8909 // Source: Philips In short, whether you prefer reactivity, image quality, brightness or immersion, there are now televisions perfectly suited to the Nintendo Switch 2.', 'OLED, Mini LED, QLED or LED, each technology has its advantages, but all the references cited here guarantee a fluid, immersive gaming experience that is faithful to the vision of Nintendo game creators.', 'All you need to know about the Switch 2 Want to know everything about the Nintendo Switch 2 after the Direct announcements? Find our video recap on YouTube for a quick and clear summary.']</t>
         </is>
       </c>
       <c r="H78" t="n">
-        <v>0.4939</v>
+        <v>0.7964</v>
       </c>
       <c r="I78" t="n">
-        <v>0.076</v>
+        <v>0.114</v>
       </c>
       <c r="J78" t="n">
         <v>0</v>
@@ -3862,42 +3862,42 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>DL-c7b1d654f43bf3a0aede5a40cc6ebaca</t>
+          <t>DL-4de785c3d00dac3779286d8e34763c81</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>You probably don't have this Switch 2 launch title on your screen and it comes with a pretty cool co-op feature</t>
+          <t>How to Transfer Your Switch Data to Nintendo Switch 2</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>https://www.gamepro.de/artikel/nintendo-switch-2-gameshare-survival-kids,3434002.html</t>
+          <t>https://www.iphoneincanada.ca/2025/06/05/how-to-transfer-your-data-nintendo-switch-2/</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>This week, Nintendo Switch 2 comes out with a whole series of launch titles that you can play directly on the new console on June 5th. This includes Survival Kids, which besides Mario Kart World or Donkey Kong flies rather under the radar. You take on the role of four children who are stranded on an island and explore crafts and the surroundings to find a way home.</t>
+          <t>Nintendo provides a streamlined way to conduct a system transfer from Nintendo Switch to the Switch 2. Players can transfer profile data, save data, screenshots or video, and system settings. Nintendo notes that there is an expiry date for all system transfer data.</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>0.6768379</v>
+        <v>0.7033691399999999</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2025-06-03T11:27:17+00:00</t>
+          <t>2025-06-05T11:06:10+00:00</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>['So you can play locally on a total of three devices as long as at least one person in the group has a Nintendo Switch 2 and the game supports GameShare. In the case of Survival Kids, the game runs via GameShare with two consoles for both in 60 fps.', 'On the other hand, if you start on three devices, the frame rate is reduced to 30 fps for everyone involved. Nevertheless, this way of playing together is a cool thing that has a lot of potential.']</t>
+          <t>['By selecting ‘ I Don’t Have a Nintendo Switch 2 Yet’, you can upload your data to Nintendo’s servers in anticipation of when your Nintendo Switch 2 arrives.', 'Follow the on-screen prompts until you’re sent a ‘Verification code’ to your My Nintendo account email address. Input the code and select ‘Send Data to the Server’. This will then upload your save data to Nintendo’s cloud servers.', 'Once the upload is complete, you can review the system transfer information and select ‘Start Restoring Factory Settings’ to complete the process. Note: This will delete all data from the original console.']</t>
         </is>
       </c>
       <c r="H79" t="n">
-        <v>0.34</v>
+        <v>0.4939</v>
       </c>
       <c r="I79" t="n">
-        <v>0.036</v>
+        <v>0.076</v>
       </c>
       <c r="J79" t="n">
         <v>0</v>
@@ -3906,440 +3906,484 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>DL-194cd17a14f69417b82c9c6d47023133</t>
+          <t>DL-c7b1d654f43bf3a0aede5a40cc6ebaca</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>High demand makes Nintendo Switch 2 sell out in Brazil on its first day of release.</t>
+          <t>You probably don't have this Switch 2 launch title on your screen and it comes with a pretty cool co-op feature</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>https://www1.folha.uol.com.br/tec/2025/06/alta-demanda-faz-nintendo-switch-2-esgotar-no-brasil-no-primeiro-dia-de-vendas.shtml</t>
+          <t>https://www.gamepro.de/artikel/nintendo-switch-2-gameshare-survival-kids,3434002.html</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2, a new video game console from the Japanese company, went off the shelf this Friday in the global markets. It's already sold out in major Brazilian stores due to high demand. The console has a suggested price of R$4,499.90 in the standard version, no games.</t>
+          <t>This week, Nintendo Switch 2 comes out with a whole series of launch titles that you can play directly on the new console on June 5th. This includes Survival Kids, which besides Mario Kart World or Donkey Kong flies rather under the radar. You take on the role of four children who are stranded on an island and explore crafts and the surroundings to find a way home.</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>0.6761894000000001</v>
+        <v>0.67687225</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2025-06-05T21:23:16+00:00</t>
+          <t>2025-06-03T11:27:17+00:00</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>['Ampere predicts that Switch 2 sales will surpass 100 million units by 2030. See more about the Nintendo Switch 2.', 'Novelties The new console will have an improved 7.9-inch LCD screen, with HDR support and refresh rates of up to 120 Hz, ensuring smoother display.']</t>
+          <t>['So you can play locally on a total of three devices as long as at least one person in the group has a Nintendo Switch 2 and the game supports GameShare. In the case of Survival Kids, the game runs via GameShare with two consoles for both in 60 fps.', 'On the other hand, if you start on three devices, the frame rate is reduced to 30 fps for everyone involved. Nevertheless, this way of playing together is a cool thing that has a lot of potential.']</t>
         </is>
       </c>
       <c r="H80" t="n">
-        <v>-0.4019</v>
+        <v>0.34</v>
       </c>
       <c r="I80" t="n">
-        <v>0</v>
+        <v>0.036</v>
       </c>
       <c r="J80" t="n">
-        <v>0.081</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>DL-1f7196f9804c69956dd1ea78f94a50cf</t>
+          <t>DL-194cd17a14f69417b82c9c6d47023133</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Switch 2: Why Nintendo doesn't want you to remove the display slide</t>
+          <t>High demand makes Nintendo Switch 2 sell out in Brazil on its first day of release.</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>https://t3n.de/news/switch-2-nintendo-display-folie-1691041/</t>
+          <t>https://www1.folha.uol.com.br/tec/2025/06/alta-demanda-faz-nintendo-switch-2-esgotar-no-brasil-no-primeiro-dia-de-vendas.shtml</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>On June 5, 2025, the new Nintendo console Switch 2 will officially go on sale. Pre-ordering is currently not possible on major online trading platforms. It is currently unknown when the console will be available again. Nintendo explicitly warns against removing the factory-mounted display slide.</t>
+          <t>Nintendo Switch 2, a new video game console from the Japanese company, went off the shelf this Friday in the global markets. It's already sold out in major Brazilian stores due to high demand. The console has a suggested price of R$4,499.90 in the standard version, no games.</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>0.6726607999999999</v>
+        <v>0.6762066</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2025-06-04T11:45:37</t>
+          <t>2025-06-05T21:23:16+00:00</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>['Switch 2 is supposed to get new charging mode Nintendo is supposed to have found a solution for this with the Switch 2 – namely a battery-saving charging mode as usual with smartphones.', "View 8 images This retro technology has collector's value today Source: More on this topic MIT Technology Review Nintendo"]</t>
+          <t>['Ampere predicts that Switch 2 sales will surpass 100 million units by 2030. See more about the Nintendo Switch 2.', 'Novelties The new console will have an improved 7.9-inch LCD screen, with HDR support and refresh rates of up to 120 Hz, ensuring smoother display.']</t>
         </is>
       </c>
       <c r="H81" t="n">
-        <v>-0.1027</v>
+        <v>-0.4019</v>
       </c>
       <c r="I81" t="n">
         <v>0</v>
       </c>
       <c r="J81" t="n">
-        <v>0.032</v>
+        <v>0.081</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>DL-0baa3766bc883eba68c2dbbae1038cce</t>
+          <t>DL-1f7196f9804c69956dd1ea78f94a50cf</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Donkey Kong Bananza: Release date, trailer and highlights</t>
+          <t>Switch 2: Why Nintendo doesn't want you to remove the display slide</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>https://www.netcost-security.fr/mobilite/252228/donkey-kong-bananza-date-de-sortie-bande-annonce-et-exclusivites-eclairantes/</t>
+          <t>https://t3n.de/news/switch-2-nintendo-display-folie-1691041/</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 is now available with an exciting set of new games. Donkey Kong Bonanza is a must-see for fans of the iconic character. Discover key details, including the release date and pre-command options.</t>
+          <t>On June 5, 2025, the new Nintendo console Switch 2 will officially go on sale. Pre-ordering is currently not possible on major online trading platforms. It is currently unknown when the console will be available again. Nintendo explicitly warns against removing the factory-mounted display slide.</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>0.6710968</v>
+        <v>0.67266464</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2025-06-06T16:22:33+00:00</t>
+          <t>2025-06-04T11:45:37</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>['To make the Switch 2 more attractive, Nintendo has released a number of games compatible only with this console. One of the games in question is a new title with Donkey Kong.', 'We will review the details of the new game, the release date of Donkey Kong Bonanza, the price, the pre-order options and the gameplay. Note that this game is only available for the Nintendo Switch 2.']</t>
+          <t>['Switch 2 is supposed to get new charging mode Nintendo is supposed to have found a solution for this with the Switch 2 – namely a battery-saving charging mode as usual with smartphones.', "View 8 images This retro technology has collector's value today Source: More on this topic MIT Technology Review Nintendo"]</t>
         </is>
       </c>
       <c r="H82" t="n">
-        <v>0.4939</v>
+        <v>-0.1027</v>
       </c>
       <c r="I82" t="n">
-        <v>0.08400000000000001</v>
+        <v>0</v>
       </c>
       <c r="J82" t="n">
-        <v>0</v>
+        <v>0.032</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>DL-c530336e1b88c22a95418a5f5123d3a8</t>
+          <t>DL-0baa3766bc883eba68c2dbbae1038cce</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>I think Nintendo played it very safe with Switch 2 - but that's not a bad thing</t>
+          <t>Donkey Kong Bananza: Release date, trailer and highlights</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>https://www.indy100.com/gaming/nintendo-switch-2-first-impressions-features-gameplay-gamechat-gameshare</t>
+          <t>https://www.netcost-security.fr/mobilite/252228/donkey-kong-bananza-date-de-sortie-bande-annonce-et-exclusivites-eclairantes/</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Nintendo has just straight up called this the Switch 2 - no SNES, Wii-U or 3DS confusion here, it's clearly a successor to the Switch. This is very indicative of the route Nintendo has gone down with the new console. It's undeniably more of an upgrade rather than something completely new and revolutionary with Nintendo seemingly playing it very safe. There are now a lot more competitors in this market because of its success, such as the Steam Deck.</t>
+          <t>The Nintendo Switch 2 is now available with an exciting set of new games. Donkey Kong Bonanza is a must-see for fans of the iconic character. Discover key details, including the release date and pre-command options.</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>0.658247</v>
+        <v>0.67111206</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2025-06-05T15:07:15</t>
+          <t>2025-06-06T16:22:33+00:00</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>['With the Switch and this concept proving such a hit, Nintendo has understandably not wanted to veer too much away from what made the original Switch so successful, instead refining the experience with the Switch 2 with new features, better performance']</t>
+          <t>['To make the Switch 2 more attractive, Nintendo has released a number of games compatible only with this console. One of the games in question is a new title with Donkey Kong.', 'We will review the details of the new game, the release date of Donkey Kong Bonanza, the price, the pre-order options and the gameplay. Note that this game is only available for the Nintendo Switch 2.']</t>
         </is>
       </c>
       <c r="H83" t="n">
-        <v>0.8687</v>
+        <v>0.4939</v>
       </c>
       <c r="I83" t="n">
-        <v>0.175</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="J83" t="n">
-        <v>0.051</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>DL-fb44e9ba1c36059416a5f81b3d4717bc</t>
+          <t>DL-c530336e1b88c22a95418a5f5123d3a8</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 is here - first impressions</t>
+          <t>I think Nintendo played it very safe with Switch 2 - but that's not a bad thing</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>https://www.gram.pl/artykul/nintendo-switch-2-juz-tu-jest-pierwsze-wrazenia</t>
+          <t>https://www.indy100.com/gaming/nintendo-switch-2-first-impressions-features-gameplay-gamechat-gameshare</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 is one of my favorite consoles, which has accompanied me in various roles for over eight years. The first Switch was with me until the release of the OLED version in 2021. I forgave myself for Lite, because it did not correspond to my preferences of playing mainly on TV.</t>
+          <t>Nintendo has just straight up called this the Switch 2 - no SNES, Wii-U or 3DS confusion here, it's clearly a successor to the Switch. This is very indicative of the route Nintendo has gone down with the new console. It's undeniably more of an upgrade rather than something completely new and revolutionary with Nintendo seemingly playing it very safe. There are now a lot more competitors in this market because of its success, such as the Steam Deck.</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>0.62556076</v>
+        <v>0.6582527</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2025-06-07T19:00:00</t>
+          <t>2025-06-05T15:07:15</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>['But when the long-awaited Switch 2 appeared on the horizon, placing a pre-release order was obvious.', 'I will immediately point out that this text is not a racial review of the equipment, but rather an impression, a collection of first impressions and thoughts about the new Nintendo toy.', 'Nintendo Switch 2 is a console that can be labeled the “new generation”, and at the same time it is very strongly rooted in what the first Switch accustomed us to. More a subdued but significant evolution than a surprising revolution.']</t>
+          <t>['With the Switch and this concept proving such a hit, Nintendo has understandably not wanted to veer too much away from what made the original Switch so successful, instead refining the experience with the Switch 2 with new features, better performance']</t>
         </is>
       </c>
       <c r="H84" t="n">
-        <v>0.7351</v>
+        <v>0.8687</v>
       </c>
       <c r="I84" t="n">
-        <v>0.133</v>
+        <v>0.175</v>
       </c>
       <c r="J84" t="n">
-        <v>0</v>
+        <v>0.051</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>DL-6f733f86e304a8935fcf4754a27bb178</t>
+          <t>DL-fb44e9ba1c36059416a5f81b3d4717bc</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>New Florida education commissioner selected, Trump and Putin discuss Ukraine and Iran and Pasco County launches "Summer Haul Pass"</t>
+          <t>Nintendo Switch 2 is here - first impressions</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>https://baynews9.com/fl/tampa/evening-briefing/2025/06/04/evening-briefing-tampa-june-4-2025</t>
+          <t>https://www.gram.pl/artykul/nintendo-switch-2-juz-tu-jest-pierwsze-wrazenia</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Your Weather Planner It will be partly to mostly cloudy on Thursday with highs in the upper 80s. Low temperatures fall to the mid 70s overnight with scattered storms ending in the evening. Donald Trump talks to Putin on Ukraine and Iran, says it was 'not a conversation that will lead to immediate Peace'</t>
+          <t>Nintendo Switch 2 is one of my favorite consoles, which has accompanied me in various roles for over eight years. The first Switch was with me until the release of the OLED version in 2021. I forgave myself for Lite, because it did not correspond to my preferences of playing mainly on TV.</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>0.6108513</v>
+        <v>0.6255646</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2025-06-04T20:45:00+00:00</t>
+          <t>2025-06-07T19:00:00</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>["NATO defence ministers meeting\nBET Experience 2025, annual week of 'entertainment, engagement, and empowerment all anchored in the brilliance and creativity of Black culture' ahead of the Black Entertainment Television\nNintendo releases the new Nintendo", 'Switch 2 games console, which features a bigger screen and better graphics than its predecessor.']</t>
+          <t>['But when the long-awaited Switch 2 appeared on the horizon, placing a pre-release order was obvious.', 'I will immediately point out that this text is not a racial review of the equipment, but rather an impression, a collection of first impressions and thoughts about the new Nintendo toy.', 'Nintendo Switch 2 is a console that can be labeled the “new generation”, and at the same time it is very strongly rooted in what the first Switch accustomed us to. More a subdued but significant evolution than a surprising revolution.']</t>
         </is>
       </c>
       <c r="H85" t="n">
-        <v>0.34</v>
+        <v>0.7351</v>
       </c>
       <c r="I85" t="n">
-        <v>0.064</v>
+        <v>0.133</v>
       </c>
       <c r="J85" t="n">
-        <v>0.038</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>DL-52361e315938e25ca5f998c23b324103</t>
+          <t>DL-6f733f86e304a8935fcf4754a27bb178</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: Should I buy it now or wait?</t>
+          <t>New Florida education commissioner selected, Trump and Putin discuss Ukraine and Iran and Pasco County launches "Summer Haul Pass"</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>https://www.presse-citron.net/nintendo-switch-2-faut-il-lacheter-maintenant-ou-attendre/</t>
+          <t>https://baynews9.com/fl/tampa/evening-briefing/2025/06/04/evening-briefing-tampa-june-4-2025</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Nintendo is changing its habits with the Switch 2. For the first time in years, the Kyoto firm did not send its console to journalists several weeks before the launch. As a result, in-depth testing will arrive after the sale, leaving some players in uncertainty.</t>
+          <t>Your Weather Planner It will be partly to mostly cloudy on Thursday with highs in the upper 80s. Low temperatures fall to the mid 70s overnight with scattered storms ending in the evening. Donald Trump talks to Putin on Ukraine and Iran, says it was 'not a conversation that will lead to immediate Peace'</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>0.4359665</v>
+        <v>0.6108513</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2025-06-05T10:19:31+00:00</t>
+          <t>2025-06-04T20:45:00+00:00</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>['So, are we buying Switch 2 today or not? The decision ultimately depends on your player profile and your priorities. The unconditional Nintendo fans and early adopters assumed will in any case dark without remorse.', 'I think the more measured players will benefit from waiting for our full review next week by identifying the console’s strengths and weaknesses, and then being able to make a fully informed choice.']</t>
+          <t>["NATO defence ministers meeting\nBET Experience 2025, annual week of 'entertainment, engagement, and empowerment all anchored in the brilliance and creativity of Black culture' ahead of the Black Entertainment Television\nNintendo releases the new Nintendo", 'Switch 2 games console, which features a bigger screen and better graphics than its predecessor.']</t>
         </is>
       </c>
       <c r="H86" t="n">
-        <v>-0.34</v>
+        <v>0.34</v>
       </c>
       <c r="I86" t="n">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J86" t="n">
-        <v>0.053</v>
+        <v>0.038</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>DL-265565bae7e63a61079d64b43bdbf11e</t>
+          <t>DL-52361e315938e25ca5f998c23b324103</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: What is the real power of the console Cyberpunk 2077 answers</t>
+          <t>Nintendo Switch 2: Should I buy it now or wait?</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>https://diariodelyaqui.mx/nacional/nintendo-switch-2-cual-es-la-verdadera-potencia-de-la-consola-cyberpunk-2077-lo-responde/110733</t>
+          <t>https://www.presse-citron.net/nintendo-switch-2-faut-il-lacheter-maintenant-ou-attendre/</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Cyberpunk 2077 has been a technically demanding game. This is why it was a surprise to see it run smoothly on Nintendo Switch 2 with a good graphical level. The CD Projekt Red game has served as an unofficial but very revealing test of the console's potential.</t>
+          <t>Nintendo is changing its habits with the Switch 2. For the first time in years, the Kyoto firm did not send its console to journalists several weeks before the launch. As a result, in-depth testing will arrive after the sale, leaving some players in uncertainty.</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>0.38474274</v>
+        <v>0.43597412</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2025-06-06T00:00:00</t>
+          <t>2025-06-05T10:19:31+00:00</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>['COMPARISON WITH OTHER CONSOLIDATIONS An analysis conducted by the Bits Analyzer channel compared the performance of Cyberpunk 2077 on Switch 2 to that of PS4 Pro and Xbox Series S.', "In 'Quality' mode, the Nintendo console achieves 1080p on both laptop and desktop thanks to the DLSS.", "In 'Resolution' mode, it maintains this resolution on the dock, but on the laptop it drops to 720p, with an increase in frame rate of up to 40 fps, although not always stable."]</t>
+          <t>['So, are we buying Switch 2 today or not? The decision ultimately depends on your player profile and your priorities. The unconditional Nintendo fans and early adopters assumed will in any case dark without remorse.', 'I think the more measured players will benefit from waiting for our full review next week by identifying the console’s strengths and weaknesses, and then being able to make a fully informed choice.']</t>
         </is>
       </c>
       <c r="H87" t="n">
-        <v>0.2617</v>
+        <v>-0.34</v>
       </c>
       <c r="I87" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="J87" t="n">
-        <v>0.033</v>
+        <v>0.053</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>DL-d75fb6cd5f8f9f354bda0b190d88b772</t>
+          <t>DL-265565bae7e63a61079d64b43bdbf11e</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>10 Tech Stocks on Wall Street’s Radar</t>
+          <t>Nintendo Switch 2: What is the real power of the console Cyberpunk 2077 answers</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>https://www.insidermonkey.com/blog/10-tech-stocks-on-wall-streets-radar-1549836/</t>
+          <t>https://diariodelyaqui.mx/nacional/nintendo-switch-2-cual-es-la-verdadera-potencia-de-la-consola-cyberpunk-2077-lo-responde/110733</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Mark Malek said that not all sectors react the same to market headlines. He added that news can even create chances for late investors to join in. In fact, the opportunity in the mid to long term will transcend these sort of news items.</t>
+          <t>Cyberpunk 2077 has been a technically demanding game. This is why it was a surprise to see it run smoothly on Nintendo Switch 2 with a good graphical level. The CD Projekt Red game has served as an unofficial but very revealing test of the console's potential.</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>0.2867546</v>
+        <v>0.38476562</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2025-06-09T14:02:05+00:00</t>
+          <t>2025-06-06T00:00:00</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>['On June 5, B.Riley increased its price target on Silicon Motion Technology Corporation (NASDAQ:SIMO) to $90 from $75 and reaffirmed its Buy rating on the stock.', 'The firm pointed to the expanded Nvidia Bluefield DPU win and the upcoming Nintendo Switch 2 cycle as drivers of longer-term gains for the company.']</t>
+          <t>['COMPARISON WITH OTHER CONSOLIDATIONS An analysis conducted by the Bits Analyzer channel compared the performance of Cyberpunk 2077 on Switch 2 to that of PS4 Pro and Xbox Series S.', "In 'Quality' mode, the Nintendo console achieves 1080p on both laptop and desktop thanks to the DLSS.", "In 'Resolution' mode, it maintains this resolution on the dock, but on the laptop it drops to 720p, with an increase in frame rate of up to 40 fps, although not always stable."]</t>
         </is>
       </c>
       <c r="H88" t="n">
-        <v>0.7845</v>
+        <v>0.2617</v>
       </c>
       <c r="I88" t="n">
-        <v>0.182</v>
+        <v>0.08</v>
       </c>
       <c r="J88" t="n">
-        <v>0</v>
+        <v>0.033</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
+          <t>DL-d75fb6cd5f8f9f354bda0b190d88b772</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>10 Tech Stocks on Wall Street’s Radar</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://www.insidermonkey.com/blog/10-tech-stocks-on-wall-streets-radar-1549836/</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Mark Malek said that not all sectors react the same to market headlines. He added that news can even create chances for late investors to join in. In fact, the opportunity in the mid to long term will transcend these sort of news items.</t>
+        </is>
+      </c>
+      <c r="E89" t="n">
+        <v>0.28679657</v>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>2025-06-09T14:02:05+00:00</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>['On June 5, B.Riley increased its price target on Silicon Motion Technology Corporation (NASDAQ:SIMO) to $90 from $75 and reaffirmed its Buy rating on the stock.', 'The firm pointed to the expanded Nvidia Bluefield DPU win and the upcoming Nintendo Switch 2 cycle as drivers of longer-term gains for the company.']</t>
+        </is>
+      </c>
+      <c r="H89" t="n">
+        <v>0.7845</v>
+      </c>
+      <c r="I89" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="J89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
           <t>DL-1c749b3242262132fa02efa86da3ad6e</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="B90" t="inlineStr">
         <is>
           <t>Mario Kart World review: You need to know these things before it drops</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
+      <c r="C90" t="inlineStr">
         <is>
           <t>https://www.the-independent.com/extras/indybest/gadgets-tech/video-games-consoles/mario-kart-world-review-b2763892.html</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr">
+      <c r="D90" t="inlineStr">
         <is>
           <t>Your support helps us to tell the story Read more Support Now From reproductive rights to climate change to Big Tech, The Independent is on the ground when the story is developing. Your donation allows us to keep sending journalists to both sides of the story. We choose not to lock Americans out of our reporting and analysis with paywalls. Expectations are sky-high for the latest entry in the 33-year-old racing series, which carries the weight of a new console’s fortunes on its shoulders.</t>
         </is>
       </c>
-      <c r="E89" t="n">
+      <c r="E90" t="n">
         <v>0.15307999</v>
       </c>
-      <c r="F89" t="inlineStr">
+      <c r="F90" t="inlineStr">
         <is>
           <t>2025-06-04T20:26:36</t>
         </is>
       </c>
-      <c r="G89" t="inlineStr">
+      <c r="G90" t="inlineStr">
         <is>
           <t>['That feels choppy compared to the silky smooth frame rate of single player mode at first, but your eyes will adjust to the difference before you’ve finished your first race.\nopen image in gallery Split-screen dials back the frame rate but keeps 24-player', 'races and the ability to explore the open world ( Nintendo )\nAs an aside, if you don’t think you can spot the difference between games running at 30, 60 and 120 frames per second, the Nintendo Switch 2 Welcome Tour has a special minigame where you can']</t>
         </is>
       </c>
-      <c r="H89" t="n">
+      <c r="H90" t="n">
         <v>0.7906</v>
       </c>
-      <c r="I89" t="n">
+      <c r="I90" t="n">
         <v>0.089</v>
       </c>
-      <c r="J89" t="n">
+      <c r="J90" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4472,10 +4516,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B2" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
worked on more backend stuff
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>320.6878</v>
+        <v>452.00644</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
@@ -530,42 +530,42 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DL-56b3456fa4d4c2c0316f8c748ec38942</t>
+          <t>DL-735f6f5e7ee6d998aecda59ababcdbcc</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 Welcome Tour Review</t>
+          <t>How I plan to review the Nintendo Switch 2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.rocketchainsaw.com.au/review/nintendo-switch-2-welcome-tour-review/</t>
+          <t>https://www.theverge.com/nintendo/679346/nintendo-switch-2-review-guidelines-plan-launch</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>The Welcome Tour is presented as a virtual museum, an enormous virtual representation of the Switch 2. The camera is set high from an isometric perspective, sometimes zooming out to encompass an entire area with people browsing the exhibits like ants. There’s even some mildly funny dialogue and little set pieces thrown in among the attendees you can chat to.</t>
+          <t>Nintendo has decided to not send out early review units to The Verge or other outlets, citing the need for day-one software updates. It’s a way to explore every facet of a new console and get a wide variety of perspectives. This time, we’re going to start with those deeper dives.</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>163.0597</v>
+        <v>253.22185</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-06-09T04:20:44+00:00</t>
+          <t>2025-06-04T12:00:00+00:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Almost everything about the Switch 2 ahead of launch has been a little weird, from the confusing messaging and high pricing to the unfortunately timed connection with spiking tariffs.', 'Intent to keep that strange energy going, Nintendo has decided to not send out early review units to The Verge or other outlets, citing the need for day-one software updates. (This was not the case with the original Switch.)']</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0.8126</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.132</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -574,42 +574,42 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DL-2a418e6f75f602bcd521348ca4edc33a</t>
+          <t>DL-56b3456fa4d4c2c0316f8c748ec38942</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 Camera review - good for GameChat but not much else</t>
+          <t>Nintendo Switch 2 Welcome Tour Review</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.pockettactics.com/nintendo-switch-2-camera-review</t>
+          <t>https://www.rocketchainsaw.com.au/review/nintendo-switch-2-welcome-tour-review/</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>I'm talking about the Nintendo Switch 2 Camera. It doesn't have many uses outside of GameChat, the Switch 2's new social feature, and a few Mario Party Jamboree – Switch 2 Edition minigames. At Pocket Tactics, our experts spend days testing games, phones, tech, and services. We always share honest opinions to help you buy the best.</t>
+          <t>The Welcome Tour is presented as a virtual museum, an enormous virtual representation of the Switch 2. The camera is set high from an isometric perspective, sometimes zooming out to encompass an entire area with people browsing the exhibits like ants. There’s even some mildly funny dialogue and little set pieces thrown in among the attendees you can chat to.</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>157.74315</v>
+        <v>248.0075</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-06-07T16:55:45</t>
+          <t>2025-06-09T04:20:44+00:00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>["Unlike most reviews on Pocket Tactics, I'm not scoring the Nintendo Switch 2 Camera out of 10 right now. That's because I've not used any other Switch 2 cameras, so there's no prior context to base a score on.", "For more of our post-launch coverage, be sure to take a look at our Nintendo Switch 2 review, Nintendo Switch 2 Pro Controller review, and Mario Kart World review while you're here.", "Or, if you'd rather grab something to complete your new gaming setup, see our guides to the best Nintendo Switch 2 accessories and the best Nintendo Switch 2 controllers."]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>0.9337</v>
+        <v>0.8126</v>
       </c>
       <c r="I4" t="n">
-        <v>0.247</v>
+        <v>0.132</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -618,306 +618,306 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DL-251c66dcd4b421aa53f620b9134f31c2</t>
+          <t>DL-2a418e6f75f602bcd521348ca4edc33a</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Nintendo confirms no Switch 2 reviews ahead of launch</t>
+          <t>Nintendo Switch 2 Camera review - good for GameChat but not much else</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://mobilesyrup.com/2025/06/03/nintendo-confirms-no-switch-2-reviews/</t>
+          <t>https://www.pockettactics.com/nintendo-switch-2-camera-review</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Report from Video Game Chronicle says a company spokesperson confirmed there would be no pre-launch review units for the press. Further, the report suggests that the press will receive units after launch once an update with unnamed “important features” hits on June 5. This is likely an excuse since consoles have been at events worldwide.</t>
+          <t>I'm talking about the Nintendo Switch 2 Camera. It doesn't have many uses outside of GameChat, the Switch 2's new social feature, and a few Mario Party Jamboree – Switch 2 Edition minigames. At Pocket Tactics, our experts spend days testing games, phones, tech, and services. We always share honest opinions to help you buy the best.</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>146.0713</v>
+        <v>225.95374</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-06-03T20:53:17+00:00</t>
+          <t>2025-06-07T16:55:45</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['That’s not to say that Nintendo expects Switch 2 reviews to be bad; I expect it to be the opposite. However, the press is unpredictable, so one rogue bug or a wave of people against the new price could derail the hype around the console.']</t>
+          <t>["Unlike most reviews on Pocket Tactics, I'm not scoring the Nintendo Switch 2 Camera out of 10 right now. That's because I've not used any other Switch 2 cameras, so there's no prior context to base a score on.", "For more of our post-launch coverage, be sure to take a look at our Nintendo Switch 2 review, Nintendo Switch 2 Pro Controller review, and Mario Kart World review while you're here.", "Or, if you'd rather grab something to complete your new gaming setup, see our guides to the best Nintendo Switch 2 accessories and the best Nintendo Switch 2 controllers."]</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>-0.0258</v>
+        <v>0.9337</v>
       </c>
       <c r="I5" t="n">
-        <v>0.055</v>
+        <v>0.247</v>
       </c>
       <c r="J5" t="n">
-        <v>0.039</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DL-735f6f5e7ee6d998aecda59ababcdbcc</t>
+          <t>DL-251c66dcd4b421aa53f620b9134f31c2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>How I plan to review the Nintendo Switch 2</t>
+          <t>Nintendo confirms no Switch 2 reviews ahead of launch</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.theverge.com/nintendo/679346/nintendo-switch-2-review-guidelines-plan-launch</t>
+          <t>https://mobilesyrup.com/2025/06/03/nintendo-confirms-no-switch-2-reviews/</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Nintendo has decided to not send out early review units to The Verge or other outlets, citing the need for day-one software updates. It’s a way to explore every facet of a new console and get a wide variety of perspectives. This time, we’re going to start with those deeper dives.</t>
+          <t>Report from Video Game Chronicle says a company spokesperson confirmed there would be no pre-launch review units for the press. Further, the report suggests that the press will receive units after launch once an update with unnamed “important features” hits on June 5. This is likely an excuse since consoles have been at events worldwide.</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>76.48631</v>
+        <v>218.52092</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-06-04T12:00:00+00:00</t>
+          <t>2025-06-03T20:53:17+00:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['Almost everything about the Switch 2 ahead of launch has been a little weird, from the confusing messaging and high pricing to the unfortunately timed connection with spiking tariffs.', 'Intent to keep that strange energy going, Nintendo has decided to not send out early review units to The Verge or other outlets, citing the need for day-one software updates. (This was not the case with the original Switch.)']</t>
+          <t>['That’s not to say that Nintendo expects Switch 2 reviews to be bad; I expect it to be the opposite. However, the press is unpredictable, so one rogue bug or a wave of people against the new price could derail the hype around the console.']</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>-0.0258</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>0.055</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>0.039</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DL-ccc15128eb3abd5f12b5083c5890631b</t>
+          <t>DL-71efe679f350333810130f285a628d0b</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 Welcome Tour - Unique console launch experience</t>
+          <t>Nintendo Switch 2 Improves Pokémon Karmesin and Purple with Graphics and Frame Rate Update</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.playcentral.de/nintendo-switch-2-welcome-tour-einzigartiges-spielerlebnis-zur-einfuehrung-der-konsole/</t>
+          <t>https://www.playcentral.de/nintendo-switch-2-verbessert-pokemon-karmesin-und-purpur-mit-grafik-und-bildraten-update/</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Nintendo is known for its unusual and charming games that stand out from the competition. The Nintendo Switch 2 Welcome Tour is designed as an introduction to the new system. It shows both great new features like mouse support as well as obvious inclusions like the HD Rumble. From an educational perspective, it is fascinating to see what design decisions are behind the console.</t>
+          <t>Version 4.0.0, released on June 2, 2025, brings several improvements when the game is played on the Nintendo Switch 2. This means that as soon as Switch 2 is available, players can download the update and enjoy everything it has to offer. These improvements could eliminate some of the biggest criticisms of Pokémon Karmesin and Purple.</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>65.02419999999999</v>
+        <v>78.859695</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-06-03T22:22:32</t>
+          <t>2025-06-03T15:01:19</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>["The price of the Nintendo Switch 2 Welcome Tour is hotly debated. With only 9.99 euros to start, the game is relatively cheap. However, some fans argue that it should have been offered as an add-on, similar to Astro's Playroom on the PS5.", 'Interactive experiences and challenges What interactive elements does the game offer? The content of the game is a mixture of quizzes, mini-games and technical demos.']</t>
+          <t>['The release of the Nintendo Switch 2 is near, and with it come significant improvements for the popular games Pokémon Karmesin and Purple. These titles from 2022 will experience improved graphics and frame rate thanks to the new console.', 'Although the Nintendo Switch 2 will only be available on June 5, 2025, the major update for these games has already been released and upgrades them to version 4.0.0.', 'The graphics have been optimized for the display of the Nintendo Switch 2 and high-resolution televisions, resulting in improved image quality. In addition, the frame rate has been improved so that the games run more smoothly.']</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>0.9726</v>
+        <v>0.8074</v>
       </c>
       <c r="I7" t="n">
-        <v>0.306</v>
+        <v>0.173</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>0.032</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DL-71efe679f350333810130f285a628d0b</t>
+          <t>DL-ccc15128eb3abd5f12b5083c5890631b</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 Improves Pokémon Karmesin and Purple with Graphics and Frame Rate Update</t>
+          <t>Nintendo Switch 2 Welcome Tour - Unique console launch experience</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.playcentral.de/nintendo-switch-2-verbessert-pokemon-karmesin-und-purpur-mit-grafik-und-bildraten-update/</t>
+          <t>https://www.playcentral.de/nintendo-switch-2-welcome-tour-einzigartiges-spielerlebnis-zur-einfuehrung-der-konsole/</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Version 4.0.0, released on June 2, 2025, brings several improvements when the game is played on the Nintendo Switch 2. This means that as soon as Switch 2 is available, players can download the update and enjoy everything it has to offer. These improvements could eliminate some of the biggest criticisms of Pokémon Karmesin and Purple.</t>
+          <t>Nintendo is known for its unusual and charming games that stand out from the competition. The Nintendo Switch 2 Welcome Tour is designed as an introduction to the new system. It shows both great new features like mouse support as well as obvious inclusions like the HD Rumble. From an educational perspective, it is fascinating to see what design decisions are behind the console.</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>46.007133</v>
+        <v>65.02605</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-06-03T15:01:19</t>
+          <t>2025-06-03T22:22:32</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['The release of the Nintendo Switch 2 is near, and with it come significant improvements for the popular games Pokémon Karmesin and Purple. These titles from 2022 will experience improved graphics and frame rate thanks to the new console.', 'Although the Nintendo Switch 2 will only be available on June 5, 2025, the major update for these games has already been released and upgrades them to version 4.0.0.', 'The graphics have been optimized for the display of the Nintendo Switch 2 and high-resolution televisions, resulting in improved image quality. In addition, the frame rate has been improved so that the games run more smoothly.']</t>
+          <t>["The price of the Nintendo Switch 2 Welcome Tour is hotly debated. With only 9.99 euros to start, the game is relatively cheap. However, some fans argue that it should have been offered as an add-on, similar to Astro's Playroom on the PS5.", 'Interactive experiences and challenges What interactive elements does the game offer? The content of the game is a mixture of quizzes, mini-games and technical demos.']</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>0.8074</v>
+        <v>0.9726</v>
       </c>
       <c r="I8" t="n">
-        <v>0.173</v>
+        <v>0.306</v>
       </c>
       <c r="J8" t="n">
-        <v>0.032</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DL-b4835f4fe1a96ea2d9f3e5a83449cefc</t>
+          <t>DL-5d2f13b7c79bab32f93ef41a84b5e6de</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>I've already tried the'mouse' mode on Nintendo Switch 2, it opens a door that has so far been closed on consoles.</t>
+          <t>Pokémon Scarlet &amp; Violet runs at 4K and 60 FPS on Switch 2 after patching.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.xataka.com/videojuegos/he-probado-modo-raton-nintendo-switch-2-abre-puerta-ahora-cerrada-consolas</t>
+          <t>https://www.adrenaline.com.br/games/pokemon-scarlet-violet-roda-a-4k-e-60-fps-no-switch-2-apos-patch/</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 is not a machine to experiment with. The 152 million Switches sold are a reflection that the company has achieved a product that people have liked. They don't need something as disruptive as Switch or Wii in their day, but a continuous console. And apart from the size, a change comes with the optical technology.</t>
+          <t>Pokémon Scarlet &amp; Violet has been plagued by severe performance issues. Nintendo Switch 2 will be able to deliver all of the potential that it's been rated for in 2022.</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>25.759068</v>
+        <v>34.473312</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-06-05T16:15:49</t>
+          <t>2025-06-03T11:54:48+00:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['Turning to the Joy-Con Nintendo Switch 2 is not a machine to experiment with. The 152 million Switches sold, and rising, are a reflection that the company has achieved a product that people have liked.']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>0.0644</v>
+        <v>-0.3818</v>
       </c>
       <c r="I9" t="n">
-        <v>0.036</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.031</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DL-4b86e968a9b1646ef4716b8b7c26d9ad</t>
+          <t>DL-fa269e8a0e19a32b2bf0f8ce731d82b1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Starting shot for Nintendo Switch 2 – German streamer is already playing Mario Kart World</t>
+          <t>Mario Kart World on Metacritic: First test scores are live and an absolute dream!</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.giga.de/games/startschuss-fuer-nintendo-switch-2-deutsche-streamerin-zockt-schon-mario-kart-world--01JWXN645JPPJSCMF79ZYQ7SQH</t>
+          <t>https://www.gamepro.de/artikel/mario-kart-world-metacritic-erste-tests-wertung,3434246.html</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: Day-One Patch is here The first gamers already have their Switch 2 at home. Version 20.1.1 is live and there are first experiences with the new hybrid console. Nintendo didn't miss a day, it's already June 5th in New Zealand.</t>
+          <t>Nintendo Switch 2 is here and we're shooting our first 37 minutes in Mario Kart World Autoplay What's being praised? Nintenduo gives it a score of 92 and writes: "Everything can still change" Nintendo has perfectly balanced classic and modern elements to create an engaging and accessible experience that will delight both veterans and newcomers.</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>24.691805</v>
+        <v>31.769712</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-06-04T14:23:08+00:00</t>
+          <t>2025-06-06T10:14:00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>['Nintendo Switch 2: Day-One Patch is here The first gamers already have their Switch 2 at home. Until now, the console was completely useless – a day-one patch from Nintendo was missing. That has now changed.', 'The German streamer LostKittn has not only got her Switch 2, she is even now playing Mario Kart World on Twitch. According to the pinned message of a chat moderator, she has received the console from Nintendo and is allowed to play since 2 pm.', 'Players showcase Switch 2 eShop Other players also share their experiences with Switch 2. On Reddit, users show GabSam, for example, the new and improved Nintendo eShop. It now runs much more smoothly than the one on the old console.']</t>
+          <t>["The first ratings for Mario Kart World are enthusiastic. No Nintendo Switch 2 consoles and review samples were sent in advance, we received Nintendo's newest flagship on release day.", "37:48 The Nintendo Switch 2 is here and we're shooting our first 37 minutes in Mario Kart World Autoplay What's being praised?", 'This means: Mario Kart World is the latest and perhaps best part of the long-standing arcade racing series and is taken to the next level with the hardware of Nintendo Switch 2 and an extensive roster of drivers, tracks and endless fun.']</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>-0.1531</v>
+        <v>0.9413</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>0.252</v>
       </c>
       <c r="J10" t="n">
-        <v>0.039</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DL-fa269e8a0e19a32b2bf0f8ce731d82b1</t>
+          <t>DL-c561b4eb3764195a1fd4e2ea1b9e581b</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mario Kart World on Metacritic: First test scores are live and an absolute dream!</t>
+          <t>Free update to Pokémon Scarlet and Violet for Nintendo Switch 2</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.gamepro.de/artikel/mario-kart-world-metacritic-erste-tests-wertung,3434246.html</t>
+          <t>https://thatsgaming.nl/gratis-update-pokemon-scarlet-en-violet-voor-nintendo-switch-2/</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 is here and we're shooting our first 37 minutes in Mario Kart World Autoplay What's being praised? Nintenduo gives it a score of 92 and writes: "Everything can still change" Nintendo has perfectly balanced classic and modern elements to create an engaging and accessible experience that will delight both veterans and newcomers.</t>
+          <t>Pokémon Scarlet and Pokémon Violet are available for the Nintendo Switch 2. This update makes the adventures in the Paldea region even more exciting. Improved image quality allows fans to recharge their batteries.</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>21.261477</v>
+        <v>30.33068</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-06-06T10:14:00</t>
+          <t>2025-06-05T09:38:52+00:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>["The first ratings for Mario Kart World are enthusiastic. No Nintendo Switch 2 consoles and review samples were sent in advance, we received Nintendo's newest flagship on release day.", "37:48 The Nintendo Switch 2 is here and we're shooting our first 37 minutes in Mario Kart World Autoplay What's being praised?", 'This means: Mario Kart World is the latest and perhaps best part of the long-standing arcade racing series and is taken to the next level with the hardware of Nintendo Switch 2 and an extensive roster of drivers, tracks and endless fun.']</t>
+          <t>["A sharper image quality: the optimizations for both the Nintendo Switch 2's screen and HD televisions provide even better image quality. A higher frame rate: the improved frame rates of the Nintendo Switch 2 allow for more fluid motion.", 'An immersive Paldea: on the Nintendo Switch 2, the already bustling Paldea region comes to life in an unprecedented way, whether players explore the open world, fight Pokémon or complete the Pokédex.', "Trainers who have a Nintendo Switch 2 and Pokémon Scarlet or Pokémon Violet can now experience the games even more intensely and beautifully. And it's completely free. 0 comments 0"]</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>0.9413</v>
+        <v>0.8508</v>
       </c>
       <c r="I11" t="n">
-        <v>0.252</v>
+        <v>0.23</v>
       </c>
       <c r="J11" t="n">
         <v>0</v>
@@ -926,306 +926,306 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DL-5d2f13b7c79bab32f93ef41a84b5e6de</t>
+          <t>DL-cb75051a141fa6e7e2afc84e6953afba</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Pokémon Scarlet &amp; Violet runs at 4K and 60 FPS on Switch 2 after patching.</t>
+          <t>IGN goes hands on with Mario Kart World for 5 hours</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.adrenaline.com.br/games/pokemon-scarlet-violet-roda-a-4k-e-60-fps-no-switch-2-apos-patch/</t>
+          <t>https://mynintendonews.com/2025/06/03/ign-goes-hands-on-with-mario-kart-world-for-5-hours/</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Pokémon Scarlet &amp; Violet has been plagued by severe performance issues. Nintendo Switch 2 will be able to deliver all of the potential that it's been rated for in 2022.</t>
+          <t>IGN recently attended a hands-on session with Mario Kart World. They have come away suitably impressed by the track designs, the Knockout Tour and the game’s all-important handling.</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>19.36528</v>
+        <v>27.381319</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-06-03T11:54:48+00:00</t>
+          <t>2025-06-03T16:37:43+00:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['We all know that media and influencers won’t be providing pre-launch reviews for the Nintendo Switch 2 hardware and software and you can expect our own reviews some time after launch.']</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>-0.3818</v>
+        <v>0.5994</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>0.154</v>
       </c>
       <c r="J12" t="n">
-        <v>0.08799999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DL-c561b4eb3764195a1fd4e2ea1b9e581b</t>
+          <t>DL-b4835f4fe1a96ea2d9f3e5a83449cefc</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Free update to Pokémon Scarlet and Violet for Nintendo Switch 2</t>
+          <t>I've already tried the'mouse' mode on Nintendo Switch 2, it opens a door that has so far been closed on consoles.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://thatsgaming.nl/gratis-update-pokemon-scarlet-en-violet-voor-nintendo-switch-2/</t>
+          <t>https://www.xataka.com/videojuegos/he-probado-modo-raton-nintendo-switch-2-abre-puerta-ahora-cerrada-consolas</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Pokémon Scarlet and Pokémon Violet are available for the Nintendo Switch 2. This update makes the adventures in the Paldea region even more exciting. Improved image quality allows fans to recharge their batteries.</t>
+          <t>Nintendo Switch 2 is not a machine to experiment with. The 152 million Switches sold are a reflection that the company has achieved a product that people have liked. They don't need something as disruptive as Switch or Wii in their day, but a continuous console. And apart from the size, a change comes with the optical technology.</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>16.283268</v>
+        <v>25.756937</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-06-05T09:38:52+00:00</t>
+          <t>2025-06-05T16:15:49</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>["A sharper image quality: the optimizations for both the Nintendo Switch 2's screen and HD televisions provide even better image quality. A higher frame rate: the improved frame rates of the Nintendo Switch 2 allow for more fluid motion.", 'An immersive Paldea: on the Nintendo Switch 2, the already bustling Paldea region comes to life in an unprecedented way, whether players explore the open world, fight Pokémon or complete the Pokédex.', "Trainers who have a Nintendo Switch 2 and Pokémon Scarlet or Pokémon Violet can now experience the games even more intensely and beautifully. And it's completely free. 0 comments 0"]</t>
+          <t>['Turning to the Joy-Con Nintendo Switch 2 is not a machine to experiment with. The 152 million Switches sold, and rising, are a reflection that the company has achieved a product that people have liked.']</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>0.8508</v>
+        <v>0.0644</v>
       </c>
       <c r="I13" t="n">
-        <v>0.23</v>
+        <v>0.036</v>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>DL-05650dfb79bd8bf7ef997bb2ce2f3cd3</t>
+          <t>DL-4b86e968a9b1646ef4716b8b7c26d9ad</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 First Impressions And A Surprising Purchasing Score</t>
+          <t>Starting shot for Nintendo Switch 2 – German streamer is already playing Mario Kart World</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://hothardware.com/news/nintendo-switch-2-first-impressions-and-a-surprising-purchasing</t>
+          <t>https://www.giga.de/games/startschuss-fuer-nintendo-switch-2-deutsche-streamerin-zockt-schon-mario-kart-world--01JWXN645JPPJSCMF79ZYQ7SQH</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 is finally out, and I have some first impressions on the experience of both playing and purchasing the console. I was not lucky enough to secure a preorder ahead of the console's June 5th release. Third-party entrepreneurs were already listing the console for a premium over its $449 MSRP. My local Walmart was nearly empty and upon inquiring, I was told it had around six to eight consoles still available in the back.</t>
+          <t>Nintendo Switch 2: Day-One Patch is here The first gamers already have their Switch 2 at home. Version 20.1.1 is live and there are first experiences with the new hybrid console. Nintendo didn't miss a day, it's already June 5th in New Zealand.</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>12.020853</v>
+        <v>24.692564</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-06-06T14:31:00+00:00</t>
+          <t>2025-06-04T14:23:08+00:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['The Nintendo Switch 2 is finally out, and I have some first impressions on the experience of both playing and purchasing the console.']</t>
+          <t>['Nintendo Switch 2: Day-One Patch is here The first gamers already have their Switch 2 at home. Until now, the console was completely useless – a day-one patch from Nintendo was missing. That has now changed.', 'The German streamer LostKittn has not only got her Switch 2, she is even now playing Mario Kart World on Twitch. According to the pinned message of a chat moderator, she has received the console from Nintendo and is allowed to play since 2 pm.', 'Players showcase Switch 2 eShop Other players also share their experiences with Switch 2. On Reddit, users show GabSam, for example, the new and improved Nintendo eShop. It now runs much more smoothly than the one on the old console.']</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>0.5673</v>
+        <v>-0.1531</v>
       </c>
       <c r="I14" t="n">
-        <v>0.114</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0.054</v>
+        <v>0.039</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DL-cb75051a141fa6e7e2afc84e6953afba</t>
+          <t>DL-ec8624ffe681d5f29d095a287c5219aa</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>IGN goes hands on with Mario Kart World for 5 hours</t>
+          <t>The lack of day one Switch 2 reviews isn't as problematic as it sounds</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://mynintendonews.com/2025/06/03/ign-goes-hands-on-with-mario-kart-world-for-5-hours/</t>
+          <t>https://www.xda-developers.com/thread/the-lack-of-day-one-switch-2-reviews-isnt-as-problematic-as-it-sounds/</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>IGN recently attended a hands-on session with Mario Kart World. They have come away suitably impressed by the track designs, the Knockout Tour and the game’s all-important handling.</t>
+          <t>Nintendo has been making a lot of little weird decisions with the Switch 2. Switch 2 pre-orders were flying off the shelves in the US, and the extra stock available at launch is probably going to be swooped up by die hard fans. Is it still a bad look for Nintendo to break tradition like this?</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>11.56027</v>
+        <v>19.407114</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-06-03T16:37:43+00:00</t>
+          <t>2025-06-03T22:01:23+00:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>['We all know that media and influencers won’t be providing pre-launch reviews for the Nintendo Switch 2 hardware and software and you can expect our own reviews some time after launch.']</t>
+          <t>["And now, that's happening again, as outlets have confirmed they won't be publishing reviews of the Switch 2 on release day due to Nintendo not providing review units this time around.\nBut in reality, how much does it matter?", 'Switch 2 pre-orders were flying off the shelves in the US, and the extra stock available at launch is probably going to be swooped up by die hard fans.']</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>0.5994</v>
+        <v>-0.7722</v>
       </c>
       <c r="I15" t="n">
-        <v>0.154</v>
+        <v>0.041</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>0.168</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DL-2fa26bf724852abc5c72c9f822028c52</t>
+          <t>DL-daa7370e17bbf6699977f90dd9dcc32e</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Zelda: The underrated game that deserves a remake for Switch 2</t>
+          <t>Nintendo Switch 2: New game console officially launches today</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.zazoom.it/2025-06-07/zelda-il-gioco-sottovalutato-che-merita-un-remake-per-switch-2/17144781/</t>
+          <t>https://www.appgefahren.de/nintendo-switch-2-neue-spielkonsole-geht-heute-offiziell-an-den-start-380403.html</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Nintendo would have the opportunity to strengthen the connection between the past and the future, providing an unforgettable experience. With the advent of the new console, the challenge for Nintendo will be to continue to innovate and deliver experiences that meet the expectations of the passionate. The Legend of Zelda: Tears of the Kingdom game shows up on Nintendo Switch 2 with 20 minutes of gameplay.</t>
+          <t>Nintendo officially unveiled the new generation of the popular Switch game console, the Nintendo Switch 2. The new model, equipped with a 7.9′′ screen and support for 4K content, is now available on the market. At the same thickness, the console features a significantly larger 7.9-inch LCD screen, 1080p resolution, HDR support, and frame rates of up to 120 fps. If the Switch 2 is connected to a TV via the also updated dock. For 4K playback, the frame</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>11.422516</v>
+        <v>15.065126</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-06-07T18:16:28</t>
+          <t>2025-06-05T12:38:11+00:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['But what can the new Nintendo Switch 2 do? Compared to its predecessor, the Nintendo Switch (OLED), the Switch 2 has done quite a bit.', 'At the same thickness, the console features a significantly larger 7.9-inch LCD screen, 1080p resolution, HDR support, and frame rates of up to 120 fps.']</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>0.8779</v>
+        <v>0.802</v>
       </c>
       <c r="I16" t="n">
-        <v>0.178</v>
+        <v>0.111</v>
       </c>
       <c r="J16" t="n">
-        <v>0.026</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DL-c9dfbd021d961275503a96f92b6c77b0</t>
+          <t>DL-cce7387fccad72acd7b577de07a1a6e3</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: Better Performance for Pokémon</t>
+          <t>Nintendo Switch 2 unboxing: What do you get with the console?</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://www.4p.de/news/pokemon-endlich-fluessig-riesiges-update-fuer-nintendo-switch-2-bringt-das-was-fans-sich-immer-wuenschten/3325530</t>
+          <t>https://www.indy100.com/gaming/nintendo-switch-2-unboxing-console-2672317405</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Pokémon on the Nintendo Switch 2: Better Performance and Textures Like in Nintendo Today! -App announced and immediately proved thanks to an enclosed video, the current generation of pocket monsters on the Switch 2 will now finally run in 60 FPS. The resolution has also been noticeably screwed up, so that Karmesin &amp; Purpur look much nicer on the console that will be released on June 5.</t>
+          <t>Nintendo has sent review units out to media outlets for them to check out the new console and games running on it. The first thing that will be seen when unboxing are the two new Joy-Con controllers and main part of the console with the bigger screen. Below that on the next layer down is a brief user manual, a HDMI cable to connect the dock to a TV and the wrist strap accessories that connect to the Switch 2.</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>11.269152</v>
+        <v>14.932243</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-06-03T15:43:17</t>
+          <t>2025-06-05T15:19:37</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>['Recommended reading: All information about Pokémon Legends: Z-A Since the update is already there, you can start directly to the release of the Nintendo Switch 2 and experience Pokémon Karmesin &amp; Purpur as it should have been at the time of the release']</t>
+          <t>['Nintendo has sent Switch 2 review units out to media outlets for them to check out the new console and games running on it.\nindy100 is very fortunate to have been sent one of these units and this is what comes in the box - read our first impressions of']</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>0.7906</v>
+        <v>0.5859</v>
       </c>
       <c r="I17" t="n">
-        <v>0.155</v>
+        <v>0.048</v>
       </c>
       <c r="J17" t="n">
-        <v>0.044</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DL-cce7387fccad72acd7b577de07a1a6e3</t>
+          <t>DL-64e742892b89791778db24a855e573ee</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 unboxing: What do you get with the console?</t>
+          <t>Nintendo "Switch 2, using the included HDMI cable" Lack of performance in the first-generation accessory</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://www.indy100.com/gaming/nintendo-switch-2-unboxing-console-2672317405</t>
+          <t>https://ascii.jp/elem/000/004/280/4280590/</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Nintendo has sent review units out to media outlets for them to check out the new console and games running on it. The first thing that will be seen when unboxing are the two new Joy-Con controllers and main part of the console with the bigger screen. Below that on the next layer down is a brief user manual, a HDMI cable to connect the dock to a TV and the wrist strap accessories that connect to the Switch 2.</t>
+          <t>Nintendo announced on Support Official X (Twitter) that they would be using the included "Ultra High Speed HDMI Cable" When connecting Nintendo Switch 2 to a TV, use the included Ultra Highspeed HDMI cable. The most important difference is the transmission speed. It is the standard evolved from those included with the original Switch.</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>9.852928</v>
+        <v>14.281282</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-06-05T15:19:37</t>
+          <t>2025-06-10T00:00:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>['Nintendo has sent Switch 2 review units out to media outlets for them to check out the new console and games running on it.\nindy100 is very fortunate to have been sent one of these units and this is what comes in the box - read our first impressions of']</t>
+          <t>['There are more than four times as many differences in numerical values, and this number must be higher in order to enjoy high-quality, high-frame rate games. The Nintendo Switch 2 is a video game console that supports up to 4K/60 fps in TV mode.']</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>0.5859</v>
+        <v>0.7264</v>
       </c>
       <c r="I18" t="n">
-        <v>0.048</v>
+        <v>0.129</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
@@ -1234,86 +1234,86 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DL-ec8624ffe681d5f29d095a287c5219aa</t>
+          <t>DL-0aac9eb3cc370dc0acf115375a664310</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>The lack of day one Switch 2 reviews isn't as problematic as it sounds</t>
+          <t>Nintendo Switch 2 launch day build-up live: all the latest news, updates, and our thoughts ahead of the console's release</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://www.xda-developers.com/thread/the-lack-of-day-one-switch-2-reviews-isnt-as-problematic-as-it-sounds/</t>
+          <t>https://www.techradar.com/news/live/nintendo-switch-2-launch-day-build-up-review-in-progress-live</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Nintendo has been making a lot of little weird decisions with the Switch 2. Switch 2 pre-orders were flying off the shelves in the US, and the extra stock available at launch is probably going to be swooped up by die hard fans. Is it still a bad look for Nintendo to break tradition like this?</t>
+          <t>TechRadar Gaming has been covering huge console and game launches for years - everything from reviews of Nintendo, PlayStation, and Xbox systems to key live events like Nintendo Direct and Summer Game Fest presentations. Here's a quick glance at all the Nintendo Switch 2 launch games you can expect to purchase and play on June 5.</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>9.773457000000001</v>
+        <v>13.722183</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-06-03T22:01:23+00:00</t>
+          <t>2025-06-04T12:00:34</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>["And now, that's happening again, as outlets have confirmed they won't be publishing reviews of the Switch 2 on release day due to Nintendo not providing review units this time around.\nBut in reality, how much does it matter?", 'Switch 2 pre-orders were flying off the shelves in the US, and the extra stock available at launch is probably going to be swooped up by die hard fans.']</t>
+          <t>['Like a kid on Christmas Eve, this final day before the Nintendo Switch 2 launch may feel as long as the time between now and its official announcement way back in January. But that’s why we’re here.', 'At TechRadar Gaming, we’ve been covering huge console and game launches for years - everything from reviews of Nintendo, PlayStation, and Xbox systems to key live events like Nintendo Direct and Summer Game Fest presentations.']</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>-0.7722</v>
+        <v>0.7351</v>
       </c>
       <c r="I19" t="n">
-        <v>0.041</v>
+        <v>0.128</v>
       </c>
       <c r="J19" t="n">
-        <v>0.168</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DL-8d8caf04d65da8ebac6136b7cec59a11</t>
+          <t>DL-d8592a0cf2cffdc39ad7fabcf4457939</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 Unboxing, Setup &amp; What You Need to Know</t>
+          <t>It's already available to buy in stores for the new Nintendo Switch 2.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://www.geeky-gadgets.com/nintendo-switch-2-4/</t>
+          <t>https://portugalgamers.pt/ja-esta-disponivel-para-compra-nas-lojas-a-nova-nintendo-switch-2/</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>This guide explores the unboxing experience, setup process, design changes, hardware advancements, and new features, while also comparing it to the original Nintendo Switch. The packaging is compact and eco-friendly, underscoring Nintendo’s commitment to reducing environmental impact. Inside the box, you’ll find: The Nintendo Switch 2 console Two redesigned Joy-Con controllers A revamped dock featuring an Ethernet port An HDMI cable A power adapter.</t>
+          <t>The Nintendo Switch 2 is out in the shops today. Add your favorite titles to a screen larger than 1080p. Compatible with high dynamic range and update rate up to 120 fps. Match the new Joy-Con 2 commands on the console with the magnetic dials. Each command can be used as a mouse.</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>8.218931</v>
+        <v>12.77504</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-06-08T13:00:24</t>
+          <t>2025-06-05T16:28:29+00:00</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>['The video below from Zollotech gives us a detailed look at the new Switch console.\nUnboxing: What’s Inside the Box?\nThe unboxing experience of the Nintendo Switch 2 reflects a focus on simplicity and sustainability.', 'Setting Up: From Box to Gameplay\nSetting up the Nintendo Switch 2 is a straightforward process designed to get you gaming quickly.', 'New Features: Enhancing the Experience\nThe Nintendo Switch 2 introduces several new features that enhance the overall user experience and cater to modern gaming needs:\nOnline Functionality: Faster download speeds and a more stable connection improve multiplayer']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>0.8979</v>
+        <v>0.8555</v>
       </c>
       <c r="I20" t="n">
-        <v>0.166</v>
+        <v>0.173</v>
       </c>
       <c r="J20" t="n">
         <v>0</v>
@@ -1322,174 +1322,174 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>DL-f955c260113cb461bc83d07b7ef513dd</t>
+          <t>DL-05650dfb79bd8bf7ef997bb2ce2f3cd3</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 Comes With a Below-Average Display and Disappointing HDR Support, New In-Depth Analysis Reveals</t>
+          <t>Nintendo Switch 2 First Impressions And A Surprising Purchasing Score</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://wccftech.com/nintendo-switch-2-below-average-hdr/</t>
+          <t>https://hothardware.com/news/nintendo-switch-2-first-impressions-and-a-surprising-purchasing</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>The new analysis by GamingTech takes a good look at the new Nintendo system's display. Measuring the brightness in Zelda: Breath of the Wild returned a maximum value of 420 nits, but in Cyberpunk 2077, it is locked to 450 nit, likely the maximum peak brightness the display is capable of. This peak brightness is not even close to providing a proper HDR experience.</t>
+          <t>Nintendo Switch 2 is finally out, and I have some first impressions on the experience of both playing and purchasing the console. I was not lucky enough to secure a preorder ahead of the console's June 5th release. Third-party entrepreneurs were already listing the console for a premium over its $449 MSRP. My local Walmart was nearly empty and upon inquiring, I was told it had around six to eight consoles still available in the back.</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>7.700903</v>
+        <v>12.0216465</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-06-05T11:37:00+00:00</t>
+          <t>2025-06-06T14:31:00+00:00</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>["Related Story Level Up Your Switch 2 Experience With Mumba’s Blade Series, Clear Series Dockable Cases, and Carrying Case\nThe Nintendo Switch 2's HDR support in docked mode fares a little better.", 'The system-level calibration is found to be adequate, and in games like Cyberpunk 2077, the system delivers an HDR experience on par with that of the other versions of the game.', 'In other games like Zelda: Breath of the Wild, the HDR experience is rather disappointing, as the game looks washed out due to its aesthetics and the lack of contrast.\nThe Nintendo Switch 2 launches today worldwide.']</t>
+          <t>['The Nintendo Switch 2 is finally out, and I have some first impressions on the experience of both playing and purchasing the console.']</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>0.928</v>
+        <v>0.5673</v>
       </c>
       <c r="I21" t="n">
-        <v>0.231</v>
+        <v>0.114</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>0.054</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>DL-daa7370e17bbf6699977f90dd9dcc32e</t>
+          <t>DL-2fa26bf724852abc5c72c9f822028c52</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: New game console officially launches today</t>
+          <t>Zelda: The underrated game that deserves a remake for Switch 2</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://www.appgefahren.de/nintendo-switch-2-neue-spielkonsole-geht-heute-offiziell-an-den-start-380403.html</t>
+          <t>https://www.zazoom.it/2025-06-07/zelda-il-gioco-sottovalutato-che-merita-un-remake-per-switch-2/17144781/</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Nintendo officially unveiled the new generation of the popular Switch game console, the Nintendo Switch 2. The new model, equipped with a 7.9′′ screen and support for 4K content, is now available on the market. At the same thickness, the console features a significantly larger 7.9-inch LCD screen, 1080p resolution, HDR support, and frame rates of up to 120 fps. If the Switch 2 is connected to a TV via the also updated dock. For 4K playback, the frame</t>
+          <t>Nintendo would have the opportunity to strengthen the connection between the past and the future, providing an unforgettable experience. With the advent of the new console, the challenge for Nintendo will be to continue to innovate and deliver experiences that meet the expectations of the passionate. The Legend of Zelda: Tears of the Kingdom game shows up on Nintendo Switch 2 with 20 minutes of gameplay.</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>7.6617393</v>
+        <v>11.423676</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-06-05T12:38:11+00:00</t>
+          <t>2025-06-07T18:16:28</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>['But what can the new Nintendo Switch 2 do? Compared to its predecessor, the Nintendo Switch (OLED), the Switch 2 has done quite a bit.', 'At the same thickness, the console features a significantly larger 7.9-inch LCD screen, 1080p resolution, HDR support, and frame rates of up to 120 fps.']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>0.802</v>
+        <v>0.8779</v>
       </c>
       <c r="I22" t="n">
-        <v>0.111</v>
+        <v>0.178</v>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>DL-3b9c455fdfdecda911fc03f986c53590</t>
+          <t>DL-c9dfbd021d961275503a96f92b6c77b0</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Split Fiction is already available for the Nintendo Switch 2.</t>
+          <t>Nintendo Switch 2: Better Performance for Pokémon</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://portugalgamers.pt/split-fiction-ja-esta-disponivel-para-a-nintendo-switch-2/</t>
+          <t>https://www.4p.de/news/pokemon-endlich-fluessig-riesiges-update-fuer-nintendo-switch-2-bringt-das-was-fans-sich-immer-wuenschten/3325530</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Split Fiction is already available for the Nintendo Switch 2, PlayStation 5, Xbox Series X|S and PC through Steam, Epic Games Store and the EA app, starting at $49.99. GameShare will allow Nintendo Switch 2 owners to invite another player for a local wireless connection with just a copy of the video game. With exclusive Friend Pass functionality from Hazelight Studios, players can invite an online friend to play.</t>
+          <t>Pokémon on the Nintendo Switch 2: Better Performance and Textures Like in Nintendo Today! -App announced and immediately proved thanks to an enclosed video, the current generation of pocket monsters on the Switch 2 will now finally run in 60 FPS. The resolution has also been noticeably screwed up, so that Karmesin &amp; Purpur look much nicer on the console that will be released on June 5.</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>7.1621685</v>
+        <v>11.268633</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-06-06T07:58:52+00:00</t>
+          <t>2025-06-03T15:43:17</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>["The wait's over — the explosive cooperative adventure by Hazelight Studios and EA, Split Fiction, is already available for the Nintendo Switch 2 as a release title for $49.99!", 'On the newly launched Nintendo Switch 2, players can now experience one of the best-rated video games of 2025 wherever they are and connect with fellow gamers in a collaborative way through GameShare and GameChat to dive on an unforgettable and challenging', 'GameShare will allow Nintendo Switch 2 owners to invite another player for a local wireless connection with just a copy of the video game, even for original Nintendo Switch users.']</t>
+          <t>['Recommended reading: All information about Pokémon Legends: Z-A Since the update is already there, you can start directly to the release of the Nintendo Switch 2 and experience Pokémon Karmesin &amp; Purpur as it should have been at the time of the release']</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>0.9081</v>
+        <v>0.7906</v>
       </c>
       <c r="I23" t="n">
-        <v>0.219</v>
+        <v>0.155</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>DL-d8592a0cf2cffdc39ad7fabcf4457939</t>
+          <t>DL-7fdb288e26fb545394f161b0835d8979</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>It's already available to buy in stores for the new Nintendo Switch 2.</t>
+          <t>Nintendo Switch 2 with Mario Kart World : Here’s how to make it cheaper with the return of your old Switch!</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://portugalgamers.pt/ja-esta-disponivel-para-compra-nas-lojas-a-nova-nintendo-switch-2/</t>
+          <t>https://www.phonandroid.com/nintendo-switch-2-avec-mario-kart-world-voici-comment-lavoir-moins-chere-avec-la-reprise-de-votre-ancienne-switch.html</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 is out in the shops today. Add your favorite titles to a screen larger than 1080p. Compatible with high dynamic range and update rate up to 120 fps. Match the new Joy-Con 2 commands on the console with the magnetic dials. Each command can be used as a mouse.</t>
+          <t>Switch 2 + Mario Kart World is available at Darty at €499.99. You can save up to €133.20 by recycling your old Switch. The Switch 2 is a new pillar of the franchise. It introduces an open world linking all circuits and 24-player races.</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>6.864105</v>
+        <v>9.114084</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-06-05T16:28:29+00:00</t>
+          <t>2025-06-07T05:00:34+00:00</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['A thoroughly reviewed console and an unprecedented Mario Kart The Nintendo Switch 2 marks a real evolution from the original model.', 'It comes with a 7.9-inch 1080p LCD screen, a refresh rate raised to 120 Hz for increased fluidity, and 256GB of internal memory, which can be expanded via a Micro SD Express card (not compatible with older Micro SD cards).']</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>0.8555</v>
+        <v>0.4939</v>
       </c>
       <c r="I24" t="n">
-        <v>0.173</v>
+        <v>0.08</v>
       </c>
       <c r="J24" t="n">
         <v>0</v>
@@ -1498,42 +1498,42 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>DL-0aac9eb3cc370dc0acf115375a664310</t>
+          <t>DL-8d8caf04d65da8ebac6136b7cec59a11</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 launch day build-up live: all the latest news, updates, and our thoughts ahead of the console's release</t>
+          <t>Nintendo Switch 2 Unboxing, Setup &amp; What You Need to Know</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://www.techradar.com/news/live/nintendo-switch-2-launch-day-build-up-review-in-progress-live</t>
+          <t>https://www.geeky-gadgets.com/nintendo-switch-2-4/</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>TechRadar Gaming has been covering huge console and game launches for years - everything from reviews of Nintendo, PlayStation, and Xbox systems to key live events like Nintendo Direct and Summer Game Fest presentations. Here's a quick glance at all the Nintendo Switch 2 launch games you can expect to purchase and play on June 5.</t>
+          <t>This guide explores the unboxing experience, setup process, design changes, hardware advancements, and new features, while also comparing it to the original Nintendo Switch. The packaging is compact and eco-friendly, underscoring Nintendo’s commitment to reducing environmental impact. Inside the box, you’ll find: The Nintendo Switch 2 console Two redesigned Joy-Con controllers A revamped dock featuring an Ethernet port An HDMI cable A power adapter.</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>6.452999</v>
+        <v>8.219427</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-06-04T12:00:34</t>
+          <t>2025-06-08T13:00:24</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>['Like a kid on Christmas Eve, this final day before the Nintendo Switch 2 launch may feel as long as the time between now and its official announcement way back in January. But that’s why we’re here.', 'At TechRadar Gaming, we’ve been covering huge console and game launches for years - everything from reviews of Nintendo, PlayStation, and Xbox systems to key live events like Nintendo Direct and Summer Game Fest presentations.']</t>
+          <t>['The video below from Zollotech gives us a detailed look at the new Switch console.\nUnboxing: What’s Inside the Box?\nThe unboxing experience of the Nintendo Switch 2 reflects a focus on simplicity and sustainability.', 'Setting Up: From Box to Gameplay\nSetting up the Nintendo Switch 2 is a straightforward process designed to get you gaming quickly.', 'New Features: Enhancing the Experience\nThe Nintendo Switch 2 introduces several new features that enhance the overall user experience and cater to modern gaming needs:\nOnline Functionality: Faster download speeds and a more stable connection improve multiplayer']</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>0.7351</v>
+        <v>0.8979</v>
       </c>
       <c r="I25" t="n">
-        <v>0.128</v>
+        <v>0.166</v>
       </c>
       <c r="J25" t="n">
         <v>0</v>
@@ -1542,42 +1542,42 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>DL-ee2569beb5cd763340f09ccc36ad4f33</t>
+          <t>DL-f955c260113cb461bc83d07b7ef513dd</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Tamagotchi Plaza to be available on Nintendo Switch 2 with exclusive stores</t>
+          <t>Nintendo Switch 2 Comes With a Below-Average Display and Disappointing HDR Support, New In-Depth Analysis Reveals</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://www.gamesvillage.it/7205733/tamagotchi-plaza-sara-disponibile-su-nintendo-switch-2-con-negozi-esclusivi/</t>
+          <t>https://wccftech.com/nintendo-switch-2-below-average-hdr/</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 Edition gives players access to three exclusive stores. The new title in the TAMAGOTCHI CONNECTION: CORNER SHOP series is also coming on the Nintendo Switch. Each store offers a unique gameplay where players serve and attract customers, meeting over 100 different Tamagotchis and improving their reputation.</t>
+          <t>The new analysis by GamingTech takes a good look at the new Nintendo system's display. Measuring the brightness in Zelda: Breath of the Wild returned a maximum value of 420 nits, but in Cyberpunk 2077, it is locked to 450 nit, likely the maximum peak brightness the display is capable of. This peak brightness is not even close to providing a proper HDR experience.</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>5.8221245</v>
+        <v>7.701069</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-06-06T17:07:41+00:00</t>
+          <t>2025-06-05T11:37:00+00:00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>['Recommended Articles Nintendo Switch 2 players who already own the original Switch version of TAMGOTCHI PLAZA can access the exclusive content by purchasing the Tamagotchi Plaza update package for Nintendo Switch 2 and can access the exclusive content', 'during the switch to the Nintendo Switch 2 device.', 'TAMAGOTCHI PLAZA brings back the unique and engaging experience of setting up awesome stores and serving cute characters. The Great Gothic King declared that the Tamagotchi Fest would be held in the most exciting city on the planet Tamagotchi.']</t>
+          <t>["Related Story Level Up Your Switch 2 Experience With Mumba’s Blade Series, Clear Series Dockable Cases, and Carrying Case\nThe Nintendo Switch 2's HDR support in docked mode fares a little better.", 'The system-level calibration is found to be adequate, and in games like Cyberpunk 2077, the system delivers an HDR experience on par with that of the other versions of the game.', 'In other games like Zelda: Breath of the Wild, the HDR experience is rather disappointing, as the game looks washed out due to its aesthetics and the lack of contrast.\nThe Nintendo Switch 2 launches today worldwide.']</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>0.7003</v>
+        <v>0.928</v>
       </c>
       <c r="I26" t="n">
-        <v>0.137</v>
+        <v>0.231</v>
       </c>
       <c r="J26" t="n">
         <v>0</v>
@@ -1586,86 +1586,86 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>DL-c076e5bfb5dc9961cab30b68e0ec0dc1</t>
+          <t>DL-39e749ba8f4fabb28b4c41cfc788cbe9</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>TAMAGOTCHI PLAZA released for the Nintendo Switch 2</t>
+          <t>Nintendo Switch 2: everything you need to know about the new console</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://game2gether.de/2025/06/tamagotchi-plaza-erscheint-fuer-nintendo-switch-2/</t>
+          <t>https://www.publimetro.com.mx/plus/2025/06/05/nintendo-switch-2-todo-lo-que-debes-saber-de-la-nueva-consola/</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>TAMAGOTCHI PLAZA will be released on June 27 for the Nintendo Switch and Nintendo Switch 2. The players take over different shops in Tamahiko Town and can thus interact with over 100 different Tamagotchis. It is important to expand more than a dozen different stores and expand the reputation in the city.</t>
+          <t>Nintendo Switch 2 will cost 13,599 Mexican pesos in Mexico, with no games included. The price goes up to 14.899 in the case of the version with Mario Kart World Photo: Courtesy Nintendo of America The wait finally ended for millions of gamers as the new console officially arrived on June 5th.</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>5.511585</v>
+        <v>7.5558243</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-06-08T15:29:52</t>
+          <t>2025-06-05T03:09:27</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>['Learn More Unlock Content Accept Required Service and Unlock Content TAMAGOTCHI PLAZA Nintendo Switch 2 Edition extends the gaming experience with three new stores, bringing the total to 15.']</t>
+          <t>['Nintendo Switch 2 Photo: Courtesy of Nintendo of America It also has a rate of up to 120 fps on some titles, allowing a smoother gaming experience.', 'As for the portable mode, it has a Full HD resolution of 1920 x 1080 pixels and a refresh rate of 120 Hz.', 'The Nintendo Switch 2 can also be used in a semi-portable way thanks to the built-in support that allows you to tilt it up to 150 degrees to find the most comfortable position to play.']</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>0.6597</v>
+        <v>0.0772</v>
       </c>
       <c r="I27" t="n">
-        <v>0.125</v>
+        <v>0.048</v>
       </c>
       <c r="J27" t="n">
-        <v>0</v>
+        <v>0.043</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>DL-64e742892b89791778db24a855e573ee</t>
+          <t>DL-3b9c455fdfdecda911fc03f986c53590</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Nintendo "Switch 2, using the included HDMI cable" Lack of performance in the first-generation accessory</t>
+          <t>Split Fiction is already available for the Nintendo Switch 2.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://ascii.jp/elem/000/004/280/4280590/</t>
+          <t>https://portugalgamers.pt/split-fiction-ja-esta-disponivel-para-a-nintendo-switch-2/</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Nintendo announced on Support Official X (Twitter) that they would be using the included "Ultra High Speed HDMI Cable" When connecting Nintendo Switch 2 to a TV, use the included Ultra Highspeed HDMI cable. The most important difference is the transmission speed. It is the standard evolved from those included with the original Switch.</t>
+          <t>Split Fiction is already available for the Nintendo Switch 2, PlayStation 5, Xbox Series X|S and PC through Steam, Epic Games Store and the EA app, starting at $49.99. GameShare will allow Nintendo Switch 2 owners to invite another player for a local wireless connection with just a copy of the video game. With exclusive Friend Pass functionality from Hazelight Studios, players can invite an online friend to play.</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>4.806385</v>
+        <v>7.164835</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-06-10T00:00:00</t>
+          <t>2025-06-06T07:58:52+00:00</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>['There are more than four times as many differences in numerical values, and this number must be higher in order to enjoy high-quality, high-frame rate games. The Nintendo Switch 2 is a video game console that supports up to 4K/60 fps in TV mode.']</t>
+          <t>["The wait's over — the explosive cooperative adventure by Hazelight Studios and EA, Split Fiction, is already available for the Nintendo Switch 2 as a release title for $49.99!", 'On the newly launched Nintendo Switch 2, players can now experience one of the best-rated video games of 2025 wherever they are and connect with fellow gamers in a collaborative way through GameShare and GameChat to dive on an unforgettable and challenging', 'GameShare will allow Nintendo Switch 2 owners to invite another player for a local wireless connection with just a copy of the video game, even for original Nintendo Switch users.']</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>0.7264</v>
+        <v>0.9081</v>
       </c>
       <c r="I28" t="n">
-        <v>0.129</v>
+        <v>0.219</v>
       </c>
       <c r="J28" t="n">
         <v>0</v>
@@ -1674,42 +1674,42 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>DL-e8fdaa27ea9510e7798fabc955bb2d44</t>
+          <t>DL-2e469f3f8789d2c101197abc3c31aac9</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 eShop is super fast.</t>
+          <t>Mario Kart World review – the final verdict on the Switch 2’s biggest game</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://nintendon.it/2025/06/05/leshop-di-nintendo-switch-2-e-velocissimo-312800</t>
+          <t>https://metro.co.uk/2025/06/10/mario-kart-world-review-final-verdict-switch-2s-biggest-game-23373706/</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>the eShop on the Nintendo Switch 2 is much more responsive and responsive. Even loading the game preview through the simple tab on the main screen is significantly faster. We can only imagine that, over the next few years, this will only get better.</t>
+          <t>Mario Kart 8 Deluxe is one of the very few games we’ve ever given a 10/10 score. That’s not something we regret either, especially after the extremely generous Booster Course DLC. The idea of making the next game an open world title seemed an excellent new direction to take the series. It’s very poorly utilised, with lots of hidden secrets and yet nothing of substance to gain from them.</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>4.701643</v>
+        <v>5.9429245</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-06-05T07:01:52+00:00</t>
+          <t>2025-06-10T08:07:26+00:00</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>["If there's one part of the original Nintendo Switch that was really annoying, it was definitely the experience of using the eShop. But in the end, it came to a respectable conclusion.", 'It turns out that the eShop on the Nintendo Switch 2 is much more responsive and responsive, allowing you to enjoy the content much more smoothly, both with the classic Joycon 2 keyboards and in mouse mode.']</t>
+          <t>['Thanks to Nintendo not sending out review units of the Nintendo Switch 2 more than a day before launch we’ve previously only been able to do a review in progress of World, during which it became clear that it is not quite the game that many imagined.']</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>0.8169</v>
+        <v>0.919</v>
       </c>
       <c r="I29" t="n">
-        <v>0.175</v>
+        <v>0.171</v>
       </c>
       <c r="J29" t="n">
         <v>0</v>
@@ -1718,42 +1718,42 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>DL-9ead5a4840a28021df89936d4039541b</t>
+          <t>DL-ee2569beb5cd763340f09ccc36ad4f33</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Switch 2 games load much slower from cartridges than a microSD Express card or internal storage</t>
+          <t>Tamagotchi Plaza to be available on Nintendo Switch 2 with exclusive stores</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://www.notebookcheck.net/Switch-2-games-load-much-slower-from-cartridges-than-a-microSD-Express-card-or-internal-storage.1032520.0.html</t>
+          <t>https://www.gamesvillage.it/7205733/tamagotchi-plaza-sara-disponibile-su-nintendo-switch-2-con-negozi-esclusivi/</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Switch 2 specs include internal 256GB UFS storage, which wins the checkered flag with a time of 16.60 seconds. SanDisk, Samsung, and Lexar microSD Express cards finish second between 19.18 and 19.78 seconds, and Game Card finishes in last place.</t>
+          <t>Nintendo Switch 2 Edition gives players access to three exclusive stores. The new title in the TAMAGOTCHI CONNECTION: CORNER SHOP series is also coming on the Nintendo Switch. Each store offers a unique gameplay where players serve and attract customers, meeting over 100 different Tamagotchis and improving their reputation.</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>4.325392</v>
+        <v>5.8248024</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-06-08T04:13:27+00:00</t>
+          <t>2025-06-06T17:07:41+00:00</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>['The number of ways to play or store Switch 2 games can confuse buyers. In addition to cartridges, internal storage, and microSD Express cards, gamers can experiment with Game-Key Cards.', "For Nintendo fans who prioritize speed, a new benchmark compares these different formats. It's no shock that the console's built-in flash storage ranks first. Still, the fact that Switch 2 cartridges are significantly slower may surprise gamers."]</t>
+          <t>['Recommended Articles Nintendo Switch 2 players who already own the original Switch version of TAMGOTCHI PLAZA can access the exclusive content by purchasing the Tamagotchi Plaza update package for Nintendo Switch 2 and can access the exclusive content', 'during the switch to the Nintendo Switch 2 device.', 'TAMAGOTCHI PLAZA brings back the unique and engaging experience of setting up awesome stores and serving cute characters. The Great Gothic King declared that the Tamagotchi Fest would be held in the most exciting city on the planet Tamagotchi.']</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>0.5719</v>
+        <v>0.7003</v>
       </c>
       <c r="I30" t="n">
-        <v>0.098</v>
+        <v>0.137</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
@@ -1762,170 +1762,174 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>DL-24b1842a456f3df8f5436bc5f2ff0e03</t>
+          <t>DL-be4b0877ab72d480615d2f3254053e13</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Your Nintendo Switch 2 Launch Kit: The Best Accessories</t>
+          <t>Moving my self-hosted empire to Proxmox was a breeze</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://www.techlicious.com/guide/nintendo-switch-2-accessories/</t>
+          <t>https://www.xda-developers.com/thread/moving-my/</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>The official Nintendo Switch 2 Pro Controller is one of the best that money can buy. From controllers to carry cases, cameras to microSD cards, there are plenty of ways to maximize your Switch 2 experience. This wireless controller offers responsive buttons, precise analog sticks, and ergonomic grips designed to keep your hands comfortable during extended play sessions. It also features built-in motion controls and HD rumble.</t>
+          <t>Nintendo has been making a lot of little weird decisions with the Switch 2. It's been a long wait for a new generation of consoles since the launch of the original hardware. Fans have speculated on a successor or major upgrade to the Switch.</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>4.281063</v>
+        <v>5.68388</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-06-05T00:00:00</t>
+          <t>2025-06-04T22:16:05+00:00</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>['From controllers to carry cases, cameras to microSD cards, there are plenty of ways to maximize your Switch 2 experience. So without further ado, here are the best Nintendo Switch 2 accessories currently (and shortly) available.', 'Best Controllers for a Premium Play Experience\nNintendo Switch 2 Pro Controller\nIf you’re planning on couch-playing with your Switch 2 in docked mode, a decent controller is an absolute must-have, and the official Nintendo Switch 2 Pro Controller is one']</t>
+          <t>["And now, that's happening again, as outlets have confirmed they won't be publishing reviews of the Switch 2 on release day due to Nintendo not providing review units this time around. But in reality, how much does it matter?", 'Switch 2 pre-orders were flying off the shelves in the US, and the extra stock available at launch is probably going to be swooped up by die hard fans.']</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>0.9081</v>
+        <v>0.4201</v>
       </c>
       <c r="I31" t="n">
-        <v>0.167</v>
+        <v>0.101</v>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>0.034</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>DL-9d1bad91e8b4cc20db3b991779086ad1</t>
+          <t>DL-c076e5bfb5dc9961cab30b68e0ec0dc1</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Islanders: New Shores to debut on PC and console in July</t>
+          <t>TAMAGOTCHI PLAZA released for the Nintendo Switch 2</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://www.gamereactor.it/islanders-new-shores-debuttera-su-pc-e-console-a-luglio-1481313/</t>
+          <t>https://game2gether.de/2025/06/tamagotchi-plaza-erscheint-fuer-nintendo-switch-2/</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>The Station has announced that their sequel to city building, Islanders: New Shores, will be released for PC and consoles in July. The game is described as a fascinating experience that allows players to "explore rooftop volcanic peaks, in fantastically intricate serene environments" the release date is set for July 10th, and the platforms are PC (Steam), Nintendo Switch (no word on Switch 2 yet), PS5 and Xbox Series X/S/S.</t>
+          <t>TAMAGOTCHI PLAZA will be released on June 27 for the Nintendo Switch and Nintendo Switch 2. The players take over different shops in Tamahiko Town and can thus interact with over 100 different Tamagotchis. It is important to expand more than a dozen different stores and expand the reputation in the city.</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>4.1608124</v>
-      </c>
-      <c r="F32" t="inlineStr"/>
+        <v>5.5119667</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-06-08T15:29:52</t>
+        </is>
+      </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Learn More Unlock Content Accept Required Service and Unlock Content TAMAGOTCHI PLAZA Nintendo Switch 2 Edition extends the gaming experience with three new stores, bringing the total to 15.']</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>0.7096</v>
+        <v>0.6597</v>
       </c>
       <c r="I32" t="n">
-        <v>0.111</v>
+        <v>0.125</v>
       </c>
       <c r="J32" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>DL-7fdb288e26fb545394f161b0835d8979</t>
+          <t>DL-887a2385045f651122c064ee4d0928fc</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 with Mario Kart World : Here’s how to make it cheaper with the return of your old Switch!</t>
+          <t>Endless coughs to buy the latest Nintendo console... and miss it</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://www.phonandroid.com/nintendo-switch-2-avec-mario-kart-world-voici-comment-lavoir-moins-chere-avec-la-reprise-de-votre-ancienne-switch.html</t>
+          <t>https://www.vozpopuli.com/altavoz/cultura/colas-interminables-para-comprar-la-ultima-consola-de-nintendo-y-se-quedan-sin-ella.html</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Switch 2 + Mario Kart World is available at Darty at €499.99. You can save up to €133.20 by recycling your old Switch. The Switch 2 is a new pillar of the franchise. It introduces an open world linking all circuits and 24-player races.</t>
+          <t>Nintendo announced the launch of their new Nintendo Switch 2 console on May 5th. The lack of'stock' has caused the consequent anger of those who have been left without their longed-for toy. Even some, who had paid in advance months in advance, have ended up without theirs.</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>4.1213493</v>
+        <v>4.928055</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-06-07T05:00:34+00:00</t>
+          <t>2025-06-07T02:45:07+00:00</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>['A thoroughly reviewed console and an unprecedented Mario Kart The Nintendo Switch 2 marks a real evolution from the original model.', 'It comes with a 7.9-inch 1080p LCD screen, a refresh rate raised to 120 Hz for increased fluidity, and 256GB of internal memory, which can be expanded via a Micro SD Express card (not compatible with older Micro SD cards).']</t>
+          <t>['The Nintendo Switch is today the third best-selling video game console in history and, at the rate it is going, everything indicates that it will soon reach second place.', 'The Nintendo Switch 2 was officially released on June 5, 2025, although there were people who were able to get it on June 4 to try it out earlier. However, there is a big problem with its release: there is not enough stock for everyone.']</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>0.4939</v>
+        <v>-0.7184</v>
       </c>
       <c r="I33" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>0</v>
+        <v>0.115</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>DL-069b859981ec37c594fae5168c6bcee6</t>
+          <t>DL-e8fdaa27ea9510e7798fabc955bb2d44</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>All official Nintendo Switch 2 accessories: complete list</t>
+          <t>The Nintendo Switch 2 eShop is super fast.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://www.larazon.es/videojuegos/setup-pro/todos-accesorios-oficiales-nintendo-switch-2-lista-completa_20250603683f34e17b27927d3dba1f42.html</t>
+          <t>https://nintendon.it/2025/06/05/leshop-di-nintendo-switch-2-e-velocissimo-312800</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Nintendo has always stood out for its ability to accompany the release of its consoles with a carefully designed environment. In order to enrich the user experience, the company bets on a wide range of essential accessories that enhance the possibilities of the console. The main protagonist is the new camera, an innovative accessory that introduces unique game dynamics and improves connectivity.</t>
+          <t>the eShop on the Nintendo Switch 2 is much more responsive and responsive. Even loading the game preview through the simple tab on the main screen is significantly faster. We can only imagine that, over the next few years, this will only get better.</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>4.095972</v>
+        <v>4.701721</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-06-03T17:46:39+00:00</t>
+          <t>2025-06-05T07:01:52+00:00</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>['Nintendo has always stood out for its ability to accompany the release of its consoles with a carefully designed environment, and Nintendo Switch 2 is no exception.', 'Nintendo GameCube Controller: Directed at nostalgic gamers, this GameCube classic replica control offers a true retro experience for Switch 2 compatible titles. It is available on the My Nintendo Store for €69.99.', 'The standard Nintendo Switch 2 pack is carefully designed to offer players a complete experience from the moment they open the box, providing all the essential components to immerse themselves in the new generation of Nintendo.']</t>
+          <t>["If there's one part of the original Nintendo Switch that was really annoying, it was definitely the experience of using the eShop. But in the end, it came to a respectable conclusion.", 'It turns out that the eShop on the Nintendo Switch 2 is much more responsive and responsive, allowing you to enjoy the content much more smoothly, both with the classic Joycon 2 keyboards and in mouse mode.']</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>0.8625</v>
+        <v>0.8169</v>
       </c>
       <c r="I34" t="n">
-        <v>0.174</v>
+        <v>0.175</v>
       </c>
       <c r="J34" t="n">
         <v>0</v>
@@ -1934,482 +1938,474 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>DL-6d0e71949253ac54c4daa072e2911a23</t>
+          <t>DL-9ead5a4840a28021df89936d4039541b</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Fortnite Nintendo Switch 2 has no 120fps mode on launch, but it’s a massive improvement over the rancid Switch 1 port</t>
+          <t>Switch 2 games load much slower from cartridges than a microSD Express card or internal storage</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://www.videogamer.com/news/fortnite-nintendo-switch-2-no-120fps-mode-launch/</t>
+          <t>https://www.notebookcheck.net/Switch-2-games-load-much-slower-from-cartridges-than-a-microSD-Express-card-or-internal-storage.1032520.0.html</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Epic Games has released the full list of features for the Nintendo Switch 2 Edition of its free-to-play battle royale game. Fortnite runs at 60fps in both docked and handheld play, which is heaps better than the original handheld. The new handheld has higher-quality asseta across the board with textures on-par with other costumes, actual shadows and water shaders.</t>
+          <t>Switch 2 specs include internal 256GB UFS storage, which wins the checkered flag with a time of 16.60 seconds. SanDisk, Samsung, and Lexar microSD Express cards finish second between 19.18 and 19.78 seconds, and Game Card finishes in last place.</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>3.4143333</v>
+        <v>4.3257656</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-06-04T14:57:18+00:00</t>
+          <t>2025-06-08T04:13:27+00:00</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>["Our team of gaming experts spend hours testing and reviewing the latest games, to ensure you're reading the most comprehensive guide possible. Rest assured, all imagery and advice is unique and original.", 'Check out how we test and review games here\nEpic Games has released the full list of features for the Nintendo Switch 2 Edition of its free-to-play battle royale game.']</t>
+          <t>['The number of ways to play or store Switch 2 games can confuse buyers. In addition to cartridges, internal storage, and microSD Express cards, gamers can experiment with Game-Key Cards.', "For Nintendo fans who prioritize speed, a new benchmark compares these different formats. It's no shock that the console's built-in flash storage ranks first. Still, the fact that Switch 2 cartridges are significantly slower may surprise gamers."]</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>0.8658</v>
+        <v>0.5719</v>
       </c>
       <c r="I35" t="n">
-        <v>0.185</v>
+        <v>0.098</v>
       </c>
       <c r="J35" t="n">
-        <v>0.036</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>DL-39e749ba8f4fabb28b4c41cfc788cbe9</t>
+          <t>DL-24b1842a456f3df8f5436bc5f2ff0e03</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: everything you need to know about the new console</t>
+          <t>Your Nintendo Switch 2 Launch Kit: The Best Accessories</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://www.publimetro.com.mx/plus/2025/06/05/nintendo-switch-2-todo-lo-que-debes-saber-de-la-nueva-consola/</t>
+          <t>https://www.techlicious.com/guide/nintendo-switch-2-accessories/</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 will cost 13,599 Mexican pesos in Mexico, with no games included. The price goes up to 14.899 in the case of the version with Mario Kart World Photo: Courtesy Nintendo of America The wait finally ended for millions of gamers as the new console officially arrived on June 5th.</t>
+          <t>The official Nintendo Switch 2 Pro Controller is one of the best that money can buy. From controllers to carry cases, cameras to microSD cards, there are plenty of ways to maximize your Switch 2 experience. This wireless controller offers responsive buttons, precise analog sticks, and ergonomic grips designed to keep your hands comfortable during extended play sessions. It also features built-in motion controls and HD rumble.</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>3.3168545</v>
+        <v>4.2812214</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-06-05T03:09:27</t>
+          <t>2025-06-05T00:00:00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>['Nintendo Switch 2 Photo: Courtesy of Nintendo of America It also has a rate of up to 120 fps on some titles, allowing a smoother gaming experience.', 'As for the portable mode, it has a Full HD resolution of 1920 x 1080 pixels and a refresh rate of 120 Hz.', 'The Nintendo Switch 2 can also be used in a semi-portable way thanks to the built-in support that allows you to tilt it up to 150 degrees to find the most comfortable position to play.']</t>
+          <t>['From controllers to carry cases, cameras to microSD cards, there are plenty of ways to maximize your Switch 2 experience. So without further ado, here are the best Nintendo Switch 2 accessories currently (and shortly) available.', 'Best Controllers for a Premium Play Experience\nNintendo Switch 2 Pro Controller\nIf you’re planning on couch-playing with your Switch 2 in docked mode, a decent controller is an absolute must-have, and the official Nintendo Switch 2 Pro Controller is one']</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>0.0772</v>
+        <v>0.9081</v>
       </c>
       <c r="I36" t="n">
-        <v>0.048</v>
+        <v>0.167</v>
       </c>
       <c r="J36" t="n">
-        <v>0.043</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>DL-0baa58f2b21229daa16ed87a04ee6380</t>
+          <t>DL-4a140a18c5aefde1b5970f7608d46b27</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>I missed those games on the release of Nintendo Switch 2</t>
+          <t>Nintendo Switch 2: Live updates on launch night</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://antyweb.pl/tych-gier-zabraklo-mi-na-premierze-nintendo-switch-2</t>
+          <t>https://www.independent.co.uk/extras/indybest/gadgets-tech/video-games-consoles/nintendo-switch-2-stock-live-uk-b2763929.html</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 officially went on sale yesterday and is enjoying great interest – also in Poland, where a night event was organized. Nintendo did not have a strong presence among the original titles.</t>
+          <t>Smyths Toys opened all of its shops at midnight, offering a limited amount of walk-in stoc, but doors are closing at 12.30am. Over on Oxford Street, Currys is running a launch event at its flagship store. A few retailers are holding back stock for the early hours of the morning. Retailers are gearing up to drop more Switch 2 stock online as the morning unfolds.</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>3.1638184</v>
+        <v>4.200737</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-06-06T10:30:18</t>
+          <t>2025-06-04T21:52:05+00:00</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>['Undoubtedly the biggest hit will be Mario Kart World – a game that develops the concept of racing with the protagonists of Nintendo games giving a breath of freshness with new fun modes.', 'Special mention should be made of Cyberpunk 2077 in the Ultimate edition, which is available on the day of the Nintendo Switch 2 release and offers the full experience of Night City in a portable version.']</t>
+          <t>["Alex Lee4 June 2025 23:10\n57 minutes ago\nIt's almost time\nLess than an hour to go until retailers start going live with Nintendo Switch 2 stock. Who do you think will go first?", 'Unboxing my Switch 2 was like Christmas morning, so I’m excited for you all to experience the same.\nAre you in one of Smyths Toys’s flagship shops already? What’s the vibe? Let me know.', 'Oh, and there will be limited stock of the Nintendo Switch 2 available, too.']</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>0.8778</v>
+        <v>-0.3612</v>
       </c>
       <c r="I37" t="n">
-        <v>0.316</v>
+        <v>0.025</v>
       </c>
       <c r="J37" t="n">
-        <v>0.067</v>
+        <v>0.063</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>DL-2a978e6f0390cba5e2c1c92d76359a8c</t>
+          <t>DL-9d1bad91e8b4cc20db3b991779086ad1</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>EE launches exclusive Nintendo Switch 2 bundles</t>
+          <t>Islanders: New Shores to debut on PC and console in July</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://www.techdigest.tv/2025/06/ee-launches-exclusive-nintendo-switch-2-bundles.html?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=ee-launches-exclusive-nintendo-switch-2-bundles</t>
+          <t>https://www.gamereactor.it/islanders-new-shores-debuttera-su-pc-e-console-a-luglio-1481313/</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Share Mobile and broadband provider EE has announced a range of exclusive new bundles for the highly anticipated Nintendo Switch 2 console. Each bundle requires a £20 upfront cost on a 24-month plan and includes the new console, the upcoming Mario Kart World game and a 12-month Nintendo Switch Online subscription with Expansion Pack. A key feature across all bundles is a 24month subscription to EE’s Gamer and Video Data Pass, allowing users to stream and play games without impacting their standard data allowance </t>
+          <t>The Station has announced that their sequel to city building, Islanders: New Shores, will be released for PC and consoles in July. The game is described as a fascinating experience that allows players to "explore rooftop volcanic peaks, in fantastically intricate serene environments" the release date is set for July 10th, and the platforms are PC (Steam), Nintendo Switch (no word on Switch 2 yet), PS5 and Xbox Series X/S/S.</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>3.0962734</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>2025-06-05T08:36:40</t>
-        </is>
-      </c>
+        <v>4.161209</v>
+      </c>
+      <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
-          <t>['Share\nMobile and broadband provider EE has announced a range of exclusive new bundles for the highly anticipated Nintendo Switch 2 console.', 'Available from today, June 5th, these packages aim to offer gamers an enhanced experience with included connectivity features.', 'Each bundle requires a £20 upfront cost on a 24-month plan and includes the new Nintendo Switch 2 console, the upcoming Mario Kart World game and a 12-month Nintendo Switch Online subscription with Expansion Pack.']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>0.6249</v>
+        <v>0.7096</v>
       </c>
       <c r="I38" t="n">
-        <v>0.077</v>
+        <v>0.111</v>
       </c>
       <c r="J38" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>DL-4a140a18c5aefde1b5970f7608d46b27</t>
+          <t>DL-c52009334545d09049979dae231d50d4</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: Live updates on launch night</t>
+          <t>How to get a Nintendo Switch 2 from Best Buy, GameStop, Target and more</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://www.independent.co.uk/extras/indybest/gadgets-tech/video-games-consoles/nintendo-switch-2-stock-live-uk-b2763929.html</t>
+          <t>https://www.independent.co.uk/extras/indybest/us/nintendo-switch-2-gamestop-best-buy-target-b2762563.html</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Smyths Toys opened all of its shops at midnight, offering a limited amount of walk-in stoc, but doors are closing at 12.30am. Over on Oxford Street, Currys is running a launch event at its flagship store. A few retailers are holding back stock for the early hours of the morning. Retailers are gearing up to drop more Switch 2 stock online as the morning unfolds.</t>
+          <t>Your support helps us to tell the story Read more Support Now From reproductive rights to Big Tech, The Independent is on the ground when the story is developing. Your donation allows us to keep sending journalists to both sides of the story. We believe quality journalism should be available to everyone, paid for by those who can afford it.</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>2.9316483</v>
+        <v>4.141777</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-06-04T21:52:05+00:00</t>
+          <t>2025-06-03T10:15:58</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>["Alex Lee4 June 2025 23:10\n57 minutes ago\nIt's almost time\nLess than an hour to go until retailers start going live with Nintendo Switch 2 stock. Who do you think will go first?", 'Unboxing my Switch 2 was like Christmas morning, so I’m excited for you all to experience the same.\nAre you in one of Smyths Toys’s flagship shops already? What’s the vibe? Let me know.', 'Oh, and there will be limited stock of the Nintendo Switch 2 available, too.']</t>
+          <t>['We got a first look at the Nintendo Switch 2 – read our hands-on review']</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>-0.3612</v>
+        <v>0.7906</v>
       </c>
       <c r="I39" t="n">
-        <v>0.025</v>
+        <v>0.123</v>
       </c>
       <c r="J39" t="n">
-        <v>0.063</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>DL-be4b0877ab72d480615d2f3254053e13</t>
+          <t>DL-069b859981ec37c594fae5168c6bcee6</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Moving my self-hosted empire to Proxmox was a breeze</t>
+          <t>All official Nintendo Switch 2 accessories: complete list</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://www.xda-developers.com/thread/moving-my/</t>
+          <t>https://www.larazon.es/videojuegos/setup-pro/todos-accesorios-oficiales-nintendo-switch-2-lista-completa_20250603683f34e17b27927d3dba1f42.html</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Nintendo has been making a lot of little weird decisions with the Switch 2. It's been a long wait for a new generation of consoles since the launch of the original hardware. Fans have speculated on a successor or major upgrade to the Switch.</t>
+          <t>Nintendo has always stood out for its ability to accompany the release of its consoles with a carefully designed environment. In order to enrich the user experience, the company bets on a wide range of essential accessories that enhance the possibilities of the console. The main protagonist is the new camera, an innovative accessory that introduces unique game dynamics and improves connectivity.</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>2.8678513</v>
+        <v>4.0958786</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-06-04T22:16:05+00:00</t>
+          <t>2025-06-03T17:46:39+00:00</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>["And now, that's happening again, as outlets have confirmed they won't be publishing reviews of the Switch 2 on release day due to Nintendo not providing review units this time around. But in reality, how much does it matter?", 'Switch 2 pre-orders were flying off the shelves in the US, and the extra stock available at launch is probably going to be swooped up by die hard fans.']</t>
+          <t>['Nintendo has always stood out for its ability to accompany the release of its consoles with a carefully designed environment, and Nintendo Switch 2 is no exception.', 'Nintendo GameCube Controller: Directed at nostalgic gamers, this GameCube classic replica control offers a true retro experience for Switch 2 compatible titles. It is available on the My Nintendo Store for €69.99.', 'The standard Nintendo Switch 2 pack is carefully designed to offer players a complete experience from the moment they open the box, providing all the essential components to immerse themselves in the new generation of Nintendo.']</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>0.4201</v>
+        <v>0.8625</v>
       </c>
       <c r="I40" t="n">
-        <v>0.101</v>
+        <v>0.174</v>
       </c>
       <c r="J40" t="n">
-        <v>0.034</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>DL-b2b049aaa24705881044f0a75bfc6392</t>
+          <t>DL-ce5f9cdf63998a111dd0a2e7410853d6</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 : some players have had a very bad surprise with their console</t>
+          <t>Meta in talks with Disney, A24 and others to secure content for VR headsets</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://www.gameblog.fr/jeu-video/ed/news/nintendo-switch-2-mauvaises-surprises-696414</t>
+          <t>https://gigazine.net/gsc_news/en/20250605-meta-vr-contents-from-disney-a24/</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 is always a major event, both for the manufacturer and for the players. This, unfortunately, can involve blindness. At the end of 2020, the launches of the PS5 and Xbox Series marked the story in this sense, in the midst of the coronavirus pandemic.</t>
+          <t>FFmpeg has integrated WebRTC support, enabling ultra-low latency streaming of less than 1 second with OBS, the latest codecs can be selected, and even streaming without a server is now possible X files lawsuit against eight users who tried to unfairly increase their revenue by abusing 'creator revenue sharing' Meta announces details of AI smart glasses 'Aria Gen 2', explaining cutting-edge camera and sensor technology Results of 'MLPerf Training v5.0', which</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>2.666113</v>
+        <v>4.092514</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-06-06T11:31:30+00:00</t>
+          <t>2025-06-05T06:24:00+00:00</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>['The Nintendo Switch 2 has unfortunately not escaped some unforeseen, as some players have unfortunately had the bitter experience of opening the cardboard of their console.']</t>
+          <t>["reaffirms plans to invest $100 billion in Arizona over next five years\nPart of 'MetaHuman', a game development tool that allows you to create and move ultra-realistic 3DCG characters for free, is integrated into Unreal Engine 5.6\nThe reason why the Nintendo", "Switch 2 was not loaned to the media for pre-release review was because 'important features and updates for the console' will be provided on the release date of June 5th.", "Speculation is rife that the Chinese-made high-performance AI model 'DeepSeek-R1-0528' may have been distilled using Google's AI 'Gemini'\nAttention is drawn to the warning in the Nintendo Switch 2 manual that reads, 'Do not remove the shatterproof film"]</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>-0.4118</v>
+        <v>0.4588</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>0.133</v>
       </c>
       <c r="J41" t="n">
-        <v>0.06</v>
+        <v>0.108</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>DL-c52009334545d09049979dae231d50d4</t>
+          <t>DL-6d0e71949253ac54c4daa072e2911a23</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>How to get a Nintendo Switch 2 from Best Buy, GameStop, Target and more</t>
+          <t>Fortnite Nintendo Switch 2 has no 120fps mode on launch, but it’s a massive improvement over the rancid Switch 1 port</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://www.independent.co.uk/extras/indybest/us/nintendo-switch-2-gamestop-best-buy-target-b2762563.html</t>
+          <t>https://www.videogamer.com/news/fortnite-nintendo-switch-2-no-120fps-mode-launch/</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Your support helps us to tell the story Read more Support Now From reproductive rights to Big Tech, The Independent is on the ground when the story is developing. Your donation allows us to keep sending journalists to both sides of the story. We believe quality journalism should be available to everyone, paid for by those who can afford it.</t>
+          <t>Epic Games has released the full list of features for the Nintendo Switch 2 Edition of its free-to-play battle royale game. Fortnite runs at 60fps in both docked and handheld play, which is heaps better than the original handheld. The new handheld has higher-quality asseta across the board with textures on-par with other costumes, actual shadows and water shaders.</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>2.630474</v>
+        <v>3.9428139</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-06-03T10:15:58</t>
+          <t>2025-06-04T14:57:18+00:00</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>['We got a first look at the Nintendo Switch 2 – read our hands-on review']</t>
+          <t>["Our team of gaming experts spend hours testing and reviewing the latest games, to ensure you're reading the most comprehensive guide possible. Rest assured, all imagery and advice is unique and original.", 'Check out how we test and review games here\nEpic Games has released the full list of features for the Nintendo Switch 2 Edition of its free-to-play battle royale game.']</t>
         </is>
       </c>
       <c r="H42" t="n">
-        <v>0.7906</v>
+        <v>0.8658</v>
       </c>
       <c r="I42" t="n">
-        <v>0.123</v>
+        <v>0.185</v>
       </c>
       <c r="J42" t="n">
-        <v>0</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>DL-9e7bd803a3254229cbb9e3b27f0fda79</t>
+          <t>DL-b080cb5509d88a1ec15ee8a2c6106938</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 is here: everything you need to know about the new console</t>
+          <t>Get the most out of your Nintendo Switch 2 with these 3 TVs I've picked to pair with it, including one of the best OLED TVs I've seen</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://www.lavanguardia.com/vida/20250605/10755562/nintendo-switch-2-caracteristicas-modelos-precio-accesorios-juegos.html</t>
+          <t>https://www.techradar.com/televisions/get-the-most-out-of-your-nintendo-switch-2-with-these-3-tvs-ive-picked-to-pair-with-it-including-one-of-the-best-oled-tvs-ive-seen</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 comes to stores eight years after the first model surprised with its hybrid design (portable and desktop), but also after one of the biggest commercial triumphs in the history of video games. The rise in the price of both the machine and the games has monopolized the conversation since Nintendo introduced Switch 2 at the beginning of April. This article discusses the price, but also the main features of the console, its compatibility with the original model or its accessories.</t>
+          <t>TechRadar look for VRR, 120Hz refresh rate and Auto Low Latency Mode. Low input lag for responsive performance and top-notch picture quality are also important. LG B4 48-inch 4K OLED TV : £879 now £849 at Best Buy The LG C4 provides premium OLED picture quality and a full array of gaming features.</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>2.6206264</v>
+        <v>3.8008957</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-06-05T06:00:00</t>
+          <t>2025-06-06T08:00:00</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>["At the moment, few highlighted Games 'Cyberpunk 2077' is one of the most striking games of Nintendo Switch 2 • Mario Kart World: In the absence of a thorough trial, and with only a first hour of play, the first big must-have of Nintendo Switch 2 is this", 'This is a game that incorporates important innovations, such as the inclusion of a great open world, and that demonstrates the leap in power compared to the original Nintendo Switch. • Nintendo Switch 2 Welcome Tour: This collection of minigames and experiences', 'It would be the typical game that comes with the console, but Nintendo has decided to charge 10 euros for it. • Cyberpunk 2077 Ultimate Edition: The ambitious futuristic adventure of CD Projekt Red is one of the most surprising games to see running on']</t>
+          <t>['The Nintendo Switch 2 has finally arrived, and it brings several upgrades over its predecessor, including 4K resolution, 120Hz (at 1080p resolution) and HDR support.', 'And there’s no better time to buy one to pair with your Nintendo Switch 2 with ambitious ports such as Cyberpunk: 2077 available from launch.', 'The Switch 2 can once again take advantage of that low input lag time for ultra-responsive performance (crucial for Mario Kart World) and the B4’s 4K, HDR and 120Hz support to level-up their experience from the original Nintendo Switch.']</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>0.7227</v>
+        <v>0.5719</v>
       </c>
       <c r="I43" t="n">
-        <v>0.096</v>
+        <v>0.181</v>
       </c>
       <c r="J43" t="n">
-        <v>0.027</v>
+        <v>0.116</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>DL-182e127a12c29e22cad855da74591ca5</t>
+          <t>DL-6b1dfb573ca972c47a35c3452e0b887c</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Zelda: Tears of the Kingdom Modded With Ray Tracing Looks Stunning in New 8K Video</t>
+          <t>With the release of the Nintendo Switch 2, what's the future for the Switch?</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://wccftech.com/zelda-tears-of-the-kingdom-ray-tracing-8k/</t>
+          <t>https://www.gamekult.com/actualite/avec-la-sortie-de-la-nintendo-switch-2-quel-avenir-pour-la-switch-3050864092.html</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>The Legend of Zelda: Tears of the Kingdom can look stunning with some choice mods on PC, which outshine the recently released Nintendo Switch 2 edition. A new video shared a few days ago shows the latest main entry in the series running on PC via an emulator at 8K resolution with some mods.</t>
+          <t>Nintendo has always shown a rigorous follow-up on its previous consoles. Examples include the 3DS, which was eligible for new features until 2019 (two years after Switch’s release), and an online store until 2023. The real question would be whether Nintendo would be willing to offer its productions on both machines at the same time.</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>2.6030064</v>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>2025-06-06T12:07:00+00:00</t>
-        </is>
-      </c>
+        <v>3.2541294</v>
+      </c>
+      <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
-          <t>['As even an RTX 5090 has some trouble running the game at 60 FPS at such a high resolution and with these mods, it would have been unreasonable to expect such a makeover to run on the Nintendo Switch 2, so those who wish to experience the game like never', "Related Story Batman Arkham Knight, One of the Worst Nintendo Switch Ports Ever, Gets Significant Performance Boost on Nintendo Switch 2\nThe fact that The Legend of Zelda: Tears of the Kingdom on Nintendo Switch 2 doesn't feature any transformative visual"]</t>
+          <t>['Samus will be on both Switches A situation that is explained by Nintendo’s legacy, but also by the fact that the adoption rate of the console is probably still questionable at the moment.', 'If Nintendo has not spoken out on this issue, Kyoto is well aware that the switch 2 adoption curve is more uncertain than the first one, in the sense that consumers will be much more reluctant to switch, mainly for price reasons of course.']</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>0.4767</v>
+        <v>-0.2732</v>
       </c>
       <c r="I44" t="n">
-        <v>0.093</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>0.035</v>
+        <v>0.039</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>DL-2e469f3f8789d2c101197abc3c31aac9</t>
+          <t>DL-f5ec55248d270c706daae41500b0144a</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Mario Kart World review – the final verdict on the Switch 2’s biggest game</t>
+          <t>Nintendo Switch 2 launches with Street Fighter 6 demo in the eShop</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://metro.co.uk/2025/06/10/mario-kart-world-review-final-verdict-switch-2s-biggest-game-23373706/</t>
+          <t>https://www.playcentral.de/nintendo-switch-2-startet-mit-street-fighter-6-demo-im-eshop-durch/</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Mario Kart 8 Deluxe is one of the very few games we’ve ever given a 10/10 score. That’s not something we regret either, especially after the extremely generous Booster Course DLC. The idea of making the next game an open world title seemed an excellent new direction to take the series. It’s very poorly utilised, with lots of hidden secrets and yet nothing of substance to gain from them.</t>
+          <t>Street Fighter 6 demo is now available in the Nintendo eShop. It allows players to test some of the game's modes before purchasing. The demo is available on the Nintendo Switch 2 and offers fans the opportunity to try out the game.</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>2.5434074</v>
+        <v>3.204979</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-06-10T08:07:26+00:00</t>
+          <t>2025-06-08T17:02:54</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>['Thanks to Nintendo not sending out review units of the Nintendo Switch 2 more than a day before launch we’ve previously only been able to do a review in progress of World, during which it became clear that it is not quite the game that many imagined.']</t>
+          <t>['It offers players the ability to enjoy the game in 1080p resolution with a refresh rate of 120Hz in handheld or table mode, while it supports 4K at 60Hz in dock mode.', 'Conclusion and Community Issue The availability of the free demo of Street Fighter 6 on the Nintendo Switch 2 is welcome news for all those who were disappointed by the limited number of new games introduced on the console.', 'It offers the opportunity to experience one of the best fighting games of 2023 on the new hardware. How do you find the current line-up of the Nintendo Switch 2? Are you going to try the Street Fighter 6 demo?']</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>0.919</v>
+        <v>0.5266999999999999</v>
       </c>
       <c r="I45" t="n">
-        <v>0.171</v>
+        <v>0.104</v>
       </c>
       <c r="J45" t="n">
         <v>0</v>
@@ -2418,86 +2414,86 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>DL-f5ec55248d270c706daae41500b0144a</t>
+          <t>DL-0baa58f2b21229daa16ed87a04ee6380</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 launches with Street Fighter 6 demo in the eShop</t>
+          <t>I missed those games on the release of Nintendo Switch 2</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://www.playcentral.de/nintendo-switch-2-startet-mit-street-fighter-6-demo-im-eshop-durch/</t>
+          <t>https://antyweb.pl/tych-gier-zabraklo-mi-na-premierze-nintendo-switch-2</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Street Fighter 6 demo is now available in the Nintendo eShop. It allows players to test some of the game's modes before purchasing. The demo is available on the Nintendo Switch 2 and offers fans the opportunity to try out the game.</t>
+          <t>Nintendo Switch 2 officially went on sale yesterday and is enjoying great interest – also in Poland, where a night event was organized. Nintendo did not have a strong presence among the original titles.</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>2.4696312</v>
+        <v>3.1655617</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-06-08T17:02:54</t>
+          <t>2025-06-06T10:30:18</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>['It offers players the ability to enjoy the game in 1080p resolution with a refresh rate of 120Hz in handheld or table mode, while it supports 4K at 60Hz in dock mode.', 'Conclusion and Community Issue The availability of the free demo of Street Fighter 6 on the Nintendo Switch 2 is welcome news for all those who were disappointed by the limited number of new games introduced on the console.', 'It offers the opportunity to experience one of the best fighting games of 2023 on the new hardware. How do you find the current line-up of the Nintendo Switch 2? Are you going to try the Street Fighter 6 demo?']</t>
+          <t>['Undoubtedly the biggest hit will be Mario Kart World – a game that develops the concept of racing with the protagonists of Nintendo games giving a breath of freshness with new fun modes.', 'Special mention should be made of Cyberpunk 2077 in the Ultimate edition, which is available on the day of the Nintendo Switch 2 release and offers the full experience of Night City in a portable version.']</t>
         </is>
       </c>
       <c r="H46" t="n">
-        <v>0.5266999999999999</v>
+        <v>0.8778</v>
       </c>
       <c r="I46" t="n">
-        <v>0.104</v>
+        <v>0.316</v>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
+        <v>0.067</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>DL-37c373fee1dff1bb24a16495a09080f5</t>
+          <t>DL-2a978e6f0390cba5e2c1c92d76359a8c</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 vs Nintendo Switch : what are the main differences?</t>
+          <t>EE launches exclusive Nintendo Switch 2 bundles</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://www.numerama.com/tech/1988347-nintendo-switch-2-vs-nintendo-switch-quelles-sont-les-principales-differences.html</t>
+          <t>https://www.techdigest.tv/2025/06/ee-launches-exclusive-nintendo-switch-2-bundles.html?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=ee-launches-exclusive-nintendo-switch-2-bundles</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Switch 2 is a direct evolution of the Switch (Standard and OLED) it is also able to play its games, thanks to backwards compatibility. The launch catalogue already offers its own exclusives with the latest Mario Kart World, available only on this new model. There are also many improvements that, when completed, make this console a much more significant advance than the OLED Switch had been compared to the classic Switch.</t>
+          <t xml:space="preserve">Share Mobile and broadband provider EE has announced a range of exclusive new bundles for the highly anticipated Nintendo Switch 2 console. Each bundle requires a £20 upfront cost on a 24-month plan and includes the new console, the upcoming Mario Kart World game and a 12-month Nintendo Switch Online subscription with Expansion Pack. A key feature across all bundles is a 24month subscription to EE’s Gamer and Video Data Pass, allowing users to stream and play games without impacting their standard data allowance </t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>2.4266968</v>
+        <v>3.0963783</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-06-10T14:12:11+00:00</t>
+          <t>2025-06-05T08:36:40</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>['The Nintendo Switch 2 relies on a catalogue of exclusive games. Mario kart World is the first of its kind and there is no chance that it will be seen on previous generations. So a big argument: that of ensuring compatibility with the next games.', 'Which Nintendo Switch to choose? After reviewing the many differences between the models, the question remains: what is the best choice for Nintendo Switch in 2025?', 'In short, the Switch 2 is now the best option at Nintendo, not only because it’s the latest console to date (the OLED Switch was not specifically recommended at the time of its release). But this new Switch 2 marks a new chapter.']</t>
+          <t>['Share\nMobile and broadband provider EE has announced a range of exclusive new bundles for the highly anticipated Nintendo Switch 2 console.', 'Available from today, June 5th, these packages aim to offer gamers an enhanced experience with included connectivity features.', 'Each bundle requires a £20 upfront cost on a 24-month plan and includes the new Nintendo Switch 2 console, the upcoming Mario Kart World game and a 12-month Nintendo Switch Online subscription with Expansion Pack.']</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>0.8268</v>
+        <v>0.6249</v>
       </c>
       <c r="I47" t="n">
-        <v>0.132</v>
+        <v>0.077</v>
       </c>
       <c r="J47" t="n">
         <v>0</v>
@@ -2506,302 +2502,306 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>DL-887a2385045f651122c064ee4d0928fc</t>
+          <t>DL-37c373fee1dff1bb24a16495a09080f5</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Endless coughs to buy the latest Nintendo console... and miss it</t>
+          <t>Nintendo Switch 2 vs Nintendo Switch : what are the main differences?</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://www.vozpopuli.com/altavoz/cultura/colas-interminables-para-comprar-la-ultima-consola-de-nintendo-y-se-quedan-sin-ella.html</t>
+          <t>https://www.numerama.com/tech/1988347-nintendo-switch-2-vs-nintendo-switch-quelles-sont-les-principales-differences.html</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Nintendo announced the launch of their new Nintendo Switch 2 console on May 5th. The lack of'stock' has caused the consequent anger of those who have been left without their longed-for toy. Even some, who had paid in advance months in advance, have ended up without theirs.</t>
+          <t>Switch 2 is a direct evolution of the Switch (Standard and OLED) it is also able to play its games, thanks to backwards compatibility. The launch catalogue already offers its own exclusives with the latest Mario Kart World, available only on this new model. There are also many improvements that, when completed, make this console a much more significant advance than the OLED Switch had been compared to the classic Switch.</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>2.3237877</v>
+        <v>2.8471222</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-06-07T02:45:07+00:00</t>
+          <t>2025-06-10T14:12:11+00:00</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>['The Nintendo Switch is today the third best-selling video game console in history and, at the rate it is going, everything indicates that it will soon reach second place.', 'The Nintendo Switch 2 was officially released on June 5, 2025, although there were people who were able to get it on June 4 to try it out earlier. However, there is a big problem with its release: there is not enough stock for everyone.']</t>
+          <t>['The Nintendo Switch 2 relies on a catalogue of exclusive games. Mario kart World is the first of its kind and there is no chance that it will be seen on previous generations. So a big argument: that of ensuring compatibility with the next games.', 'Which Nintendo Switch to choose? After reviewing the many differences between the models, the question remains: what is the best choice for Nintendo Switch in 2025?', 'In short, the Switch 2 is now the best option at Nintendo, not only because it’s the latest console to date (the OLED Switch was not specifically recommended at the time of its release). But this new Switch 2 marks a new chapter.']</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>-0.7184</v>
+        <v>0.8268</v>
       </c>
       <c r="I48" t="n">
-        <v>0</v>
+        <v>0.132</v>
       </c>
       <c r="J48" t="n">
-        <v>0.115</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>DL-ce5f9cdf63998a111dd0a2e7410853d6</t>
+          <t>DL-f18eecd6ae1aa3953cec4cf5dcc3e634</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Meta in talks with Disney, A24 and others to secure content for VR headsets</t>
+          <t>'I own a Switch 2 - this console case beats Nintendo's thanks to one main feature'</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://gigazine.net/gsc_news/en/20250605-meta-vr-contents-from-disney-a24/</t>
+          <t>https://www.birminghammail.co.uk/whats-on/shopping/i-switch-2-console-case-31823315</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>FFmpeg has integrated WebRTC support, enabling ultra-low latency streaming of less than 1 second with OBS, the latest codecs can be selected, and even streaming without a server is now possible X files lawsuit against eight users who tried to unfairly increase their revenue by abusing 'creator revenue sharing' Meta announces details of AI smart glasses 'Aria Gen 2', explaining cutting-edge camera and sensor technology Results of 'MLPerf Training v5.0', which</t>
+          <t>The Nintendo Switch 2 is out and I was lucky enough to get my hands on the Switch 2 on release day. There are plenty of choices out there, including the official Nintendo Switch 2, which can be bought almost everywhere. Amazon lawnmower reduced from over £100 is 'lightweight' and 'easy to handle'</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>2.3176746</v>
+        <v>2.7896347</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-06-05T06:24:00+00:00</t>
+          <t>2025-06-10T10:29:21+00:00</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>["reaffirms plans to invest $100 billion in Arizona over next five years\nPart of 'MetaHuman', a game development tool that allows you to create and move ultra-realistic 3DCG characters for free, is integrated into Unreal Engine 5.6\nThe reason why the Nintendo", "Switch 2 was not loaned to the media for pre-release review was because 'important features and updates for the console' will be provided on the release date of June 5th.", "Speculation is rife that the Chinese-made high-performance AI model 'DeepSeek-R1-0528' may have been distilled using Google's AI 'Gemini'\nAttention is drawn to the warning in the Nintendo Switch 2 manual that reads, 'Do not remove the shatterproof film"]</t>
+          <t>["The Nintendo Switch 2 is out and in the search for a new case - I might have found my top choice thanks to one main feature\nI was lucky enough to get my hands on the Nintendo Switch 2 on release day, and it's definitely one of my favourite purchases so", "Without going into a massive review of the console, it is the definitive Switch experience, and it's exciting to see what the future holds for it."]</t>
         </is>
       </c>
       <c r="H49" t="n">
-        <v>0.4588</v>
+        <v>0.7287</v>
       </c>
       <c r="I49" t="n">
-        <v>0.133</v>
+        <v>0.137</v>
       </c>
       <c r="J49" t="n">
-        <v>0.108</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>DL-b080cb5509d88a1ec15ee8a2c6106938</t>
+          <t>DL-b2b049aaa24705881044f0a75bfc6392</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Get the most out of your Nintendo Switch 2 with these 3 TVs I've picked to pair with it, including one of the best OLED TVs I've seen</t>
+          <t>Nintendo Switch 2 : some players have had a very bad surprise with their console</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://www.techradar.com/televisions/get-the-most-out-of-your-nintendo-switch-2-with-these-3-tvs-ive-picked-to-pair-with-it-including-one-of-the-best-oled-tvs-ive-seen</t>
+          <t>https://www.gameblog.fr/jeu-video/ed/news/nintendo-switch-2-mauvaises-surprises-696414</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>TechRadar look for VRR, 120Hz refresh rate and Auto Low Latency Mode. Low input lag for responsive performance and top-notch picture quality are also important. LG B4 48-inch 4K OLED TV : £879 now £849 at Best Buy The LG C4 provides premium OLED picture quality and a full array of gaming features.</t>
+          <t>Nintendo Switch 2 is always a major event, both for the manufacturer and for the players. This, unfortunately, can involve blindness. At the end of 2020, the launches of the PS5 and Xbox Series marked the story in this sense, in the midst of the coronavirus pandemic.</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>2.0356522</v>
+        <v>2.6671867</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-06-06T08:00:00</t>
+          <t>2025-06-06T11:31:30+00:00</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>['The Nintendo Switch 2 has finally arrived, and it brings several upgrades over its predecessor, including 4K resolution, 120Hz (at 1080p resolution) and HDR support.', 'And there’s no better time to buy one to pair with your Nintendo Switch 2 with ambitious ports such as Cyberpunk: 2077 available from launch.', 'The Switch 2 can once again take advantage of that low input lag time for ultra-responsive performance (crucial for Mario Kart World) and the B4’s 4K, HDR and 120Hz support to level-up their experience from the original Nintendo Switch.']</t>
+          <t>['The Nintendo Switch 2 has unfortunately not escaped some unforeseen, as some players have unfortunately had the bitter experience of opening the cardboard of their console.']</t>
         </is>
       </c>
       <c r="H50" t="n">
-        <v>0.5719</v>
+        <v>-0.4118</v>
       </c>
       <c r="I50" t="n">
-        <v>0.181</v>
+        <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>0.116</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>DL-bc0bf2ef431589eeb38d530dce7bdf45</t>
+          <t>DL-9e7bd803a3254229cbb9e3b27f0fda79</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Bouncemasters demo now available on Steam</t>
+          <t>Nintendo Switch 2 is here: everything you need to know about the new console</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://thatsgaming.nl/bouncemasters-demo-nu-beschikbaar-op-steam/</t>
+          <t>https://www.lavanguardia.com/vida/20250605/10755562/nintendo-switch-2-caracteristicas-modelos-precio-accesorios-juegos.html</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Bouncemasters is a fun physics-based arcade game inspired by Yetisports. The full version comes out on Steam in the third quarter of 2025. TAMAGOTCHI PLAZA is coming to the Nintendo Switch 2 and Nintendo Switch 2. Both versions will be compatible with the Tamagotchi Uni device.</t>
+          <t>Nintendo Switch 2 comes to stores eight years after the first model surprised with its hybrid design (portable and desktop), but also after one of the biggest commercial triumphs in the history of video games. The rise in the price of both the machine and the games has monopolized the conversation since Nintendo introduced Switch 2 at the beginning of April. This article discusses the price, but also the main features of the console, its compatibility with the original model or its accessories.</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>1.8311577</v>
+        <v>2.6207256</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-06-06T18:57:55+00:00</t>
+          <t>2025-06-05T06:00:00</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>['Nintendo Switch 2 players who already own the original Switch version of TAMGOTCHI PLAZA can access the exclusive content by creating the Tamagotchi Plaza Nintendo Switch 2 upgrade package.', 'TAMAGOTCHI PLAZA brings back the unique and engaging experience of the series: setting up idiosyncratic shops and serving cute characters.']</t>
+          <t>["At the moment, few highlighted Games 'Cyberpunk 2077' is one of the most striking games of Nintendo Switch 2 • Mario Kart World: In the absence of a thorough trial, and with only a first hour of play, the first big must-have of Nintendo Switch 2 is this", 'This is a game that incorporates important innovations, such as the inclusion of a great open world, and that demonstrates the leap in power compared to the original Nintendo Switch. • Nintendo Switch 2 Welcome Tour: This collection of minigames and experiences', 'It would be the typical game that comes with the console, but Nintendo has decided to charge 10 euros for it. • Cyberpunk 2077 Ultimate Edition: The ambitious futuristic adventure of CD Projekt Red is one of the most surprising games to see running on']</t>
         </is>
       </c>
       <c r="H51" t="n">
-        <v>0.7579</v>
+        <v>0.7227</v>
       </c>
       <c r="I51" t="n">
-        <v>0.137</v>
+        <v>0.096</v>
       </c>
       <c r="J51" t="n">
-        <v>0</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>DL-17c1cd3dca5a8d385d5f912ade6383f3</t>
+          <t>DL-182e127a12c29e22cad855da74591ca5</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 launches today. Here’s what to know</t>
+          <t>Zelda: Tears of the Kingdom Modded With Ray Tracing Looks Stunning in New 8K Video</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://www.wsaw.com/2025/06/05/nintendo-switch-2-launches-today-heres-what-know/</t>
+          <t>https://wccftech.com/zelda-tears-of-the-kingdom-ray-tracing-8k/</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Nintendo’s new console, the Switch 2, arrives on store shelves globally after being announced in April. Nearly all US Best Buy stores opened just after midnight to accommodate eager fans. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table.</t>
+          <t>The Legend of Zelda: Tears of the Kingdom can look stunning with some choice mods on PC, which outshine the recently released Nintendo Switch 2 edition. A new video shared a few days ago shows the latest main entry in the series running on PC via an emulator at 8K resolution with some mods.</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>1.7731247</v>
+        <v>2.6041756</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-06-05T13:46:00+00:00</t>
+          <t>2025-06-06T12:07:00+00:00</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>['In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.', 'Nintendo Switch 2 gaming devices are stored on the day Nintendo starts selling the new consoles globally, at an electronics store in Tokyo, Japan, on June 5.\nNintendo has also given the console hardware a much-needed upgrade.']</t>
+          <t>['As even an RTX 5090 has some trouble running the game at 60 FPS at such a high resolution and with these mods, it would have been unreasonable to expect such a makeover to run on the Nintendo Switch 2, so those who wish to experience the game like never', "Related Story Batman Arkham Knight, One of the Worst Nintendo Switch Ports Ever, Gets Significant Performance Boost on Nintendo Switch 2\nThe fact that The Legend of Zelda: Tears of the Kingdom on Nintendo Switch 2 doesn't feature any transformative visual"]</t>
         </is>
       </c>
       <c r="H52" t="n">
-        <v>0.8442</v>
+        <v>0.4767</v>
       </c>
       <c r="I52" t="n">
-        <v>0.171</v>
+        <v>0.093</v>
       </c>
       <c r="J52" t="n">
-        <v>0</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>DL-6b1dfb573ca972c47a35c3452e0b887c</t>
+          <t>DL-05605b9ac8551ba2df3061a3bb23d284</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>With the release of the Nintendo Switch 2, what's the future for the Switch?</t>
+          <t>My Switch 2 Review in Progress: It's Good, but Don't Give In to the FOMO Yet</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://www.gamekult.com/actualite/avec-la-sortie-de-la-nintendo-switch-2-quel-avenir-pour-la-switch-3050864092.html</t>
+          <t>https://www.cnet.com/tech/gaming/my-switch-2-review-in-progress-its-good-but-dont-give-in-to-the-fomo-yet/</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Nintendo has always shown a rigorous follow-up on its previous consoles. Examples include the 3DS, which was eligible for new features until 2019 (two years after Switch’s release), and an online store until 2023. The real question would be whether Nintendo would be willing to offer its productions on both machines at the same time.</t>
+          <t>The Nintendo Switch 2 is all anyone in gaming is talking about right now, and it could very well be the biggest gadget of 2025. By now, thousands of Switch 2 owners have one in hand as well, and the company will certainly sell thousands more this year. This clearly feels like a really good upgrade to aging Switches, but it's also not anything any current Switch owner needs to rush into.</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>1.5550461</v>
-      </c>
-      <c r="F53" t="inlineStr"/>
+        <v>2.49646</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2025-06-06T22:34:00+00:00</t>
+        </is>
+      </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>['Samus will be on both Switches A situation that is explained by Nintendo’s legacy, but also by the fact that the adoption rate of the console is probably still questionable at the moment.', 'If Nintendo has not spoken out on this issue, Kyoto is well aware that the switch 2 adoption curve is more uncertain than the first one, in the sense that consumers will be much more reluctant to switch, mainly for price reasons of course.']</t>
+          <t>["By now, thousands of Switch 2 owners have one in hand as well, and the company will certainly sell thousands more this year, especially during the holidays. So, how good is Nintendo's new console? And is it worth upgrading from the original Switch?", "I haven't had enough time to fully review the Switch 2 yet, and the Switch 2 hasn't had enough time to spread its wings and grow its game library. These are early days for Nintendo's new console, but there's some stuff I can already tell you.", "It's a simple thing, but it really makes swapping them into accessories and back into the Switch feel effortless, the way Nintendo always advertised the experience as feeling."]</t>
         </is>
       </c>
       <c r="H53" t="n">
-        <v>-0.2732</v>
+        <v>0.8443000000000001</v>
       </c>
       <c r="I53" t="n">
-        <v>0</v>
+        <v>0.177</v>
       </c>
       <c r="J53" t="n">
-        <v>0.039</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>DL-05605b9ac8551ba2df3061a3bb23d284</t>
+          <t>DL-b108c340c0dc3990b6d0f186f3c32267</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>My Switch 2 Review in Progress: It's Good, but Don't Give In to the FOMO Yet</t>
+          <t>Nintendo Switch2 India Launch On THIS Date --Check Features And Expected Price</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://www.cnet.com/tech/gaming/my-switch-2-review-in-progress-its-good-but-dont-give-in-to-the-fomo-yet/</t>
+          <t>https://zeenews.india.com/technology/nintendo-switch2-india-launch-on-this-date-check-features-and-expected-price-2911893.html</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 is all anyone in gaming is talking about right now, and it could very well be the biggest gadget of 2025. By now, thousands of Switch 2 owners have one in hand as well, and the company will certainly sell thousands more this year. This clearly feels like a really good upgrade to aging Switches, but it's also not anything any current Switch owner needs to rush into.</t>
+          <t>Nintendo Switch2 has gone out of stock globally within a day of its roll out. Priced at $499, Switch 2 comes with some major features upgrade over previous gen Switch. Switch2 is Powered by Nvidia Terga T239 chip with an octa-core ARM CORTEX- A78C CPU AND 12SM Ampere GPU. It comes with 12GB LPDDR5X RAM AND Faster loading speed.</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>1.5476952</v>
+        <v>2.270216</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-06-06T22:34:00+00:00</t>
+          <t>2025-06-06T00:00:00</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>["By now, thousands of Switch 2 owners have one in hand as well, and the company will certainly sell thousands more this year, especially during the holidays. So, how good is Nintendo's new console? And is it worth upgrading from the original Switch?", "I haven't had enough time to fully review the Switch 2 yet, and the Switch 2 hasn't had enough time to spread its wings and grow its game library. These are early days for Nintendo's new console, but there's some stuff I can already tell you.", "It's a simple thing, but it really makes swapping them into accessories and back into the Switch feel effortless, the way Nintendo always advertised the experience as feeling."]</t>
+          <t>['Priced at $499, Switch 2 comes with some major features upgrade over previous gen Switch.\nMajor Specification of Switch2\nDisplay: Nintendo Switch2 comes with larger 7.9-inch 1080p LCD touchscreen with HDR10 support and a refresh rate of 120Hz.']</t>
         </is>
       </c>
       <c r="H54" t="n">
-        <v>0.8443000000000001</v>
+        <v>0</v>
       </c>
       <c r="I54" t="n">
-        <v>0.177</v>
+        <v>0</v>
       </c>
       <c r="J54" t="n">
         <v>0</v>
@@ -2810,86 +2810,86 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>DL-f18eecd6ae1aa3953cec4cf5dcc3e634</t>
+          <t>DL-2ce32c01c084cc6ab184d989c771b28e</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>'I own a Switch 2 - this console case beats Nintendo's thanks to one main feature'</t>
+          <t>The Nintendo Switch 2 already has a flaw: its autonomy</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://www.birminghammail.co.uk/whats-on/shopping/i-switch-2-console-case-31823315</t>
+          <t>https://www.numerama.com/tech/1985971-la-nintendo-switch-2-a-deja-un-defaut-son-autonomie.html</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 is out and I was lucky enough to get my hands on the Switch 2 on release day. There are plenty of choices out there, including the official Nintendo Switch 2, which can be bought almost everywhere. Amazon lawnmower reduced from over £100 is 'lightweight' and 'easy to handle'</t>
+          <t>The console is at the level of the very first version of the Switch, dated 2017. Our first tests, with a console set to 50% brightness and 50% audio volume, are not likely to reassure those who feared the worst about Switch 2’s autonomy. Cyberpunk 2077 was first launched for half an hour: the console has been upgraded from 50% battery to 22% battery.</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>1.5207672</v>
+        <v>2.1162453</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-06-10T10:29:21+00:00</t>
+          <t>2025-06-06T08:28:24</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>["The Nintendo Switch 2 is out and in the search for a new case - I might have found my top choice thanks to one main feature\nI was lucky enough to get my hands on the Nintendo Switch 2 on release day, and it's definitely one of my favourite purchases so", "Without going into a massive review of the console, it is the definitive Switch experience, and it's exciting to see what the future holds for it."]</t>
+          <t>['I accept everything Managing my choices No miracle for Nintendo Switch 2 autonomy Your data deserves better protection. Scams, viruses and ransomware are no longer fatal.', 'If we extrapolate our little experiment (which requires repeating several times to refine), we would barely exceed the two hours of play on Cyberpunk 2077, while we could hope to reach the 3h30 on The Legend of Zelda: Breath of the Wild.', 'The Legend of Zelda: Breath of the Wild consumes a lot on Nintendo Switch 2 // Source: Nino Barbey for Numerama The choice to return to an LCD panel is really not the idea of the century, especially since its refresh rate of 120 Hz must consume more (']</t>
         </is>
       </c>
       <c r="H55" t="n">
-        <v>0.7287</v>
+        <v>-0.738</v>
       </c>
       <c r="I55" t="n">
-        <v>0.137</v>
+        <v>0.064</v>
       </c>
       <c r="J55" t="n">
-        <v>0</v>
+        <v>0.145</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>DL-518e1f4a2492da2505d9f7e5db4b46e6</t>
+          <t>DL-8eed788f4c6b98f895779a24abd5aba6</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Microsoft Launches First Portable Game Console</t>
+          <t>Nintendo Switch 2 guide: pre-order links, accessories and launch games</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://jurnalul.ro/it/tehnica/microsoft-lansare-prima-consola-jocuri-portabila-1000410.html</t>
+          <t>https://www.theshortcut.com/p/nintendo-switch-2-guide-pre-order-live</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>"Xbox Ally brings together the power offered by Xbox and the freedom offered by Windows," Bond says. The console price and exact launch dates will be announced in the coming months. Microsoft says both models evoke the brand's traditional controllers.</t>
+          <t>There are 10 tech stories in today’s Substack issue of The Shortcut Skip ahead to story 2 to 10 for more Nintendo Switch 2 is arriving at stores across the United States tonight. This is your chance to skip the line. Walmart always has more console inventory and better servers than GameStop.</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>1.5027504</v>
+        <v>1.983017</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-06-09T00:00:00</t>
+          <t>2025-06-05T03:05:04</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>['"Xbox Ally and Xbox Ally X are perfect for players who are looking for an accessible gaming experience while travelling, whether by plane or between the two comfortable indoor seats," Microsoft said in a statement, according to the AFP.', "The announcement came just days after Japan's Nintendo launched the Switch 2 portable console."]</t>
+          <t>['My personal Switch 2 pre-order from Target was delayed at the last minute. So I’m in line – with the diehard Nintendo gamers, some of whom arrived at 8am ET – hoping to secure a Switch 2 from Best Buy at midnight. Review coming soon.\nThe best part?']</t>
         </is>
       </c>
       <c r="H56" t="n">
-        <v>0.6369</v>
+        <v>0.7717000000000001</v>
       </c>
       <c r="I56" t="n">
-        <v>0.097</v>
+        <v>0.146</v>
       </c>
       <c r="J56" t="n">
         <v>0</v>
@@ -2898,262 +2898,262 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>DL-62f6feb86add6bac2ca72da8a1135b3b</t>
+          <t>DL-a693f23c7ac4e39135b5cc47d8513970</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Belkin unveils new gaming portfolio featuring power-packed charging accessories, gaming essentials</t>
+          <t>Shortly before release: Games and accessories for the Nintendo Switch 2</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://www.tahawultech.com/business/belkin-unveils-new-gaming-portfolio-featuring-power-packed-charging-accessories-gaming-essentials/</t>
+          <t>https://www.hardwareluxx.de/index.php/news/consumer-electronics/konsolen/66294-kurz-vor-dem-release-spiele-und-zubehoer-fuer-die-nintendo-switch-2.html</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Belkin is “Leveling up your play” – bringing a new level of reliability to the gaming ecosystem that differentiates through premium materials, timeless design, and in-house engineering. The new range includes elevated accessories designed to enhance the gaming experience, featuring on-the-go charging solutions, audio gear, robust screen protection, and new travel cases built for effortless portability and protection.</t>
+          <t>Nintendo Switch 2 will finally have a successor next Thursday. A new design with a larger screen and of course a more powerful hardware should make the Switch 2 a real 4K console. Some online retailers such as Amazon, MediaMarkt or Coolblue list the starting title “Mario Kart World” from 79 euros and thus 10 euros below the actual price recommendation. This also applies to "The Legend of Zelda: Tears of the Kingdom"</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>1.501461</v>
+        <v>1.9260521</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-06-06T17:45:51+00:00</t>
+          <t>2025-06-03T08:37:58</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>['Belkin’s first iteration of gaming accessories will feature products designed to be compatible with Nintendo Switch 2\nLOS ANGELES, CA – Belkin, a leading consumer electronics brand for over 40 years, today announced its entry into the gaming accessories', 'space with the launch of a new lineup designed to be compatible with the highly anticipated Nintendo Switch 2.', 'Built on decades of experience in power, connectivity and device protection, and released under Belkin’s innovation-focused Future Ventures category, this marks the company’s first collection of products tailored specifically for the gaming community.']</t>
+          <t>['Above all, you should purchase an additional memory card when buying the Nintendo Switch 2, because the integrated 256 GB could quickly become scarce. The official Nintendo SanDisk costs with 256 GB already 55 euros.', 'However, all microSD Express cards with a capacity of theoretically up to 2 TB can be used.', 'These should make data transfer rates of at least 800 MB/s possible, which in addition corresponds to the 10-fold of the predecessor and significantly restricts the selection.']</t>
         </is>
       </c>
       <c r="H57" t="n">
-        <v>0.6705</v>
+        <v>0.5849</v>
       </c>
       <c r="I57" t="n">
-        <v>0.104</v>
+        <v>0.099</v>
       </c>
       <c r="J57" t="n">
-        <v>0</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>DL-5dcc26e57d179cf942f68c4c1a43add8</t>
+          <t>DL-bc0bf2ef431589eeb38d530dce7bdf45</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: Everything to know about the price and features</t>
+          <t>Bouncemasters demo now available on Steam</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>https://abc11.com/post/nintendo-switch-2-heres-everything-need-know-price-features/16656981/</t>
+          <t>https://thatsgaming.nl/bouncemasters-demo-nu-beschikbaar-op-steam/</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>The long-awaited release of the Nintendo Switch 2 is set to arrive early Thursday morning. Here's what to know about the hype behind the Switch 2, the key features of the gaming system and how to buy it. Online pre-orders are largely sold out but gamers can purchase a limited in-store supply starting at 12:01 a.m. ET on Thursday. The Nintendo Switch has sold more than 152 million consoles.</t>
+          <t>Bouncemasters is a fun physics-based arcade game inspired by Yetisports. The full version comes out on Steam in the third quarter of 2025. TAMAGOTCHI PLAZA is coming to the Nintendo Switch 2 and Nintendo Switch 2. Both versions will be compatible with the Tamagotchi Uni device.</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>1.4305553</v>
+        <v>1.8323231</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-06-05T16:14:46</t>
+          <t>2025-06-06T18:57:55+00:00</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>['The price of the Nintendo Switch 2 in the U.S. is $449.99, while a bundle that includes "Mario Kart World" runs $499.99.\nThat price remains unchanged by Trumps tariffs, the Japan-based gaming giant said in April.', '"Nintendo Switch 2 accessories will experience price adjustments from those announced on April 2 due to changes in market conditions," the company said.', '"Other adjustments to the price of any Nintendo product are also possible in the future depending on market conditions."']</t>
+          <t>['Nintendo Switch 2 players who already own the original Switch version of TAMGOTCHI PLAZA can access the exclusive content by creating the Tamagotchi Plaza Nintendo Switch 2 upgrade package.', 'TAMAGOTCHI PLAZA brings back the unique and engaging experience of the series: setting up idiosyncratic shops and serving cute characters.']</t>
         </is>
       </c>
       <c r="H58" t="n">
-        <v>-0.34</v>
+        <v>0.7579</v>
       </c>
       <c r="I58" t="n">
-        <v>0</v>
+        <v>0.137</v>
       </c>
       <c r="J58" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>DL-a77fb4dd359d5198b3f658382e12f176</t>
+          <t>DL-17c1cd3dca5a8d385d5f912ade6383f3</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>These Nintendo Switch 2 Edition upgrades can keep you from breaking the bank</t>
+          <t>The Nintendo Switch 2 launches today. Here’s what to know</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://www.pockettactics.com/nintendo-switch/switch-2-edition-upgrades</t>
+          <t>https://www.wsaw.com/2025/06/05/nintendo-switch-2-launches-today-heres-what-know/</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>I picked up the Nintendo Switch 2 yesterday, losing many hours already to the likes of Mario Kart World and Cyberpunk 2077. On top of the price of the console itself, it'll cost you $1.2k to buy all of the Switch 2 launch games. If you do have those two excellent RPGs, you can actually upgrade them to their Switch 2 versions for free. I'm thrilled to see Pokémon Scarlet and Violet get one.</t>
+          <t>Nintendo’s new console, the Switch 2, arrives on store shelves globally after being announced in April. Nearly all US Best Buy stores opened just after midnight to accommodate eager fans. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table.</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>1.3596745</v>
+        <v>1.7731934</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-06-06T17:42:06</t>
+          <t>2025-06-05T13:46:00+00:00</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>['Looking to the future, it appears as though Nintendo is partial to Switch 2 upgrades, just like Xbox and PlayStation with their respective games and consoles, as one of the best Mario Party games, Super Mario Party Jamboree – Nintendo Switch 2 Edition', 'With an upgrade price of $19.99, you can enjoy Kirby and the Forgotten Land Switch 2 Edition. Better still, this comes with the Star-Crossed World DLC, giving you something completely new to experience as you revisit this fun Kirby adventure.', "While I already have a Nintendo Switch 2, I do like knowing that people who don't intend to pick it up just yet – perhaps even for a couple of years – have a reasonable option to upgrade some new Switch games they do buy between now and then, with other"]</t>
+          <t>['In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.', 'Nintendo Switch 2 gaming devices are stored on the day Nintendo starts selling the new consoles globally, at an electronics store in Tokyo, Japan, on June 5.\nNintendo has also given the console hardware a much-needed upgrade.']</t>
         </is>
       </c>
       <c r="H59" t="n">
-        <v>0.8979</v>
+        <v>0.8442</v>
       </c>
       <c r="I59" t="n">
-        <v>0.181</v>
+        <v>0.171</v>
       </c>
       <c r="J59" t="n">
-        <v>0.032</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>DL-2ce32c01c084cc6ab184d989c771b28e</t>
+          <t>DL-48f470a3b04e45099a9bd8f8b9d0942b</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 already has a flaw: its autonomy</t>
+          <t>What comes in the box of the Nintendo Switch 2? Look at the unboxing of the console, the Pro Controller and the camera.</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://www.numerama.com/tech/1985971-la-nintendo-switch-2-a-deja-un-defaut-son-autonomie.html</t>
+          <t>https://www.tecmundo.com.br/voxel/501558-o-que-vem-na-caixa-do-nintendo-switch-2-confira-unboxing-do-console-pro-controller-e-camera.htm</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>The console is at the level of the very first version of the Switch, dated 2017. Our first tests, with a console set to 50% brightness and 50% audio volume, are not likely to reassure those who feared the worst about Switch 2’s autonomy. Cyberpunk 2077 was first launched for half an hour: the console has been upgraded from 50% battery to 22% battery.</t>
+          <t>Derek Keller introduces the new model of the Big N, which brings a series of innovations over the first Switch. The new model accompanies the game Mario Kart World, one of the launch titles of the new console. In addition to highlighting the visual and functional changes, the video also reveals technical details and curiosities about the accessories.</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>1.3132324</v>
+        <v>1.7010574</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-06-06T08:28:24</t>
+          <t>2025-06-05T21:33:00+00:00</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>['I accept everything Managing my choices No miracle for Nintendo Switch 2 autonomy Your data deserves better protection. Scams, viruses and ransomware are no longer fatal.', 'If we extrapolate our little experiment (which requires repeating several times to refine), we would barely exceed the two hours of play on Cyberpunk 2077, while we could hope to reach the 3h30 on The Legend of Zelda: Breath of the Wild.', 'The Legend of Zelda: Breath of the Wild consumes a lot on Nintendo Switch 2 // Source: Nino Barbey for Numerama The choice to return to an LCD panel is really not the idea of the century, especially since its refresh rate of 120 Hz must consume more (']</t>
+          <t>['In addition to highlighting the visual and functional changes to the device, the video also reveals technical details and curiosities about the accessories, paving the way for the upcoming full reviews that will soon be available on the Voxel channel', "More compact box and redesigned design One of the first noticeable changes on the Nintendo Switch 2 is the new packaging format. Even though it's a physically larger console, the box has been optimized and it's more compact and organized."]</t>
         </is>
       </c>
       <c r="H60" t="n">
-        <v>-0.738</v>
+        <v>0</v>
       </c>
       <c r="I60" t="n">
-        <v>0.064</v>
+        <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>0.145</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>DL-f93e2da6e1d3e279a286496afdb81d0a</t>
+          <t>DL-56a2f5145d0be40c3efde1b4a27402f4</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>I Can't Believe How Much Easier Voice Chat Is on the Switch 2</t>
+          <t>Nintendo Switch 2: The LCD screen receives fierce criticism from fans and experts - and we too would have liked a different display</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://au.pcmag.com/gaming-systems/111364/i-cant-believe-how-much-easier-voice-chat-is-on-the-switch-2</t>
+          <t>https://www.gamepro.de/artikel/nintendo-switch-2-lcd-bildschirm-erntet-heftige-kritik,3434354.html</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>The Switch 2 promises one of the company’s most ambitious online features yet with GameChat. I tested it before launch to see how Nintendo uses cameras and microphones to turn online gaming into a more fun, welcoming experience. Nintendo Switch 2 should support most USB-C webcams, even those with lower resolutions.</t>
+          <t>Switch 2 is out and despite many new display features there is some strong criticism, both from fans and tech enthusiasts. We have therefore looked into it ourselves and also measured it, and we are also disenchanted. The LCD display from the Taiwanese manufacturer InnoLux brings some great functions – for example HDR for higher color dynamics, 120 Hertz and VRR – but also disappoints massively in some central points.</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>1.2323608</v>
+        <v>1.5776062</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-06-03T14:12:48+00:00</t>
+          <t>2025-06-08T17:30:00</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>["The Switch 2 promises one of the company’s most ambitious online features yet with GameChat, which is the system's new online communication system.", 'I tested it before launch to see how Nintendo uses cameras and microphones to turn online gaming into a more fun, welcoming experience.', "GameChat is so baked into the Switch 2 experience that there's a dedicated button for it on the Joy-Con controllers. Pressing the new C button launches the GameChat menu that lets you create a lobby or see which friends are online and ready to play."]</t>
+          <t>['Until a pixel is switched to another color, it takes a while, and the resulting image artifacts are perceived as ghosting or blurring.', 'And in this respect, the Switch 2 display with its 120 Hertz is particularly vulnerable, as many buyers write in the comments below the post. How do we rate the display of the Nintendo Switch 2?']</t>
         </is>
       </c>
       <c r="H61" t="n">
-        <v>0.9226</v>
+        <v>0.1531</v>
       </c>
       <c r="I61" t="n">
-        <v>0.264</v>
+        <v>0.108</v>
       </c>
       <c r="J61" t="n">
-        <v>0.038</v>
+        <v>0.073</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>DL-b108c340c0dc3990b6d0f186f3c32267</t>
+          <t>DL-518e1f4a2492da2505d9f7e5db4b46e6</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Nintendo Switch2 India Launch On THIS Date --Check Features And Expected Price</t>
+          <t>Microsoft Launches First Portable Game Console</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://zeenews.india.com/technology/nintendo-switch2-india-launch-on-this-date-check-features-and-expected-price-2911893.html</t>
+          <t>https://jurnalul.ro/it/tehnica/microsoft-lansare-prima-consola-jocuri-portabila-1000410.html</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Nintendo Switch2 has gone out of stock globally within a day of its roll out. Priced at $499, Switch 2 comes with some major features upgrade over previous gen Switch. Switch2 is Powered by Nvidia Terga T239 chip with an octa-core ARM CORTEX- A78C CPU AND 12SM Ampere GPU. It comes with 12GB LPDDR5X RAM AND Faster loading speed.</t>
+          <t>"Xbox Ally brings together the power offered by Xbox and the freedom offered by Windows," Bond says. The console price and exact launch dates will be announced in the coming months. Microsoft says both models evoke the brand's traditional controllers.</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>1.2009792</v>
+        <v>1.504303</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-06-06T00:00:00</t>
+          <t>2025-06-09T00:00:00</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>['Priced at $499, Switch 2 comes with some major features upgrade over previous gen Switch.\nMajor Specification of Switch2\nDisplay: Nintendo Switch2 comes with larger 7.9-inch 1080p LCD touchscreen with HDR10 support and a refresh rate of 120Hz.']</t>
+          <t>['"Xbox Ally and Xbox Ally X are perfect for players who are looking for an accessible gaming experience while travelling, whether by plane or between the two comfortable indoor seats," Microsoft said in a statement, according to the AFP.', "The announcement came just days after Japan's Nintendo launched the Switch 2 portable console."]</t>
         </is>
       </c>
       <c r="H62" t="n">
-        <v>0</v>
+        <v>0.6369</v>
       </c>
       <c r="I62" t="n">
-        <v>0</v>
+        <v>0.097</v>
       </c>
       <c r="J62" t="n">
         <v>0</v>
@@ -3162,170 +3162,174 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>DL-201b8ebcf779d686eb6aa318af25eaa9</t>
+          <t>DL-62f6feb86add6bac2ca72da8a1135b3b</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Launched sales of Nintendo Switch 2 - in which countries the console is available</t>
+          <t>Belkin unveils new gaming portfolio featuring power-packed charging accessories, gaming essentials</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>https://games.24tv.ua/ru/startovali-prodazhi-nintendo-switch-2-v-kakih-stranah-dostupna-konsol-games_n2839620/amp</t>
+          <t>https://www.tahawultech.com/business/belkin-unveils-new-gaming-portfolio-featuring-power-packed-charging-accessories-gaming-essentials/</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Nintendo decided to seriously oppose speculators who traditionally buy consoles for resale at an inflated price. Fans began to take seats in queues a few hours before the opening of the stores. Some even took a break from work to buy a novelty.</t>
+          <t>Belkin is “Leveling up your play” – bringing a new level of reliability to the gaming ecosystem that differentiates through premium materials, timeless design, and in-house engineering. The new range includes elevated accessories designed to enhance the gaming experience, featuring on-the-go charging solutions, audio gear, robust screen protection, and new travel cases built for effortless portability and protection.</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>1.0896988</v>
-      </c>
-      <c r="F63" t="inlineStr"/>
+        <v>1.5023041</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>2025-06-06T17:45:51+00:00</t>
+        </is>
+      </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>['It should be noted that neither in Ukraine nor in Russia Nintendo products are officially sold. On the eve of Nvidia CEO Jensen Huang said that Switch 2 will receive special AI processors that improve the gaming experience in real time.']</t>
+          <t>['Belkin’s first iteration of gaming accessories will feature products designed to be compatible with Nintendo Switch 2\nLOS ANGELES, CA – Belkin, a leading consumer electronics brand for over 40 years, today announced its entry into the gaming accessories', 'space with the launch of a new lineup designed to be compatible with the highly anticipated Nintendo Switch 2.', 'Built on decades of experience in power, connectivity and device protection, and released under Belkin’s innovation-focused Future Ventures category, this marks the company’s first collection of products tailored specifically for the gaming community.']</t>
         </is>
       </c>
       <c r="H63" t="n">
-        <v>-0.1779</v>
+        <v>0.6705</v>
       </c>
       <c r="I63" t="n">
-        <v>0</v>
+        <v>0.104</v>
       </c>
       <c r="J63" t="n">
-        <v>0.042</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>DL-9403699c5a8c3acb6752501c45ccc38e</t>
+          <t>DL-5dcc26e57d179cf942f68c4c1a43add8</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 – Release brings 20 games directly</t>
+          <t>Nintendo Switch 2: Everything to know about the price and features</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://www.toptechnews.de/2025/06/05/nintendo-switch-2-release-bringt-direkt-20-spiele-mit-sich/</t>
+          <t>https://abc11.com/post/nintendo-switch-2-heres-everything-need-know-price-features/16656981/</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2, Mario Kart World and more than 20 other titles are now available. Nintendo Switch 2 is the first new Nintendo console to be released since the introduction of Nintendo Switch eight years ago. The new Joy-Con 2 controllers are magnetically attached to the console and can be operated like a mouse by sliding them on a surface.</t>
+          <t>The long-awaited release of the Nintendo Switch 2 is set to arrive early Thursday morning. Here's what to know about the hype behind the Switch 2, the key features of the gaming system and how to buy it. Online pre-orders are largely sold out but gamers can purchase a limited in-store supply starting at 12:01 a.m. ET on Thursday. The Nintendo Switch has sold more than 152 million consoles.</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>1.0810337</v>
+        <v>1.4306087</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-06-05T15:28:24+00:00</t>
+          <t>2025-06-05T16:14:46</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>['If a compatible USB-C camera, such as the Nintendo Switch 2 camera (available separately), is connected, up to four people can also communicate with each other via video chat.', 'To optimize the gaming experience of Nintendo Switch titles on Nintendo Switch 2, there will be free updates for selected games that improve graphics or add new features, for example.2 The content of the free updates varies by game.', 'Sid Meier’s Civilization® VII – Nintendo Switch 2 Edition: Players can now influence the course of history on Nintendo Switch 2.']</t>
+          <t>['The price of the Nintendo Switch 2 in the U.S. is $449.99, while a bundle that includes "Mario Kart World" runs $499.99.\nThat price remains unchanged by Trumps tariffs, the Japan-based gaming giant said in April.', '"Nintendo Switch 2 accessories will experience price adjustments from those announced on April 2 due to changes in market conditions," the company said.', '"Other adjustments to the price of any Nintendo product are also possible in the future depending on market conditions."']</t>
         </is>
       </c>
       <c r="H64" t="n">
-        <v>0.743</v>
+        <v>-0.34</v>
       </c>
       <c r="I64" t="n">
-        <v>0.106</v>
+        <v>0</v>
       </c>
       <c r="J64" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>DL-90b89c57db6bd0dda29585ae2b322970</t>
+          <t>DL-a77fb4dd359d5198b3f658382e12f176</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Switch 2 is important for Nintendo, but also for a Nvidia that does not want to lose ground against AMD.</t>
+          <t>These Nintendo Switch 2 Edition upgrades can keep you from breaking the bank</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>https://www.xataka.com/videojuegos/switch-2-importante-para-nintendo-tambien-para-nvidia-que-no-quiere-perder-terreno-amd</t>
+          <t>https://www.pockettactics.com/nintendo-switch/switch-2-edition-upgrades</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 returns to the load When a leading company, what it wants is to have even more part of the cake. Nvidia dominates the world of PC video games with an iron hand. AMD is doing well with its latest generations, but the singing voice is still carried by the company led by Jensen Huang.</t>
+          <t>I picked up the Nintendo Switch 2 yesterday, losing many hours already to the likes of Mario Kart World and Cyberpunk 2077. On top of the price of the console itself, it'll cost you $1.2k to buy all of the Switch 2 launch games. If you do have those two excellent RPGs, you can actually upgrade them to their Switch 2 versions for free. I'm thrilled to see Pokémon Scarlet and Violet get one.</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>1.0760536</v>
+        <v>1.3605194</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-06-06T21:47:33+00:00</t>
+          <t>2025-06-06T17:42:06</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>['Nintendo Switch 2 is here.', 'When a new generation of consoles arrives, beyond the new games and experiences it enables, there is a fundamental issue that may not be of much interest to all users, but is of vital importance to the technology industry: who signs the processor.']</t>
+          <t>['Looking to the future, it appears as though Nintendo is partial to Switch 2 upgrades, just like Xbox and PlayStation with their respective games and consoles, as one of the best Mario Party games, Super Mario Party Jamboree – Nintendo Switch 2 Edition', 'With an upgrade price of $19.99, you can enjoy Kirby and the Forgotten Land Switch 2 Edition. Better still, this comes with the Star-Crossed World DLC, giving you something completely new to experience as you revisit this fun Kirby adventure.', "While I already have a Nintendo Switch 2, I do like knowing that people who don't intend to pick it up just yet – perhaps even for a couple of years – have a reasonable option to upgrade some new Switch games they do buy between now and then, with other"]</t>
         </is>
       </c>
       <c r="H65" t="n">
-        <v>0.4118</v>
+        <v>0.8979</v>
       </c>
       <c r="I65" t="n">
-        <v>0.08400000000000001</v>
+        <v>0.181</v>
       </c>
       <c r="J65" t="n">
-        <v>0</v>
+        <v>0.032</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>DL-8eed788f4c6b98f895779a24abd5aba6</t>
+          <t>DL-4de785c3d00dac3779286d8e34763c81</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 guide: pre-order links, accessories and launch games</t>
+          <t>How to Transfer Your Switch Data to Nintendo Switch 2</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>https://www.theshortcut.com/p/nintendo-switch-2-guide-pre-order-live</t>
+          <t>https://www.iphoneincanada.ca/2025/06/05/how-to-transfer-your-data-nintendo-switch-2/</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>There are 10 tech stories in today’s Substack issue of The Shortcut Skip ahead to story 2 to 10 for more Nintendo Switch 2 is arriving at stores across the United States tonight. This is your chance to skip the line. Walmart always has more console inventory and better servers than GameStop.</t>
+          <t>Nintendo provides a streamlined way to conduct a system transfer from Nintendo Switch to the Switch 2. Players can transfer profile data, save data, screenshots or video, and system settings. Nintendo notes that there is an expiry date for all system transfer data.</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>1.0605202</v>
+        <v>1.3527374</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-06-05T03:05:04</t>
+          <t>2025-06-05T11:06:10+00:00</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>['My personal Switch 2 pre-order from Target was delayed at the last minute. So I’m in line – with the diehard Nintendo gamers, some of whom arrived at 8am ET – hoping to secure a Switch 2 from Best Buy at midnight. Review coming soon.\nThe best part?']</t>
+          <t>['By selecting ‘ I Don’t Have a Nintendo Switch 2 Yet’, you can upload your data to Nintendo’s servers in anticipation of when your Nintendo Switch 2 arrives.', 'Follow the on-screen prompts until you’re sent a ‘Verification code’ to your My Nintendo account email address. Input the code and select ‘Send Data to the Server’. This will then upload your save data to Nintendo’s cloud servers.', 'Once the upload is complete, you can review the system transfer information and select ‘Start Restoring Factory Settings’ to complete the process. Note: This will delete all data from the original console.']</t>
         </is>
       </c>
       <c r="H66" t="n">
-        <v>0.7717000000000001</v>
+        <v>0.4939</v>
       </c>
       <c r="I66" t="n">
-        <v>0.146</v>
+        <v>0.076</v>
       </c>
       <c r="J66" t="n">
         <v>0</v>
@@ -3334,86 +3338,86 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>DL-cbe41ea394a2ced64f8f9324991f8418</t>
+          <t>DL-1f7196f9804c69956dd1ea78f94a50cf</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Osceola County Sheriff Lopez to make first court appearance after facing federal charges</t>
+          <t>Switch 2: Why Nintendo doesn't want you to remove the display slide</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>https://spotonflorida.com/central-florida/5775312/osceola-county-sheriff-lopez-to-make.html</t>
+          <t>https://t3n.de/news/switch-2-nintendo-display-folie-1691041/</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Sheriff Marcos Lopez has been booked at Lake County Jail without bond. Over 250,000 pay homage to Pope Francis as world leaders prepare to attend funeral.</t>
+          <t>On June 5, 2025, the new Nintendo console Switch 2 will officially go on sale. Pre-ordering is currently not possible on major online trading platforms. It is currently unknown when the console will be available again. Nintendo explicitly warns against removing the factory-mounted display slide.</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>1.0512486</v>
+        <v>1.3452911</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-06-06T14:15:38+00:00</t>
+          <t>2025-06-04T11:45:37</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>['Environment Day\n09:49 Disneyland ride shuts down after car derails off track: Witness\n08:35 Ex-GOP congressman David Jolly launches Democratic run for Florida governor (Video)\n08:35 Tavares residents concerned over proposed mixed-use development (Video)\n08:35 Experience', "Kissimmee aims to boost visitors through 'gastro tourism,' value-focused vacations (Video)\n08:35 The Morning News | Live Central Florida headlines, weather and traffic (Video)\n08:34 Gamers camp out for Nintendo Switch 2 (Video)\n08:34 Are traffic control"]</t>
+          <t>['Switch 2 is supposed to get new charging mode Nintendo is supposed to have found a solution for this with the Switch 2 – namely a battery-saving charging mode as usual with smartphones.', "View 8 images This retro technology has collector's value today Source: More on this topic MIT Technology Review Nintendo"]</t>
         </is>
       </c>
       <c r="H67" t="n">
-        <v>-0.2969</v>
+        <v>-0.1027</v>
       </c>
       <c r="I67" t="n">
-        <v>0.048</v>
+        <v>0</v>
       </c>
       <c r="J67" t="n">
-        <v>0.093</v>
+        <v>0.032</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>DL-f75243e86744d36c28e7960ee772b4c0</t>
+          <t>DL-c7b1d654f43bf3a0aede5a40cc6ebaca</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Microsoft unveils Xbox gaming handheld launching in 2025 (updated with hands-on)</t>
+          <t>You probably don't have this Switch 2 launch title on your screen and it comes with a pretty cool co-op feature</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>https://venturebeat.com/business/microsoft-unveils-xbox-gaming-handheld-launching-in-2025/</t>
+          <t>https://www.gamepro.de/artikel/nintendo-switch-2-gameshare-survival-kids,3434002.html</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Microsoft is diving into the handheld gaming market with its own Xbox-branded handheld in partnership with PC maker Asus. It has the Windows OS, a full Xbox screen experience, and Armoury Crate SE as a central hub for device management. The handheld will compete with rivals such as the Nintendo Switch 2 and the Valve Steam Deck.</t>
+          <t>This week, Nintendo Switch 2 comes out with a whole series of launch titles that you can play directly on the new console on June 5th. This includes Survival Kids, which besides Mario Kart World or Donkey Kong flies rather under the radar. You take on the role of four children who are stranded on an island and explore crafts and the surroundings to find a way home.</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>1.0158577</v>
+        <v>1.2888756</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-06-08T20:53:17+00:00</t>
+          <t>2025-06-03T11:27:17+00:00</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>['“The Xbox experience grows with you,” said Sarah Bond, president of Xbox, in the Xbox Showcase.\nThe company plans to launch the handheld in 2025. As such, it will compete with rivals such as the Nintendo Switch 2 and the Valve Steam Deck.', 'This one promises the power of an Xbox experience in your hands. It has a seven-inch IPS VRR screen.\nThe move could inspire both fear and derision, as the prospect for such a move has done in the past.']</t>
+          <t>['So you can play locally on a total of three devices as long as at least one person in the group has a Nintendo Switch 2 and the game supports GameShare. In the case of Survival Kids, the game runs via GameShare with two consoles for both in 60 fps.', 'On the other hand, if you start on three devices, the frame rate is reduced to 30 fps for everyone involved. Nevertheless, this way of playing together is a cool thing that has a lot of potential.']</t>
         </is>
       </c>
       <c r="H68" t="n">
-        <v>0.0772</v>
+        <v>0.34</v>
       </c>
       <c r="I68" t="n">
-        <v>0.024</v>
+        <v>0.036</v>
       </c>
       <c r="J68" t="n">
         <v>0</v>
@@ -3422,174 +3426,174 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>DL-1c59b6df7e032db28024c576f73acce5</t>
+          <t>DL-0baa3766bc883eba68c2dbbae1038cce</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>It started - Switch 2 with the first technical problems. Difficulties when downloading Mario Kart World</t>
+          <t>Donkey Kong Bananza: Release date, trailer and highlights</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>https://www.gram.pl/news/zaczelo-sie-switch-2-z-pierwszymi-problemami-technicznymi-utrudnienia-przy-pobieraniu-mario-kart-world</t>
+          <t>https://www.netcost-security.fr/mobilite/252228/donkey-kong-bananza-date-de-sortie-bande-annonce-et-exclusivites-eclairantes/</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Players who wanted to start their adventure with Nintendo Switch 2 reported serious problems with downloading the game. Error 2813-0171 The phrase "Mario Kart World doesn't want to be downloaded" quickly began to dominate search engines and forums. The source of the problem may be differences in console boot packages.</t>
+          <t>The Nintendo Switch 2 is now available with an exciting set of new games. Donkey Kong Bonanza is a must-see for fans of the iconic character. Discover key details, including the release date and pre-command options.</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>1.0081596</v>
+        <v>1.2868042</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-06-06T10:10:00</t>
+          <t>2025-06-06T16:22:33+00:00</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>['Users who purchased Nintendo Switch 2 with Mario Kart World graphics printed directly on the box have problems activating the game.', 'In turn, people who purchased the version with the attached sticker and download code, seem not to experience difficulties. GramTV reports: This is confirmed by reports from the USA.']</t>
+          <t>['To make the Switch 2 more attractive, Nintendo has released a number of games compatible only with this console. One of the games in question is a new title with Donkey Kong.', 'We will review the details of the new game, the release date of Donkey Kong Bonanza, the price, the pre-order options and the gameplay. Note that this game is only available for the Nintendo Switch 2.']</t>
         </is>
       </c>
       <c r="H69" t="n">
-        <v>-0.743</v>
+        <v>0.4939</v>
       </c>
       <c r="I69" t="n">
-        <v>0.065</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="J69" t="n">
-        <v>0.196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>DL-a693f23c7ac4e39135b5cc47d8513970</t>
+          <t>DL-fb44e9ba1c36059416a5f81b3d4717bc</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Shortly before release: Games and accessories for the Nintendo Switch 2</t>
+          <t>Nintendo Switch 2 is here - first impressions</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>https://www.hardwareluxx.de/index.php/news/consumer-electronics/konsolen/66294-kurz-vor-dem-release-spiele-und-zubehoer-fuer-die-nintendo-switch-2.html</t>
+          <t>https://www.gram.pl/artykul/nintendo-switch-2-juz-tu-jest-pierwsze-wrazenia</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 will finally have a successor next Thursday. A new design with a larger screen and of course a more powerful hardware should make the Switch 2 a real 4K console. Some online retailers such as Amazon, MediaMarkt or Coolblue list the starting title “Mario Kart World” from 79 euros and thus 10 euros below the actual price recommendation. This also applies to "The Legend of Zelda: Tears of the Kingdom"</t>
+          <t>Nintendo Switch 2 is one of my favorite consoles, which has accompanied me in various roles for over eight years. The first Switch was with me until the release of the OLED version in 2021. I forgave myself for Lite, because it did not correspond to my preferences of playing mainly on TV.</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>1.0046387</v>
+        <v>1.2802124</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-06-03T08:37:58</t>
+          <t>2025-06-07T19:00:00</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>['Above all, you should purchase an additional memory card when buying the Nintendo Switch 2, because the integrated 256 GB could quickly become scarce. The official Nintendo SanDisk costs with 256 GB already 55 euros.', 'However, all microSD Express cards with a capacity of theoretically up to 2 TB can be used.', 'These should make data transfer rates of at least 800 MB/s possible, which in addition corresponds to the 10-fold of the predecessor and significantly restricts the selection.']</t>
+          <t>['But when the long-awaited Switch 2 appeared on the horizon, placing a pre-release order was obvious.', 'I will immediately point out that this text is not a racial review of the equipment, but rather an impression, a collection of first impressions and thoughts about the new Nintendo toy.', 'Nintendo Switch 2 is a console that can be labeled the “new generation”, and at the same time it is very strongly rooted in what the first Switch accustomed us to. More a subdued but significant evolution than a surprising revolution.']</t>
         </is>
       </c>
       <c r="H70" t="n">
-        <v>0.5849</v>
+        <v>0.7351</v>
       </c>
       <c r="I70" t="n">
-        <v>0.099</v>
+        <v>0.133</v>
       </c>
       <c r="J70" t="n">
-        <v>0.028</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>DL-616a7e8681b35c912aff6ad9ed350a31</t>
+          <t>DL-194cd17a14f69417b82c9c6d47023133</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 launches today. Here's what to know</t>
+          <t>High demand makes Nintendo Switch 2 sell out in Brazil on its first day of release.</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>https://www.erienewsnow.com/story/52829208/the-nintendo-switch-2-launches-today-heres-what-to-know</t>
+          <t>https://www1.folha.uol.com.br/tec/2025/06/alta-demanda-faz-nintendo-switch-2-esgotar-no-brasil-no-primeiro-dia-de-vendas.shtml</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Nintendo's new console, the Switch 2, arrives on store shelves globally after being announced in April. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table; or on. TV when plugged in to its accompanying dock, like its predecessor. Nintendo’s decision to stick with a winning template for the Switch 2 is a testament to the original’s popularity.</t>
+          <t>Nintendo Switch 2, a new video game console from the Japanese company, went off the shelf this Friday in the global markets. It's already sold out in major Brazilian stores due to high demand. The console has a suggested price of R$4,499.90 in the standard version, no games.</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>0.9118271</v>
+        <v>1.2787685</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-06-05T13:22:00+00:00</t>
+          <t>2025-06-05T21:23:16+00:00</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>['In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.\nNintendo has also given the console hardware a much-needed upgrade.', 'The Switch 2 has a larger 7.9-inch display compared to the original Switch’s 6.2-inch screen, and the Joy-Cons now snap to the console magnetically, which should make them easier to attach or remove from the console.']</t>
+          <t>['Ampere predicts that Switch 2 sales will surpass 100 million units by 2030. See more about the Nintendo Switch 2.', 'Novelties The new console will have an improved 7.9-inch LCD screen, with HDR support and refresh rates of up to 120 Hz, ensuring smoother display.']</t>
         </is>
       </c>
       <c r="H71" t="n">
-        <v>0.9136</v>
+        <v>-0.4019</v>
       </c>
       <c r="I71" t="n">
-        <v>0.194</v>
+        <v>0</v>
       </c>
       <c r="J71" t="n">
-        <v>0</v>
+        <v>0.081</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>DL-736adae141649efa336e9f7ce03ea527</t>
+          <t>DL-9403699c5a8c3acb6752501c45ccc38e</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 launches today. Here’s what to know</t>
+          <t>Nintendo Switch 2 – Release brings 20 games directly</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>https://localnews8.com/money/cnn-business-consumer/2025/06/05/the-nintendo-switch-2-launches-today-heres-what-to-know/</t>
+          <t>https://www.toptechnews.de/2025/06/05/nintendo-switch-2-release-bringt-direkt-20-spiele-mit-sich/</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Nintendo's new console, the Switch 2, arrives on store shelves globally after being announced in April. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table; or on. a TV when plugged in to its accompanying dock, like its predecessor. Nintendo’s decision to stick with a winning template for the Switch 2 is a testament to the original’s popularity.</t>
+          <t>Nintendo Switch 2, Mario Kart World and more than 20 other titles are now available. Nintendo Switch 2 is the first new Nintendo console to be released since the introduction of Nintendo Switch eight years ago. The new Joy-Con 2 controllers are magnetically attached to the console and can be operated like a mouse by sliding them on a surface.</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>0.9118271</v>
+        <v>1.2504692</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-06-05T13:14:10</t>
+          <t>2025-06-05T15:28:24+00:00</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>['In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.\nNintendo has also given the console hardware a much-needed upgrade.', 'The Switch 2 has a larger 7.9-inch display compared to the original Switch’s 6.2-inch screen, and the Joy-Cons now snap to the console magnetically, which should make them easier to attach or remove from the console.']</t>
+          <t>['If a compatible USB-C camera, such as the Nintendo Switch 2 camera (available separately), is connected, up to four people can also communicate with each other via video chat.', 'To optimize the gaming experience of Nintendo Switch titles on Nintendo Switch 2, there will be free updates for selected games that improve graphics or add new features, for example.2 The content of the free updates varies by game.', 'Sid Meier’s Civilization® VII – Nintendo Switch 2 Edition: Players can now influence the course of history on Nintendo Switch 2.']</t>
         </is>
       </c>
       <c r="H72" t="n">
-        <v>0.9136</v>
+        <v>0.743</v>
       </c>
       <c r="I72" t="n">
-        <v>0.194</v>
+        <v>0.106</v>
       </c>
       <c r="J72" t="n">
         <v>0</v>
@@ -3598,174 +3602,170 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>DL-876ccd4580e6106d2c30aa8425da537a</t>
+          <t>DL-f93e2da6e1d3e279a286496afdb81d0a</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 launches today. Here’s what to know</t>
+          <t>I Can't Believe How Much Easier Voice Chat Is on the Switch 2</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>https://ustimesmirror.com/the-nintendo-switch-2-launches-today-heres-what-to-know/</t>
+          <t>https://au.pcmag.com/gaming-systems/111364/i-cant-believe-how-much-easier-voice-chat-is-on-the-switch-2</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Nintendo's new console, the Switch 2, arrives on store shelves globally. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table. Nintendo’s decision to stick with a winning template for the Switch 2 is a testament to the original’s popularity but also a gamble that its success will endure.</t>
+          <t>The Switch 2 promises one of the company’s most ambitious online features yet with GameChat. I tested it before launch to see how Nintendo uses cameras and microphones to turn online gaming into a more fun, welcoming experience. Nintendo Switch 2 should support most USB-C webcams, even those with lower resolutions.</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>0.9118271</v>
+        <v>1.2323341</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-06-05T15:15:59+00:00</t>
+          <t>2025-06-03T14:12:48+00:00</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>['The Switch 2 iterates its predecessor with several new features, including a Game Chat function that lets gamers communicate with other players by tapping a button on the console.', 'In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.\nNintendo has also given the console hardware a much-needed upgrade.']</t>
+          <t>["The Switch 2 promises one of the company’s most ambitious online features yet with GameChat, which is the system's new online communication system.", 'I tested it before launch to see how Nintendo uses cameras and microphones to turn online gaming into a more fun, welcoming experience.', "GameChat is so baked into the Switch 2 experience that there's a dedicated button for it on the Joy-Con controllers. Pressing the new C button launches the GameChat menu that lets you create a lobby or see which friends are online and ready to play."]</t>
         </is>
       </c>
       <c r="H73" t="n">
-        <v>0.8922</v>
+        <v>0.9226</v>
       </c>
       <c r="I73" t="n">
-        <v>0.212</v>
+        <v>0.264</v>
       </c>
       <c r="J73" t="n">
-        <v>0</v>
+        <v>0.038</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>DL-58363b4cfde0e0889c7251f2961ae5ee</t>
+          <t>DL-876ccd4580e6106d2c30aa8425da537a</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 : a promising new breath despite some disillusionment</t>
+          <t>The Nintendo Switch 2 launches today. Here’s what to know</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>https://s2pmag.ch/avis-la-nintendo-switch-2-un-nouveau-souffle-prometteur-malgre-quelques-desillusions/</t>
+          <t>https://ustimesmirror.com/the-nintendo-switch-2-launches-today-heres-what-to-know/</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 has finally slipped into our hands. What lessons can we learn from these first moments of ownership? A complete and careful case The Switch 2 comes in a package with an almost confusing simplicity, compact dimensions that are unmistakably reminiscent of its grandmother. The console is delivered ready for use, accompanied by the necessary accessories to take full advantage of it.</t>
+          <t>Nintendo's new console, the Switch 2, arrives on store shelves globally. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table. Nintendo’s decision to stick with a winning template for the Switch 2 is a testament to the original’s popularity but also a gamble that its success will endure.</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>0.8862343</v>
+        <v>1.1889267</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-06-09T06:16:01</t>
+          <t>2025-06-05T15:15:59+00:00</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>['A balanced review, promises to be confirmed In the end, this Nintendo Switch 2 turns out to be capable of the best as well as the least good, offering contrasting experiences according to titles and usages.']</t>
+          <t>['The Switch 2 iterates its predecessor with several new features, including a Game Chat function that lets gamers communicate with other players by tapping a button on the console.', 'In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.\nNintendo has also given the console hardware a much-needed upgrade.']</t>
         </is>
       </c>
       <c r="H74" t="n">
-        <v>0.5413</v>
+        <v>0.8922</v>
       </c>
       <c r="I74" t="n">
-        <v>0.094</v>
+        <v>0.212</v>
       </c>
       <c r="J74" t="n">
-        <v>0.025</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>DL-d31952a6c00a7f14a8bb1d96ce43f30c</t>
+          <t>DL-201b8ebcf779d686eb6aa318af25eaa9</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Video games: Microsoft unveils the first portable versions of the Xbox</t>
+          <t>Launched sales of Nintendo Switch 2 - in which countries the console is available</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>https://www.lessentiel.lu/fr/story/jeux-video-microsoft-devoile-les-premieres-versions-portables-de-la-xbox-103361849</t>
+          <t>https://games.24tv.ua/ru/startovali-prodazhi-nintendo-switch-2-v-kakih-stranah-dostupna-konsol-games_n2839620/amp</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Xbox portable consoles, ROG Ally and Ally X, designed with Asus, will be marketed for the end of the year celebrations. This Twitter content cannot be displayed due to your current choice of cookies. The price of the consoles and exact date of their launch will be announced in the coming months.</t>
+          <t>Nintendo decided to seriously oppose speculators who traditionally buy consoles for resale at an inflated price. Fans began to take seats in queues a few hours before the opening of the stores. Some even took a break from work to buy a novelty.</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0.8698616</v>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>2025-06-10T09:56:00+00:00</t>
-        </is>
-      </c>
+        <v>1.089735</v>
+      </c>
+      <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr">
         <is>
-          <t>["Faced with Nintendo Switch 2 The design of both models evokes the brand's traditional handles, with the same buttons, joysticks and handles, but with a longer format to integrate a central screen.", '"Xbox Ally and Xbox Ally X are perfect for players looking for an accessible gaming experience on the go, whether between two planes or between two comfortable lounge chairs," Microsoft said in a press release.']</t>
+          <t>['It should be noted that neither in Ukraine nor in Russia Nintendo products are officially sold. On the eve of Nvidia CEO Jensen Huang said that Switch 2 will receive special AI processors that improve the gaming experience in real time.']</t>
         </is>
       </c>
       <c r="H75" t="n">
-        <v>0</v>
+        <v>-0.1779</v>
       </c>
       <c r="I75" t="n">
         <v>0</v>
       </c>
       <c r="J75" t="n">
-        <v>0</v>
+        <v>0.042</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>DL-48f470a3b04e45099a9bd8f8b9d0942b</t>
+          <t>DL-90b89c57db6bd0dda29585ae2b322970</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>What comes in the box of the Nintendo Switch 2? Look at the unboxing of the console, the Pro Controller and the camera.</t>
+          <t>Switch 2 is important for Nintendo, but also for a Nvidia that does not want to lose ground against AMD.</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>https://www.tecmundo.com.br/voxel/501558-o-que-vem-na-caixa-do-nintendo-switch-2-confira-unboxing-do-console-pro-controller-e-camera.htm</t>
+          <t>https://www.xataka.com/videojuegos/switch-2-importante-para-nintendo-tambien-para-nvidia-que-no-quiere-perder-terreno-amd</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Derek Keller introduces the new model of the Big N, which brings a series of innovations over the first Switch. The new model accompanies the game Mario Kart World, one of the launch titles of the new console. In addition to highlighting the visual and functional changes, the video also reveals technical details and curiosities about the accessories.</t>
+          <t>Nintendo Switch 2 returns to the load When a leading company, what it wants is to have even more part of the cake. Nvidia dominates the world of PC video games with an iron hand. AMD is doing well with its latest generations, but the singing voice is still carried by the company led by Jensen Huang.</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>0.79125595</v>
+        <v>1.0767269</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-06-05T21:33:00+00:00</t>
+          <t>2025-06-06T21:47:33+00:00</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>['In addition to highlighting the visual and functional changes to the device, the video also reveals technical details and curiosities about the accessories, paving the way for the upcoming full reviews that will soon be available on the Voxel channel', "More compact box and redesigned design One of the first noticeable changes on the Nintendo Switch 2 is the new packaging format. Even though it's a physically larger console, the box has been optimized and it's more compact and organized."]</t>
+          <t>['Nintendo Switch 2 is here.', 'When a new generation of consoles arrives, beyond the new games and experiences it enables, there is a fundamental issue that may not be of much interest to all users, but is of vital importance to the technology industry: who signs the processor.']</t>
         </is>
       </c>
       <c r="H76" t="n">
-        <v>0</v>
+        <v>0.4118</v>
       </c>
       <c r="I76" t="n">
-        <v>0</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="J76" t="n">
         <v>0</v>
@@ -3774,86 +3774,86 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>DL-56a2f5145d0be40c3efde1b4a27402f4</t>
+          <t>DL-cbe41ea394a2ced64f8f9324991f8418</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: The LCD screen receives fierce criticism from fans and experts - and we too would have liked a different display</t>
+          <t>Osceola County Sheriff Lopez to make first court appearance after facing federal charges</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>https://www.gamepro.de/artikel/nintendo-switch-2-lcd-bildschirm-erntet-heftige-kritik,3434354.html</t>
+          <t>https://spotonflorida.com/central-florida/5775312/osceola-county-sheriff-lopez-to-make.html</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Switch 2 is out and despite many new display features there is some strong criticism, both from fans and tech enthusiasts. We have therefore looked into it ourselves and also measured it, and we are also disenchanted. The LCD display from the Taiwanese manufacturer InnoLux brings some great functions – for example HDR for higher color dynamics, 120 Hertz and VRR – but also disappoints massively in some central points.</t>
+          <t>Sheriff Marcos Lopez has been booked at Lake County Jail without bond. Over 250,000 pay homage to Pope Francis as world leaders prepare to attend funeral.</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>0.7887001</v>
+        <v>1.0517502</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-06-08T17:30:00</t>
+          <t>2025-06-06T14:15:38+00:00</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>['Until a pixel is switched to another color, it takes a while, and the resulting image artifacts are perceived as ghosting or blurring.', 'And in this respect, the Switch 2 display with its 120 Hertz is particularly vulnerable, as many buyers write in the comments below the post. How do we rate the display of the Nintendo Switch 2?']</t>
+          <t>['Environment Day\n09:49 Disneyland ride shuts down after car derails off track: Witness\n08:35 Ex-GOP congressman David Jolly launches Democratic run for Florida governor (Video)\n08:35 Tavares residents concerned over proposed mixed-use development (Video)\n08:35 Experience', "Kissimmee aims to boost visitors through 'gastro tourism,' value-focused vacations (Video)\n08:35 The Morning News | Live Central Florida headlines, weather and traffic (Video)\n08:34 Gamers camp out for Nintendo Switch 2 (Video)\n08:34 Are traffic control"]</t>
         </is>
       </c>
       <c r="H77" t="n">
-        <v>0.1531</v>
+        <v>-0.2969</v>
       </c>
       <c r="I77" t="n">
-        <v>0.108</v>
+        <v>0.048</v>
       </c>
       <c r="J77" t="n">
-        <v>0.073</v>
+        <v>0.093</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>DL-380770c64735dbc1c56d63a05fb4b763</t>
+          <t>DL-f75243e86744d36c28e7960ee772b4c0</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>What are the best TVs to choose for the Nintendo Switch 2?</t>
+          <t>Microsoft unveils Xbox gaming handheld launching in 2025 (updated with hands-on)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>https://www.frandroid.com/guide-dachat/2638901_quels-sont-les-meilleurs-tv-a-choisir-pour-la-switch-2</t>
+          <t>https://venturebeat.com/business/microsoft-unveils-xbox-gaming-handheld-launching-in-2025/</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 is available and to take full advantage of the power of the new Nintendo console, it is essential to choose a TV at the right height. The definition The Ultra HD 4K definition is now indispensable for the Switch 2, which offers graphics in very high resolution when used in dock mode. This resolution provides an image of remarkable sharpness, with finer details and greater immersion.</t>
+          <t>Microsoft is diving into the handheld gaming market with its own Xbox-branded handheld in partnership with PC maker Asus. It has the Windows OS, a full Xbox screen experience, and Armoury Crate SE as a central hub for device management. The handheld will compete with rivals such as the Nintendo Switch 2 and the Valve Steam Deck.</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0.7773247</v>
+        <v>1.0159073</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2025-06-07T17:00:06</t>
+          <t>2025-06-08T20:53:17+00:00</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>['Philips The One PUS8909 // Source: Philips In short, whether you prefer reactivity, image quality, brightness or immersion, there are now televisions perfectly suited to the Nintendo Switch 2.', 'OLED, Mini LED, QLED or LED, each technology has its advantages, but all the references cited here guarantee a fluid, immersive gaming experience that is faithful to the vision of Nintendo game creators.', 'All you need to know about the Switch 2 Want to know everything about the Nintendo Switch 2 after the Direct announcements? Find our video recap on YouTube for a quick and clear summary.']</t>
+          <t>['“The Xbox experience grows with you,” said Sarah Bond, president of Xbox, in the Xbox Showcase.\nThe company plans to launch the handheld in 2025. As such, it will compete with rivals such as the Nintendo Switch 2 and the Valve Steam Deck.', 'This one promises the power of an Xbox experience in your hands. It has a seven-inch IPS VRR screen.\nThe move could inspire both fear and derision, as the prospect for such a move has done in the past.']</t>
         </is>
       </c>
       <c r="H78" t="n">
-        <v>0.7964</v>
+        <v>0.0772</v>
       </c>
       <c r="I78" t="n">
-        <v>0.114</v>
+        <v>0.024</v>
       </c>
       <c r="J78" t="n">
         <v>0</v>
@@ -3862,86 +3862,86 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>DL-4de785c3d00dac3779286d8e34763c81</t>
+          <t>DL-1c59b6df7e032db28024c576f73acce5</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>How to Transfer Your Switch Data to Nintendo Switch 2</t>
+          <t>It started - Switch 2 with the first technical problems. Difficulties when downloading Mario Kart World</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>https://www.iphoneincanada.ca/2025/06/05/how-to-transfer-your-data-nintendo-switch-2/</t>
+          <t>https://www.gram.pl/news/zaczelo-sie-switch-2-z-pierwszymi-problemami-technicznymi-utrudnienia-przy-pobieraniu-mario-kart-world</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Nintendo provides a streamlined way to conduct a system transfer from Nintendo Switch to the Switch 2. Players can transfer profile data, save data, screenshots or video, and system settings. Nintendo notes that there is an expiry date for all system transfer data.</t>
+          <t>Players who wanted to start their adventure with Nintendo Switch 2 reported serious problems with downloading the game. Error 2813-0171 The phrase "Mario Kart World doesn't want to be downloaded" quickly began to dominate search engines and forums. The source of the problem may be differences in console boot packages.</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>0.7033691399999999</v>
+        <v>1.0086613</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2025-06-05T11:06:10+00:00</t>
+          <t>2025-06-06T10:10:00</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>['By selecting ‘ I Don’t Have a Nintendo Switch 2 Yet’, you can upload your data to Nintendo’s servers in anticipation of when your Nintendo Switch 2 arrives.', 'Follow the on-screen prompts until you’re sent a ‘Verification code’ to your My Nintendo account email address. Input the code and select ‘Send Data to the Server’. This will then upload your save data to Nintendo’s cloud servers.', 'Once the upload is complete, you can review the system transfer information and select ‘Start Restoring Factory Settings’ to complete the process. Note: This will delete all data from the original console.']</t>
+          <t>['Users who purchased Nintendo Switch 2 with Mario Kart World graphics printed directly on the box have problems activating the game.', 'In turn, people who purchased the version with the attached sticker and download code, seem not to experience difficulties. GramTV reports: This is confirmed by reports from the USA.']</t>
         </is>
       </c>
       <c r="H79" t="n">
-        <v>0.4939</v>
+        <v>-0.743</v>
       </c>
       <c r="I79" t="n">
-        <v>0.076</v>
+        <v>0.065</v>
       </c>
       <c r="J79" t="n">
-        <v>0</v>
+        <v>0.196</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>DL-c7b1d654f43bf3a0aede5a40cc6ebaca</t>
+          <t>DL-736adae141649efa336e9f7ce03ea527</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>You probably don't have this Switch 2 launch title on your screen and it comes with a pretty cool co-op feature</t>
+          <t>The Nintendo Switch 2 launches today. Here’s what to know</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>https://www.gamepro.de/artikel/nintendo-switch-2-gameshare-survival-kids,3434002.html</t>
+          <t>https://localnews8.com/money/cnn-business-consumer/2025/06/05/the-nintendo-switch-2-launches-today-heres-what-to-know/</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>This week, Nintendo Switch 2 comes out with a whole series of launch titles that you can play directly on the new console on June 5th. This includes Survival Kids, which besides Mario Kart World or Donkey Kong flies rather under the radar. You take on the role of four children who are stranded on an island and explore crafts and the surroundings to find a way home.</t>
+          <t>Nintendo's new console, the Switch 2, arrives on store shelves globally after being announced in April. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table; or on. a TV when plugged in to its accompanying dock, like its predecessor. Nintendo’s decision to stick with a winning template for the Switch 2 is a testament to the original’s popularity.</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>0.67687225</v>
+        <v>0.9118633</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2025-06-03T11:27:17+00:00</t>
+          <t>2025-06-05T13:14:10</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>['So you can play locally on a total of three devices as long as at least one person in the group has a Nintendo Switch 2 and the game supports GameShare. In the case of Survival Kids, the game runs via GameShare with two consoles for both in 60 fps.', 'On the other hand, if you start on three devices, the frame rate is reduced to 30 fps for everyone involved. Nevertheless, this way of playing together is a cool thing that has a lot of potential.']</t>
+          <t>['In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.\nNintendo has also given the console hardware a much-needed upgrade.', 'The Switch 2 has a larger 7.9-inch display compared to the original Switch’s 6.2-inch screen, and the Joy-Cons now snap to the console magnetically, which should make them easier to attach or remove from the console.']</t>
         </is>
       </c>
       <c r="H80" t="n">
-        <v>0.34</v>
+        <v>0.9136</v>
       </c>
       <c r="I80" t="n">
-        <v>0.036</v>
+        <v>0.194</v>
       </c>
       <c r="J80" t="n">
         <v>0</v>
@@ -3950,130 +3950,130 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>DL-194cd17a14f69417b82c9c6d47023133</t>
+          <t>DL-616a7e8681b35c912aff6ad9ed350a31</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>High demand makes Nintendo Switch 2 sell out in Brazil on its first day of release.</t>
+          <t>The Nintendo Switch 2 launches today. Here's what to know</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>https://www1.folha.uol.com.br/tec/2025/06/alta-demanda-faz-nintendo-switch-2-esgotar-no-brasil-no-primeiro-dia-de-vendas.shtml</t>
+          <t>https://www.erienewsnow.com/story/52829208/the-nintendo-switch-2-launches-today-heres-what-to-know</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2, a new video game console from the Japanese company, went off the shelf this Friday in the global markets. It's already sold out in major Brazilian stores due to high demand. The console has a suggested price of R$4,499.90 in the standard version, no games.</t>
+          <t>Nintendo's new console, the Switch 2, arrives on store shelves globally after being announced in April. The Switch 2, priced at $450 in the US, can be played in handheld mode, when propped up on a table; or on. TV when plugged in to its accompanying dock, like its predecessor. Nintendo’s decision to stick with a winning template for the Switch 2 is a testament to the original’s popularity.</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>0.6762066</v>
+        <v>0.9118633</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2025-06-05T21:23:16+00:00</t>
+          <t>2025-06-05T13:22:00+00:00</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>['Ampere predicts that Switch 2 sales will surpass 100 million units by 2030. See more about the Nintendo Switch 2.', 'Novelties The new console will have an improved 7.9-inch LCD screen, with HDR support and refresh rates of up to 120 Hz, ensuring smoother display.']</t>
+          <t>['In the Switch 2 version of “Metroid Prime 4: Beyond,” players will be able to move the Joy-Con like a mouse for more precise aiming when shooting enemies.', '“People who may play on a PC with a mouse and a keyboard, that’s an experience they can’t replicate,” Bowser said.\nNintendo has also given the console hardware a much-needed upgrade.', 'The Switch 2 has a larger 7.9-inch display compared to the original Switch’s 6.2-inch screen, and the Joy-Cons now snap to the console magnetically, which should make them easier to attach or remove from the console.']</t>
         </is>
       </c>
       <c r="H81" t="n">
-        <v>-0.4019</v>
+        <v>0.9136</v>
       </c>
       <c r="I81" t="n">
-        <v>0</v>
+        <v>0.194</v>
       </c>
       <c r="J81" t="n">
-        <v>0.081</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>DL-1f7196f9804c69956dd1ea78f94a50cf</t>
+          <t>DL-58363b4cfde0e0889c7251f2961ae5ee</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Switch 2: Why Nintendo doesn't want you to remove the display slide</t>
+          <t>The Nintendo Switch 2 : a promising new breath despite some disillusionment</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>https://t3n.de/news/switch-2-nintendo-display-folie-1691041/</t>
+          <t>https://s2pmag.ch/avis-la-nintendo-switch-2-un-nouveau-souffle-prometteur-malgre-quelques-desillusions/</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>On June 5, 2025, the new Nintendo console Switch 2 will officially go on sale. Pre-ordering is currently not possible on major online trading platforms. It is currently unknown when the console will be available again. Nintendo explicitly warns against removing the factory-mounted display slide.</t>
+          <t>The Nintendo Switch 2 has finally slipped into our hands. What lessons can we learn from these first moments of ownership? A complete and careful case The Switch 2 comes in a package with an almost confusing simplicity, compact dimensions that are unmistakably reminiscent of its grandmother. The console is delivered ready for use, accompanied by the necessary accessories to take full advantage of it.</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>0.67266464</v>
+        <v>0.88768387</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2025-06-04T11:45:37</t>
+          <t>2025-06-09T06:16:01</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>['Switch 2 is supposed to get new charging mode Nintendo is supposed to have found a solution for this with the Switch 2 – namely a battery-saving charging mode as usual with smartphones.', "View 8 images This retro technology has collector's value today Source: More on this topic MIT Technology Review Nintendo"]</t>
+          <t>['A balanced review, promises to be confirmed In the end, this Nintendo Switch 2 turns out to be capable of the best as well as the least good, offering contrasting experiences according to titles and usages.']</t>
         </is>
       </c>
       <c r="H82" t="n">
-        <v>-0.1027</v>
+        <v>0.5413</v>
       </c>
       <c r="I82" t="n">
-        <v>0</v>
+        <v>0.094</v>
       </c>
       <c r="J82" t="n">
-        <v>0.032</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>DL-0baa3766bc883eba68c2dbbae1038cce</t>
+          <t>DL-d31952a6c00a7f14a8bb1d96ce43f30c</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Donkey Kong Bananza: Release date, trailer and highlights</t>
+          <t>Video games: Microsoft unveils the first portable versions of the Xbox</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>https://www.netcost-security.fr/mobilite/252228/donkey-kong-bananza-date-de-sortie-bande-annonce-et-exclusivites-eclairantes/</t>
+          <t>https://www.lessentiel.lu/fr/story/jeux-video-microsoft-devoile-les-premieres-versions-portables-de-la-xbox-103361849</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>The Nintendo Switch 2 is now available with an exciting set of new games. Donkey Kong Bonanza is a must-see for fans of the iconic character. Discover key details, including the release date and pre-command options.</t>
+          <t>Xbox portable consoles, ROG Ally and Ally X, designed with Asus, will be marketed for the end of the year celebrations. This Twitter content cannot be displayed due to your current choice of cookies. The price of the consoles and exact date of their launch will be announced in the coming months.</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>0.67111206</v>
+        <v>0.8702202</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2025-06-06T16:22:33+00:00</t>
+          <t>2025-06-10T09:56:00+00:00</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>['To make the Switch 2 more attractive, Nintendo has released a number of games compatible only with this console. One of the games in question is a new title with Donkey Kong.', 'We will review the details of the new game, the release date of Donkey Kong Bonanza, the price, the pre-order options and the gameplay. Note that this game is only available for the Nintendo Switch 2.']</t>
+          <t>["Faced with Nintendo Switch 2 The design of both models evokes the brand's traditional handles, with the same buttons, joysticks and handles, but with a longer format to integrate a central screen.", '"Xbox Ally and Xbox Ally X are perfect for players looking for an accessible gaming experience on the go, whether between two planes or between two comfortable lounge chairs," Microsoft said in a press release.']</t>
         </is>
       </c>
       <c r="H83" t="n">
-        <v>0.4939</v>
+        <v>0</v>
       </c>
       <c r="I83" t="n">
-        <v>0.08400000000000001</v>
+        <v>0</v>
       </c>
       <c r="J83" t="n">
         <v>0</v>
@@ -4082,86 +4082,86 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>DL-c530336e1b88c22a95418a5f5123d3a8</t>
+          <t>DL-52361e315938e25ca5f998c23b324103</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>I think Nintendo played it very safe with Switch 2 - but that's not a bad thing</t>
+          <t>Nintendo Switch 2: Should I buy it now or wait?</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>https://www.indy100.com/gaming/nintendo-switch-2-first-impressions-features-gameplay-gamechat-gameshare</t>
+          <t>https://www.presse-citron.net/nintendo-switch-2-faut-il-lacheter-maintenant-ou-attendre/</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Nintendo has just straight up called this the Switch 2 - no SNES, Wii-U or 3DS confusion here, it's clearly a successor to the Switch. This is very indicative of the route Nintendo has gone down with the new console. It's undeniably more of an upgrade rather than something completely new and revolutionary with Nintendo seemingly playing it very safe. There are now a lot more competitors in this market because of its success, such as the Steam Deck.</t>
+          <t>Nintendo is changing its habits with the Switch 2. For the first time in years, the Kyoto firm did not send its console to journalists several weeks before the launch. As a result, in-depth testing will arrive after the sale, leaving some players in uncertainty.</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>0.6582527</v>
+        <v>0.83535385</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2025-06-05T15:07:15</t>
+          <t>2025-06-05T10:19:31+00:00</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>['With the Switch and this concept proving such a hit, Nintendo has understandably not wanted to veer too much away from what made the original Switch so successful, instead refining the experience with the Switch 2 with new features, better performance']</t>
+          <t>['So, are we buying Switch 2 today or not? The decision ultimately depends on your player profile and your priorities. The unconditional Nintendo fans and early adopters assumed will in any case dark without remorse.', 'I think the more measured players will benefit from waiting for our full review next week by identifying the console’s strengths and weaknesses, and then being able to make a fully informed choice.']</t>
         </is>
       </c>
       <c r="H84" t="n">
-        <v>0.8687</v>
+        <v>-0.34</v>
       </c>
       <c r="I84" t="n">
-        <v>0.175</v>
+        <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>0.051</v>
+        <v>0.053</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>DL-fb44e9ba1c36059416a5f81b3d4717bc</t>
+          <t>DL-380770c64735dbc1c56d63a05fb4b763</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 is here - first impressions</t>
+          <t>What are the best TVs to choose for the Nintendo Switch 2?</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>https://www.gram.pl/artykul/nintendo-switch-2-juz-tu-jest-pierwsze-wrazenia</t>
+          <t>https://www.frandroid.com/guide-dachat/2638901_quels-sont-les-meilleurs-tv-a-choisir-pour-la-switch-2</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 is one of my favorite consoles, which has accompanied me in various roles for over eight years. The first Switch was with me until the release of the OLED version in 2021. I forgave myself for Lite, because it did not correspond to my preferences of playing mainly on TV.</t>
+          <t>The Nintendo Switch 2 is available and to take full advantage of the power of the new Nintendo console, it is essential to choose a TV at the right height. The definition The Ultra HD 4K definition is now indispensable for the Switch 2, which offers graphics in very high resolution when used in dock mode. This resolution provides an image of remarkable sharpness, with finer details and greater immersion.</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>0.6255646</v>
+        <v>0.7776336700000001</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2025-06-07T19:00:00</t>
+          <t>2025-06-07T17:00:06</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>['But when the long-awaited Switch 2 appeared on the horizon, placing a pre-release order was obvious.', 'I will immediately point out that this text is not a racial review of the equipment, but rather an impression, a collection of first impressions and thoughts about the new Nintendo toy.', 'Nintendo Switch 2 is a console that can be labeled the “new generation”, and at the same time it is very strongly rooted in what the first Switch accustomed us to. More a subdued but significant evolution than a surprising revolution.']</t>
+          <t>['Philips The One PUS8909 // Source: Philips In short, whether you prefer reactivity, image quality, brightness or immersion, there are now televisions perfectly suited to the Nintendo Switch 2.', 'OLED, Mini LED, QLED or LED, each technology has its advantages, but all the references cited here guarantee a fluid, immersive gaming experience that is faithful to the vision of Nintendo game creators.', 'All you need to know about the Switch 2 Want to know everything about the Nintendo Switch 2 after the Direct announcements? Find our video recap on YouTube for a quick and clear summary.']</t>
         </is>
       </c>
       <c r="H85" t="n">
-        <v>0.7351</v>
+        <v>0.7964</v>
       </c>
       <c r="I85" t="n">
-        <v>0.133</v>
+        <v>0.114</v>
       </c>
       <c r="J85" t="n">
         <v>0</v>
@@ -4170,174 +4170,174 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>DL-6f733f86e304a8935fcf4754a27bb178</t>
+          <t>DL-c530336e1b88c22a95418a5f5123d3a8</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>New Florida education commissioner selected, Trump and Putin discuss Ukraine and Iran and Pasco County launches "Summer Haul Pass"</t>
+          <t>I think Nintendo played it very safe with Switch 2 - but that's not a bad thing</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>https://baynews9.com/fl/tampa/evening-briefing/2025/06/04/evening-briefing-tampa-june-4-2025</t>
+          <t>https://www.indy100.com/gaming/nintendo-switch-2-first-impressions-features-gameplay-gamechat-gameshare</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Your Weather Planner It will be partly to mostly cloudy on Thursday with highs in the upper 80s. Low temperatures fall to the mid 70s overnight with scattered storms ending in the evening. Donald Trump talks to Putin on Ukraine and Iran, says it was 'not a conversation that will lead to immediate Peace'</t>
+          <t>Nintendo has just straight up called this the Switch 2 - no SNES, Wii-U or 3DS confusion here, it's clearly a successor to the Switch. This is very indicative of the route Nintendo has gone down with the new console. It's undeniably more of an upgrade rather than something completely new and revolutionary with Nintendo seemingly playing it very safe. There are now a lot more competitors in this market because of its success, such as the Steam Deck.</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>0.6108513</v>
+        <v>0.65828323</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2025-06-04T20:45:00+00:00</t>
+          <t>2025-06-05T15:07:15</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>["NATO defence ministers meeting\nBET Experience 2025, annual week of 'entertainment, engagement, and empowerment all anchored in the brilliance and creativity of Black culture' ahead of the Black Entertainment Television\nNintendo releases the new Nintendo", 'Switch 2 games console, which features a bigger screen and better graphics than its predecessor.']</t>
+          <t>['With the Switch and this concept proving such a hit, Nintendo has understandably not wanted to veer too much away from what made the original Switch so successful, instead refining the experience with the Switch 2 with new features, better performance']</t>
         </is>
       </c>
       <c r="H86" t="n">
-        <v>0.34</v>
+        <v>0.8687</v>
       </c>
       <c r="I86" t="n">
-        <v>0.064</v>
+        <v>0.175</v>
       </c>
       <c r="J86" t="n">
-        <v>0.038</v>
+        <v>0.051</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>DL-52361e315938e25ca5f998c23b324103</t>
+          <t>DL-d75fb6cd5f8f9f354bda0b190d88b772</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: Should I buy it now or wait?</t>
+          <t>10 Tech Stocks on Wall Street’s Radar</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>https://www.presse-citron.net/nintendo-switch-2-faut-il-lacheter-maintenant-ou-attendre/</t>
+          <t>https://www.insidermonkey.com/blog/10-tech-stocks-on-wall-streets-radar-1549836/</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Nintendo is changing its habits with the Switch 2. For the first time in years, the Kyoto firm did not send its console to journalists several weeks before the launch. As a result, in-depth testing will arrive after the sale, leaving some players in uncertainty.</t>
+          <t>Mark Malek said that not all sectors react the same to market headlines. He added that news can even create chances for late investors to join in. In fact, the opportunity in the mid to long term will transcend these sort of news items.</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>0.43597412</v>
+        <v>0.6415367</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2025-06-05T10:19:31+00:00</t>
+          <t>2025-06-09T14:02:05+00:00</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>['So, are we buying Switch 2 today or not? The decision ultimately depends on your player profile and your priorities. The unconditional Nintendo fans and early adopters assumed will in any case dark without remorse.', 'I think the more measured players will benefit from waiting for our full review next week by identifying the console’s strengths and weaknesses, and then being able to make a fully informed choice.']</t>
+          <t>['On June 5, B.Riley increased its price target on Silicon Motion Technology Corporation (NASDAQ:SIMO) to $90 from $75 and reaffirmed its Buy rating on the stock.', 'The firm pointed to the expanded Nvidia Bluefield DPU win and the upcoming Nintendo Switch 2 cycle as drivers of longer-term gains for the company.']</t>
         </is>
       </c>
       <c r="H87" t="n">
-        <v>-0.34</v>
+        <v>0.7845</v>
       </c>
       <c r="I87" t="n">
-        <v>0</v>
+        <v>0.182</v>
       </c>
       <c r="J87" t="n">
-        <v>0.053</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>DL-265565bae7e63a61079d64b43bdbf11e</t>
+          <t>DL-6f733f86e304a8935fcf4754a27bb178</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: What is the real power of the console Cyberpunk 2077 answers</t>
+          <t>New Florida education commissioner selected, Trump and Putin discuss Ukraine and Iran and Pasco County launches "Summer Haul Pass"</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>https://diariodelyaqui.mx/nacional/nintendo-switch-2-cual-es-la-verdadera-potencia-de-la-consola-cyberpunk-2077-lo-responde/110733</t>
+          <t>https://baynews9.com/fl/tampa/evening-briefing/2025/06/04/evening-briefing-tampa-june-4-2025</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Cyberpunk 2077 has been a technically demanding game. This is why it was a surprise to see it run smoothly on Nintendo Switch 2 with a good graphical level. The CD Projekt Red game has served as an unofficial but very revealing test of the console's potential.</t>
+          <t>Your Weather Planner It will be partly to mostly cloudy on Thursday with highs in the upper 80s. Low temperatures fall to the mid 70s overnight with scattered storms ending in the evening. Donald Trump talks to Putin on Ukraine and Iran, says it was 'not a conversation that will lead to immediate Peace'</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>0.38476562</v>
+        <v>0.61086273</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2025-06-06T00:00:00</t>
+          <t>2025-06-04T20:45:00+00:00</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>['COMPARISON WITH OTHER CONSOLIDATIONS An analysis conducted by the Bits Analyzer channel compared the performance of Cyberpunk 2077 on Switch 2 to that of PS4 Pro and Xbox Series S.', "In 'Quality' mode, the Nintendo console achieves 1080p on both laptop and desktop thanks to the DLSS.", "In 'Resolution' mode, it maintains this resolution on the dock, but on the laptop it drops to 720p, with an increase in frame rate of up to 40 fps, although not always stable."]</t>
+          <t>["NATO defence ministers meeting\nBET Experience 2025, annual week of 'entertainment, engagement, and empowerment all anchored in the brilliance and creativity of Black culture' ahead of the Black Entertainment Television\nNintendo releases the new Nintendo", 'Switch 2 games console, which features a bigger screen and better graphics than its predecessor.']</t>
         </is>
       </c>
       <c r="H88" t="n">
-        <v>0.2617</v>
+        <v>0.34</v>
       </c>
       <c r="I88" t="n">
-        <v>0.08</v>
+        <v>0.064</v>
       </c>
       <c r="J88" t="n">
-        <v>0.033</v>
+        <v>0.038</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>DL-d75fb6cd5f8f9f354bda0b190d88b772</t>
+          <t>DL-bc097bf1484dc8cb970325f8ea1be195</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>10 Tech Stocks on Wall Street’s Radar</t>
+          <t>Roman Sands RE:Build release date revealed</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>https://www.insidermonkey.com/blog/10-tech-stocks-on-wall-streets-radar-1549836/</t>
+          <t>https://www.devx.com/daily-news/roman-sands-rebuild-release-date-revealed/</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Mark Malek said that not all sectors react the same to market headlines. He added that news can even create chances for late investors to join in. In fact, the opportunity in the mid to long term will transcend these sort of news items.</t>
+          <t>Roman Sands RE:Build is coming to PS5 and PS4 on September 12th. The game focuses on providing great service and making connections with others. There are also some upcoming gaming events: The Xbox Games Showcase 2025 will feature The Outer Worlds 2 Direct on June 8 at 1:00 pm.</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>0.28679657</v>
+        <v>0.5885391</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2025-06-09T14:02:05+00:00</t>
+          <t>2025-06-09T17:16:20+00:00</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>['On June 5, B.Riley increased its price target on Silicon Motion Technology Corporation (NASDAQ:SIMO) to $90 from $75 and reaffirmed its Buy rating on the stock.', 'The firm pointed to the expanded Nvidia Bluefield DPU win and the upcoming Nintendo Switch 2 cycle as drivers of longer-term gains for the company.']</t>
+          <t>['Other gaming news includes:\nReviews of how Zelda Tears of the Kingdom and Breath of the Wild run on the new Nintendo Switch 2. A look at what makes the game The Bornless different from other extraction games.', 'First impressions of the Nintendo Switch 2 after three days. The gaming community also celebrated diversity during Pride 2025. It featured LGBT voices in horror and talks with Nicole Maines and Michael Varrati.']</t>
         </is>
       </c>
       <c r="H89" t="n">
-        <v>0.7845</v>
+        <v>0.6249</v>
       </c>
       <c r="I89" t="n">
-        <v>0.182</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="J89" t="n">
         <v>0</v>
@@ -4346,44 +4346,132 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
+          <t>DL-d48247f986f1dcf830f4674167808b7f</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Nintendo Switch 2: Comparison video proves how much better Mario Odysssey looks on the new console</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://www.gamepro.de/artikel/vergleichsvideo-super-mario-odyssey-switch-2,3434189.html</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Super Mario Odyssey is one of the Switch games that get a free upgrade on Switch 2. This means that you don't have to pay extra 10 Euros or have the Nintendo Switch Online subscription with expansion package. You can look forward to a higher resolution and a better, respectively more stable performance on Switch 2, even in a nicer one.</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>0.461895</v>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>2025-06-05T17:15:00</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>['The refresh rate struggles on Switch 1, but at least occasionally with a few minor breaks when it comes to complex, busy areas. Overall, the Switch 2 beats a bit better here, but also the original ran most of the time very smoothly.', 'What stands out is that the image on the Nintendo Switch 2 is much crisper and sharper thanks to the higher resolution. Even details that are farther away are now better recognizable. Overall, the impression is even more round.']</t>
+        </is>
+      </c>
+      <c r="H90" t="n">
+        <v>0.9476</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="J90" t="n">
+        <v>0.021</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>DL-265565bae7e63a61079d64b43bdbf11e</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Nintendo Switch 2: What is the real power of the console Cyberpunk 2077 answers</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://diariodelyaqui.mx/nacional/nintendo-switch-2-cual-es-la-verdadera-potencia-de-la-consola-cyberpunk-2077-lo-responde/110733</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Cyberpunk 2077 has been a technically demanding game. This is why it was a surprise to see it run smoothly on Nintendo Switch 2 with a good graphical level. The CD Projekt Red game has served as an unofficial but very revealing test of the console's potential.</t>
+        </is>
+      </c>
+      <c r="E91" t="n">
+        <v>0.38500977</v>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>2025-06-06T00:00:00</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>['COMPARISON WITH OTHER CONSOLIDATIONS An analysis conducted by the Bits Analyzer channel compared the performance of Cyberpunk 2077 on Switch 2 to that of PS4 Pro and Xbox Series S.', "In 'Quality' mode, the Nintendo console achieves 1080p on both laptop and desktop thanks to the DLSS.", "In 'Resolution' mode, it maintains this resolution on the dock, but on the laptop it drops to 720p, with an increase in frame rate of up to 40 fps, although not always stable."]</t>
+        </is>
+      </c>
+      <c r="H91" t="n">
+        <v>0.2617</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="J91" t="n">
+        <v>0.033</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
           <t>DL-1c749b3242262132fa02efa86da3ad6e</t>
         </is>
       </c>
-      <c r="B90" t="inlineStr">
+      <c r="B92" t="inlineStr">
         <is>
           <t>Mario Kart World review: You need to know these things before it drops</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr">
+      <c r="C92" t="inlineStr">
         <is>
           <t>https://www.the-independent.com/extras/indybest/gadgets-tech/video-games-consoles/mario-kart-world-review-b2763892.html</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr">
+      <c r="D92" t="inlineStr">
         <is>
           <t>Your support helps us to tell the story Read more Support Now From reproductive rights to climate change to Big Tech, The Independent is on the ground when the story is developing. Your donation allows us to keep sending journalists to both sides of the story. We choose not to lock Americans out of our reporting and analysis with paywalls. Expectations are sky-high for the latest entry in the 33-year-old racing series, which carries the weight of a new console’s fortunes on its shoulders.</t>
         </is>
       </c>
-      <c r="E90" t="n">
-        <v>0.15307999</v>
-      </c>
-      <c r="F90" t="inlineStr">
+      <c r="E92" t="n">
+        <v>0.3213997</v>
+      </c>
+      <c r="F92" t="inlineStr">
         <is>
           <t>2025-06-04T20:26:36</t>
         </is>
       </c>
-      <c r="G90" t="inlineStr">
+      <c r="G92" t="inlineStr">
         <is>
           <t>['That feels choppy compared to the silky smooth frame rate of single player mode at first, but your eyes will adjust to the difference before you’ve finished your first race.\nopen image in gallery Split-screen dials back the frame rate but keeps 24-player', 'races and the ability to explore the open world ( Nintendo )\nAs an aside, if you don’t think you can spot the difference between games running at 30, 60 and 120 frames per second, the Nintendo Switch 2 Welcome Tour has a special minigame where you can']</t>
         </is>
       </c>
-      <c r="H90" t="n">
+      <c r="H92" t="n">
         <v>0.7906</v>
       </c>
-      <c r="I90" t="n">
+      <c r="I92" t="n">
         <v>0.089</v>
       </c>
-      <c r="J90" t="n">
+      <c r="J92" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4456,7 +4544,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>What are the latest and most unbiased reviews or ratings or experiences on the Nintendo Switch 2. Please ensure the articles are solely on the Nintendo Switch 2.</t>
+          <t>Articles with the words 'reviews' or 'ratings' or 'experiences' and Nintendo Switch 2 in the Title</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -4516,14 +4604,14 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>What are the latest and most unbiased reviews or ratings or experiences on the Nintendo Switch 2. Please ensure the articles are solely on the Nintendo Switch 2.</t>
+          <t>Articles with the words 'reviews' or 'ratings' or 'experiences' and Nintendo Switch 2 in the Title</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
working scale and word cloud
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>321.1636</v>
+        <v>452.753</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
@@ -530,42 +530,42 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DL-56b3456fa4d4c2c0316f8c748ec38942</t>
+          <t>DL-735f6f5e7ee6d998aecda59ababcdbcc</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 Welcome Tour Review</t>
+          <t>How I plan to review the Nintendo Switch 2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.rocketchainsaw.com.au/review/nintendo-switch-2-welcome-tour-review/</t>
+          <t>https://www.theverge.com/nintendo/679346/nintendo-switch-2-review-guidelines-plan-launch</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>The Welcome Tour is presented as a virtual museum, an enormous virtual representation of the Switch 2. The camera is set high from an isometric perspective, sometimes zooming out to encompass an entire area with people browsing the exhibits like ants. There’s even some mildly funny dialogue and little set pieces thrown in among the attendees you can chat to.</t>
+          <t>Nintendo has decided to not send out early review units to The Verge or other outlets, citing the need for day-one software updates. It’s a way to explore every facet of a new console and get a wide variety of perspectives. This time, we’re going to start with those deeper dives.</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>162.88614</v>
+        <v>253.28822</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-06-09T04:20:44+00:00</t>
+          <t>2025-06-04T12:00:00+00:00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Almost everything about the Switch 2 ahead of launch has been a little weird, from the confusing messaging and high pricing to the unfortunately timed connection with spiking tariffs.', 'Intent to keep that strange energy going, Nintendo has decided to not send out early review units to The Verge or other outlets, citing the need for day-one software updates. (This was not the case with the original Switch.)']</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>0.8126</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.132</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -574,42 +574,42 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DL-2a418e6f75f602bcd521348ca4edc33a</t>
+          <t>DL-56b3456fa4d4c2c0316f8c748ec38942</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 Camera review - good for GameChat but not much else</t>
+          <t>Nintendo Switch 2 Welcome Tour Review</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.pockettactics.com/nintendo-switch-2-camera-review</t>
+          <t>https://www.rocketchainsaw.com.au/review/nintendo-switch-2-welcome-tour-review/</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>I'm talking about the Nintendo Switch 2 Camera. It doesn't have many uses outside of GameChat, the Switch 2's new social feature, and a few Mario Party Jamboree – Switch 2 Edition minigames. At Pocket Tactics, our experts spend days testing games, phones, tech, and services. We always share honest opinions to help you buy the best.</t>
+          <t>The Welcome Tour is presented as a virtual museum, an enormous virtual representation of the Switch 2. The camera is set high from an isometric perspective, sometimes zooming out to encompass an entire area with people browsing the exhibits like ants. There’s even some mildly funny dialogue and little set pieces thrown in among the attendees you can chat to.</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>157.21655</v>
+        <v>247.76453</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-06-07T16:55:45</t>
+          <t>2025-06-09T04:20:44+00:00</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>["Unlike most reviews on Pocket Tactics, I'm not scoring the Nintendo Switch 2 Camera out of 10 right now. That's because I've not used any other Switch 2 cameras, so there's no prior context to base a score on.", "For more of our post-launch coverage, be sure to take a look at our Nintendo Switch 2 review, Nintendo Switch 2 Pro Controller review, and Mario Kart World review while you're here.", "Or, if you'd rather grab something to complete your new gaming setup, see our guides to the best Nintendo Switch 2 accessories and the best Nintendo Switch 2 controllers."]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>0.9337</v>
+        <v>0.8126</v>
       </c>
       <c r="I4" t="n">
-        <v>0.247</v>
+        <v>0.132</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -618,42 +618,42 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DL-735f6f5e7ee6d998aecda59ababcdbcc</t>
+          <t>DL-2a418e6f75f602bcd521348ca4edc33a</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>How I plan to review the Nintendo Switch 2</t>
+          <t>Nintendo Switch 2 Camera review - good for GameChat but not much else</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.theverge.com/nintendo/679346/nintendo-switch-2-review-guidelines-plan-launch</t>
+          <t>https://www.pockettactics.com/nintendo-switch-2-camera-review</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Nintendo has decided to not send out early review units to The Verge or other outlets, citing the need for day-one software updates. It’s a way to explore every facet of a new console and get a wide variety of perspectives. This time, we’re going to start with those deeper dives.</t>
+          <t>I'm talking about the Nintendo Switch 2 Camera. It doesn't have many uses outside of GameChat, the Switch 2's new social feature, and a few Mario Party Jamboree – Switch 2 Edition minigames. At Pocket Tactics, our experts spend days testing games, phones, tech, and services. We always share honest opinions to help you buy the best.</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>76.49751000000001</v>
+        <v>225.1066</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-06-04T12:00:00+00:00</t>
+          <t>2025-06-07T16:55:45</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>['Almost everything about the Switch 2 ahead of launch has been a little weird, from the confusing messaging and high pricing to the unfortunately timed connection with spiking tariffs.', 'Intent to keep that strange energy going, Nintendo has decided to not send out early review units to The Verge or other outlets, citing the need for day-one software updates. (This was not the case with the original Switch.)']</t>
+          <t>["Unlike most reviews on Pocket Tactics, I'm not scoring the Nintendo Switch 2 Camera out of 10 right now. That's because I've not used any other Switch 2 cameras, so there's no prior context to base a score on.", "For more of our post-launch coverage, be sure to take a look at our Nintendo Switch 2 review, Nintendo Switch 2 Pro Controller review, and Mario Kart World review while you're here.", "Or, if you'd rather grab something to complete your new gaming setup, see our guides to the best Nintendo Switch 2 accessories and the best Nintendo Switch 2 controllers."]</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>0.9337</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>0.247</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -662,130 +662,130 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DL-b4835f4fe1a96ea2d9f3e5a83449cefc</t>
+          <t>DL-4b86e968a9b1646ef4716b8b7c26d9ad</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>I've already tried the'mouse' mode on Nintendo Switch 2, it opens a door that has so far been closed on consoles.</t>
+          <t>Starting shot for Nintendo Switch 2 – German streamer is already playing Mario Kart World</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.xataka.com/videojuegos/he-probado-modo-raton-nintendo-switch-2-abre-puerta-ahora-cerrada-consolas</t>
+          <t>https://www.giga.de/games/startschuss-fuer-nintendo-switch-2-deutsche-streamerin-zockt-schon-mario-kart-world--01JWXN645JPPJSCMF79ZYQ7SQH</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 is not a machine to experiment with. The 152 million Switches sold are a reflection that the company has achieved a product that people have liked. They don't need something as disruptive as Switch or Wii in their day, but a continuous console. And apart from the size, a change comes with the optical technology.</t>
+          <t>Nintendo Switch 2: Day-One Patch is here The first gamers already have their Switch 2 at home. Version 20.1.1 is live and there are first experiences with the new hybrid console. Nintendo didn't miss a day, it's already June 5th in New Zealand.</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>25.77198</v>
+        <v>47.643147</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-06-05T16:15:49</t>
+          <t>2025-06-04T14:23:08+00:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['Turning to the Joy-Con Nintendo Switch 2 is not a machine to experiment with. The 152 million Switches sold, and rising, are a reflection that the company has achieved a product that people have liked.']</t>
+          <t>['Nintendo Switch 2: Day-One Patch is here The first gamers already have their Switch 2 at home. Until now, the console was completely useless – a day-one patch from Nintendo was missing. That has now changed.', 'The German streamer LostKittn has not only got her Switch 2, she is even now playing Mario Kart World on Twitch. According to the pinned message of a chat moderator, she has received the console from Nintendo and is allowed to play since 2 pm.', 'Players showcase Switch 2 eShop Other players also share their experiences with Switch 2. On Reddit, users show GabSam, for example, the new and improved Nintendo eShop. It now runs much more smoothly than the one on the old console.']</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>0.0644</v>
+        <v>-0.1531</v>
       </c>
       <c r="I6" t="n">
-        <v>0.036</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.031</v>
+        <v>0.039</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DL-4b86e968a9b1646ef4716b8b7c26d9ad</t>
+          <t>DL-b4835f4fe1a96ea2d9f3e5a83449cefc</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Starting shot for Nintendo Switch 2 – German streamer is already playing Mario Kart World</t>
+          <t>I've already tried the'mouse' mode on Nintendo Switch 2, it opens a door that has so far been closed on consoles.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.giga.de/games/startschuss-fuer-nintendo-switch-2-deutsche-streamerin-zockt-schon-mario-kart-world--01JWXN645JPPJSCMF79ZYQ7SQH</t>
+          <t>https://www.xataka.com/videojuegos/he-probado-modo-raton-nintendo-switch-2-abre-puerta-ahora-cerrada-consolas</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: Day-One Patch is here The first gamers already have their Switch 2 at home. Version 20.1.1 is live and there are first experiences with the new hybrid console. Nintendo didn't miss a day, it's already June 5th in New Zealand.</t>
+          <t>Nintendo Switch 2 is not a machine to experiment with. The 152 million Switches sold are a reflection that the company has achieved a product that people have liked. They don't need something as disruptive as Switch or Wii in their day, but a continuous console. And apart from the size, a change comes with the optical technology.</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>24.68355</v>
+        <v>41.942944</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-06-04T14:23:08+00:00</t>
+          <t>2025-06-05T16:15:49</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>['Nintendo Switch 2: Day-One Patch is here The first gamers already have their Switch 2 at home. Until now, the console was completely useless – a day-one patch from Nintendo was missing. That has now changed.', 'The German streamer LostKittn has not only got her Switch 2, she is even now playing Mario Kart World on Twitch. According to the pinned message of a chat moderator, she has received the console from Nintendo and is allowed to play since 2 pm.', 'Players showcase Switch 2 eShop Other players also share their experiences with Switch 2. On Reddit, users show GabSam, for example, the new and improved Nintendo eShop. It now runs much more smoothly than the one on the old console.']</t>
+          <t>['Turning to the Joy-Con Nintendo Switch 2 is not a machine to experiment with. The 152 million Switches sold, and rising, are a reflection that the company has achieved a product that people have liked.']</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>-0.1531</v>
+        <v>0.0644</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>0.036</v>
       </c>
       <c r="J7" t="n">
-        <v>0.039</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DL-22ae66fc1f099f020d69886b1441e56e</t>
+          <t>DL-fa269e8a0e19a32b2bf0f8ce731d82b1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nintendo sells 3.5 million Switch 2 consoles in four days</t>
+          <t>Mario Kart World on Metacritic: First test scores are live and an absolute dream!</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://gameliner.nl/nieuws/nintendo-verkoopt-35-miljoen-switch-2-consoles-binnen-vier-dagen/51020</t>
+          <t>https://www.gamepro.de/artikel/mario-kart-world-metacritic-erste-tests-wertung,3434246.html</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 is the most successful launch in the history of Nintendo hardware. The desired console sold over 3.5 million copies in four days. This is an indication of the trust Nintendo has in producing a console that is more than worth the effort.</t>
+          <t>Nintendo Switch 2 is here and we're shooting our first 37 minutes in Mario Kart World Autoplay What's being praised? Nintenduo gives it a score of 92 and writes: "Everything can still change" Nintendo has perfectly balanced classic and modern elements to create an engaging and accessible experience that will delight both veterans and newcomers.</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>23.607367</v>
+        <v>39.233864</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-06-11T08:15:00+00:00</t>
+          <t>2025-06-06T10:14:00</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>['And of course, this is also an indication of the trust that Nintendo has in producing a console that is more than worth the effort.', "The 3.5 million units sold in four days make the Nintendo Switch 2 the most successful launch in the history of Nintendo hardware. Check out our Nintendo Switch 2 review here. In addition, we've got a Mario Kart World review ready for you."]</t>
+          <t>["The first ratings for Mario Kart World are enthusiastic. No Nintendo Switch 2 consoles and review samples were sent in advance, we received Nintendo's newest flagship on release day.", "37:48 The Nintendo Switch 2 is here and we're shooting our first 37 minutes in Mario Kart World Autoplay What's being praised?", 'This means: Mario Kart World is the latest and perhaps best part of the long-standing arcade racing series and is taken to the next level with the hardware of Nintendo Switch 2 and an extensive roster of drivers, tracks and endless fun.']</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>0.8927</v>
+        <v>0.9413</v>
       </c>
       <c r="I8" t="n">
-        <v>0.235</v>
+        <v>0.252</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -794,42 +794,42 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DL-fa269e8a0e19a32b2bf0f8ce731d82b1</t>
+          <t>DL-22ae66fc1f099f020d69886b1441e56e</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mario Kart World on Metacritic: First test scores are live and an absolute dream!</t>
+          <t>Nintendo sells 3.5 million Switch 2 consoles in four days</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.gamepro.de/artikel/mario-kart-world-metacritic-erste-tests-wertung,3434246.html</t>
+          <t>https://gameliner.nl/nieuws/nintendo-verkoopt-35-miljoen-switch-2-consoles-binnen-vier-dagen/51020</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 is here and we're shooting our first 37 minutes in Mario Kart World Autoplay What's being praised? Nintenduo gives it a score of 92 and writes: "Everything can still change" Nintendo has perfectly balanced classic and modern elements to create an engaging and accessible experience that will delight both veterans and newcomers.</t>
+          <t>Nintendo Switch 2 is the most successful launch in the history of Nintendo hardware. The desired console sold over 3.5 million copies in four days. This is an indication of the trust Nintendo has in producing a console that is more than worth the effort.</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>21.954624</v>
+        <v>37.532463</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-06-06T10:14:00</t>
+          <t>2025-06-11T08:15:00+00:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>["The first ratings for Mario Kart World are enthusiastic. No Nintendo Switch 2 consoles and review samples were sent in advance, we received Nintendo's newest flagship on release day.", "37:48 The Nintendo Switch 2 is here and we're shooting our first 37 minutes in Mario Kart World Autoplay What's being praised?", 'This means: Mario Kart World is the latest and perhaps best part of the long-standing arcade racing series and is taken to the next level with the hardware of Nintendo Switch 2 and an extensive roster of drivers, tracks and endless fun.']</t>
+          <t>['And of course, this is also an indication of the trust that Nintendo has in producing a console that is more than worth the effort.', "The 3.5 million units sold in four days make the Nintendo Switch 2 the most successful launch in the history of Nintendo hardware. Check out our Nintendo Switch 2 review here. In addition, we've got a Mario Kart World review ready for you."]</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>0.9413</v>
+        <v>0.8927</v>
       </c>
       <c r="I9" t="n">
-        <v>0.252</v>
+        <v>0.235</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>16.278522</v>
+        <v>34.85138</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -882,130 +882,130 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DL-05650dfb79bd8bf7ef997bb2ce2f3cd3</t>
+          <t>DL-2fa26bf724852abc5c72c9f822028c52</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 First Impressions And A Surprising Purchasing Score</t>
+          <t>Zelda: The underrated game that deserves a remake for Switch 2</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://hothardware.com/news/nintendo-switch-2-first-impressions-and-a-surprising-purchasing</t>
+          <t>https://www.zazoom.it/2025-06-07/zelda-il-gioco-sottovalutato-che-merita-un-remake-per-switch-2/17144781/</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 is finally out, and I have some first impressions on the experience of both playing and purchasing the console. I was not lucky enough to secure a preorder ahead of the console's June 5th release. Third-party entrepreneurs were already listing the console for a premium over its $449 MSRP. My local Walmart was nearly empty and upon inquiring, I was told it had around six to eight consoles still available in the back.</t>
+          <t>Nintendo would have the opportunity to strengthen the connection between the past and the future, providing an unforgettable experience. With the advent of the new console, the challenge for Nintendo will be to continue to innovate and deliver experiences that meet the expectations of the passionate. The Legend of Zelda: Tears of the Kingdom game shows up on Nintendo Switch 2 with 20 minutes of gameplay.</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>12.011366</v>
+        <v>24.060257</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-06-06T14:31:00+00:00</t>
+          <t>2025-06-07T18:16:28</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>['The Nintendo Switch 2 is finally out, and I have some first impressions on the experience of both playing and purchasing the console.']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>0.5673</v>
+        <v>0.8779</v>
       </c>
       <c r="I11" t="n">
-        <v>0.114</v>
+        <v>0.178</v>
       </c>
       <c r="J11" t="n">
-        <v>0.054</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DL-2fa26bf724852abc5c72c9f822028c52</t>
+          <t>DL-05650dfb79bd8bf7ef997bb2ce2f3cd3</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Zelda: The underrated game that deserves a remake for Switch 2</t>
+          <t>Nintendo Switch 2 First Impressions And A Surprising Purchasing Score</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://www.zazoom.it/2025-06-07/zelda-il-gioco-sottovalutato-che-merita-un-remake-per-switch-2/17144781/</t>
+          <t>https://hothardware.com/news/nintendo-switch-2-first-impressions-and-a-surprising-purchasing</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Nintendo would have the opportunity to strengthen the connection between the past and the future, providing an unforgettable experience. With the advent of the new console, the challenge for Nintendo will be to continue to innovate and deliver experiences that meet the expectations of the passionate. The Legend of Zelda: Tears of the Kingdom game shows up on Nintendo Switch 2 with 20 minutes of gameplay.</t>
+          <t>Nintendo Switch 2 is finally out, and I have some first impressions on the experience of both playing and purchasing the console. I was not lucky enough to secure a preorder ahead of the console's June 5th release. Third-party entrepreneurs were already listing the console for a premium over its $449 MSRP. My local Walmart was nearly empty and upon inquiring, I was told it had around six to eight consoles still available in the back.</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>11.431488</v>
+        <v>21.127535</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-06-07T18:16:28</t>
+          <t>2025-06-06T14:31:00+00:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['The Nintendo Switch 2 is finally out, and I have some first impressions on the experience of both playing and purchasing the console.']</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>0.8779</v>
+        <v>0.5673</v>
       </c>
       <c r="I12" t="n">
-        <v>0.178</v>
+        <v>0.114</v>
       </c>
       <c r="J12" t="n">
-        <v>0.026</v>
+        <v>0.054</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DL-cce7387fccad72acd7b577de07a1a6e3</t>
+          <t>DL-8d8caf04d65da8ebac6136b7cec59a11</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 unboxing: What do you get with the console?</t>
+          <t>Nintendo Switch 2 Unboxing, Setup &amp; What You Need to Know</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://www.indy100.com/gaming/nintendo-switch-2-unboxing-console-2672317405</t>
+          <t>https://www.geeky-gadgets.com/nintendo-switch-2-4/</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Nintendo has sent review units out to media outlets for them to check out the new console and games running on it. The first thing that will be seen when unboxing are the two new Joy-Con controllers and main part of the console with the bigger screen. Below that on the next layer down is a brief user manual, a HDMI cable to connect the dock to a TV and the wrist strap accessories that connect to the Switch 2.</t>
+          <t>This guide explores the unboxing experience, setup process, design changes, hardware advancements, and new features, while also comparing it to the original Nintendo Switch. The packaging is compact and eco-friendly, underscoring Nintendo’s commitment to reducing environmental impact. Inside the box, you’ll find: The Nintendo Switch 2 console Two redesigned Joy-Con controllers A revamped dock featuring an Ethernet port An HDMI cable A power adapter.</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>9.850194999999999</v>
+        <v>19.452656</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-06-05T15:19:37</t>
+          <t>2025-06-08T13:00:24</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>['Nintendo has sent Switch 2 review units out to media outlets for them to check out the new console and games running on it.\nindy100 is very fortunate to have been sent one of these units and this is what comes in the box - read our first impressions of']</t>
+          <t>['The video below from Zollotech gives us a detailed look at the new Switch console.\nUnboxing: What’s Inside the Box?\nThe unboxing experience of the Nintendo Switch 2 reflects a focus on simplicity and sustainability.', 'Setting Up: From Box to Gameplay\nSetting up the Nintendo Switch 2 is a straightforward process designed to get you gaming quickly.', 'New Features: Enhancing the Experience\nThe Nintendo Switch 2 introduces several new features that enhance the overall user experience and cater to modern gaming needs:\nOnline Functionality: Faster download speeds and a more stable connection improve multiplayer']</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>0.5859</v>
+        <v>0.8979</v>
       </c>
       <c r="I13" t="n">
-        <v>0.048</v>
+        <v>0.166</v>
       </c>
       <c r="J13" t="n">
         <v>0</v>
@@ -1014,42 +1014,42 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>DL-8d8caf04d65da8ebac6136b7cec59a11</t>
+          <t>DL-f955c260113cb461bc83d07b7ef513dd</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 Unboxing, Setup &amp; What You Need to Know</t>
+          <t>Nintendo Switch 2 Comes With a Below-Average Display and Disappointing HDR Support, New In-Depth Analysis Reveals</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://www.geeky-gadgets.com/nintendo-switch-2-4/</t>
+          <t>https://wccftech.com/nintendo-switch-2-below-average-hdr/</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>This guide explores the unboxing experience, setup process, design changes, hardware advancements, and new features, while also comparing it to the original Nintendo Switch. The packaging is compact and eco-friendly, underscoring Nintendo’s commitment to reducing environmental impact. Inside the box, you’ll find: The Nintendo Switch 2 console Two redesigned Joy-Con controllers A revamped dock featuring an Ethernet port An HDMI cable A power adapter.</t>
+          <t>The new analysis by GamingTech takes a good look at the new Nintendo system's display. Measuring the brightness in Zelda: Breath of the Wild returned a maximum value of 420 nits, but in Cyberpunk 2077, it is locked to 450 nit, likely the maximum peak brightness the display is capable of. This peak brightness is not even close to providing a proper HDR experience.</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>8.254066</v>
+        <v>15.894136</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-06-08T13:00:24</t>
+          <t>2025-06-05T11:37:00+00:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>['The video below from Zollotech gives us a detailed look at the new Switch console.\nUnboxing: What’s Inside the Box?\nThe unboxing experience of the Nintendo Switch 2 reflects a focus on simplicity and sustainability.', 'Setting Up: From Box to Gameplay\nSetting up the Nintendo Switch 2 is a straightforward process designed to get you gaming quickly.', 'New Features: Enhancing the Experience\nThe Nintendo Switch 2 introduces several new features that enhance the overall user experience and cater to modern gaming needs:\nOnline Functionality: Faster download speeds and a more stable connection improve multiplayer']</t>
+          <t>["Related Story Level Up Your Switch 2 Experience With Mumba’s Blade Series, Clear Series Dockable Cases, and Carrying Case\nThe Nintendo Switch 2's HDR support in docked mode fares a little better.", 'The system-level calibration is found to be adequate, and in games like Cyberpunk 2077, the system delivers an HDR experience on par with that of the other versions of the game.', 'In other games like Zelda: Breath of the Wild, the HDR experience is rather disappointing, as the game looks washed out due to its aesthetics and the lack of contrast.\nThe Nintendo Switch 2 launches today worldwide.']</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>0.8979</v>
+        <v>0.928</v>
       </c>
       <c r="I14" t="n">
-        <v>0.166</v>
+        <v>0.231</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -1058,42 +1058,42 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DL-f955c260113cb461bc83d07b7ef513dd</t>
+          <t>DL-daa7370e17bbf6699977f90dd9dcc32e</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2 Comes With a Below-Average Display and Disappointing HDR Support, New In-Depth Analysis Reveals</t>
+          <t>Nintendo Switch 2: New game console officially launches today</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://wccftech.com/nintendo-switch-2-below-average-hdr/</t>
+          <t>https://www.appgefahren.de/nintendo-switch-2-neue-spielkonsole-geht-heute-offiziell-an-den-start-380403.html</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>The new analysis by GamingTech takes a good look at the new Nintendo system's display. Measuring the brightness in Zelda: Breath of the Wild returned a maximum value of 420 nits, but in Cyberpunk 2077, it is locked to 450 nit, likely the maximum peak brightness the display is capable of. This peak brightness is not even close to providing a proper HDR experience.</t>
+          <t>Nintendo officially unveiled the new generation of the popular Switch game console, the Nintendo Switch 2. The new model, equipped with a 7.9′′ screen and support for 4K content, is now available on the market. At the same thickness, the console features a significantly larger 7.9-inch LCD screen, 1080p resolution, HDR support, and frame rates of up to 120 fps. If the Switch 2 is connected to a TV via the also updated dock. For 4K playback, the frame</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>7.694647</v>
+        <v>15.065298</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-06-05T11:37:00+00:00</t>
+          <t>2025-06-05T12:38:11+00:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>["Related Story Level Up Your Switch 2 Experience With Mumba’s Blade Series, Clear Series Dockable Cases, and Carrying Case\nThe Nintendo Switch 2's HDR support in docked mode fares a little better.", 'The system-level calibration is found to be adequate, and in games like Cyberpunk 2077, the system delivers an HDR experience on par with that of the other versions of the game.', 'In other games like Zelda: Breath of the Wild, the HDR experience is rather disappointing, as the game looks washed out due to its aesthetics and the lack of contrast.\nThe Nintendo Switch 2 launches today worldwide.']</t>
+          <t>['But what can the new Nintendo Switch 2 do? Compared to its predecessor, the Nintendo Switch (OLED), the Switch 2 has done quite a bit.', 'At the same thickness, the console features a significantly larger 7.9-inch LCD screen, 1080p resolution, HDR support, and frame rates of up to 120 fps.']</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>0.928</v>
+        <v>0.802</v>
       </c>
       <c r="I15" t="n">
-        <v>0.231</v>
+        <v>0.111</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
@@ -1102,42 +1102,42 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DL-daa7370e17bbf6699977f90dd9dcc32e</t>
+          <t>DL-cce7387fccad72acd7b577de07a1a6e3</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Nintendo Switch 2: New game console officially launches today</t>
+          <t>Nintendo Switch 2 unboxing: What do you get with the console?</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://www.appgefahren.de/nintendo-switch-2-neue-spielkonsole-geht-heute-offiziell-an-den-start-380403.html</t>
+          <t>https://www.indy100.com/gaming/nintendo-switch-2-unboxing-console-2672317405</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Nintendo officially unveiled the new generation of the popular Switch game console, the Nintendo Switch 2. The new model, equipped with a 7.9′′ screen and support for 4K content, is now available on the market. At the same thickness, the console features a significantly larger 7.9-inch LCD screen, 1080p resolution, HDR support, and frame rates of up to 120 fps. If the Switch 2 is connected to a TV via the also updated dock. For 4K playback, the frame</t>
+          <t>Nintendo has sent review units out to media outlets for them to check out the new console and games running on it. The first thing that will be seen when unboxing are the two new Joy-Con controllers and main part of the console with the bigger screen. Below that on the next layer down is a brief user manual, a HDMI cable to connect the dock to a TV and the wrist strap accessories that connect to the Switch 2.</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>7.661373</v>
+        <v>14.92691</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-06-05T12:38:11+00:00</t>
+          <t>2025-06-05T15:19:37</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>['But what can the new Nintendo Switch 2 do? Compared to its predecessor, the Nintendo Switch (OLED), the Switch 2 has done quite a bit.', 'At the same thickness, the console features a significantly larger 7.9-inch LCD screen, 1080p resolution, HDR support, and frame rates of up to 120 fps.']</t>
+          <t>['Nintendo has sent Switch 2 review units out to media outlets for them to check out the new console and games running on it.\nindy100 is very fortunate to have been sent one of these units and this is what comes in the box - read our first impressions of']</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>0.802</v>
+        <v>0.5859</v>
       </c>
       <c r="I16" t="n">
-        <v>0.111</v>
+        <v>0.048</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -1276,7 +1276,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B2" t="n">
         <v>15</v>

</xml_diff>